<commit_message>
adding materials on ERBD
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="12630" windowHeight="7650"/>
-    <workbookView xWindow="4485" yWindow="-30" windowWidth="11445" windowHeight="7680" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="12630" windowHeight="7515"/>
+    <workbookView xWindow="4485" yWindow="-30" windowWidth="14805" windowHeight="7590" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="OPIC" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="1012">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -1965,54 +1966,6 @@
     <t>[Physical Cultural Resources Safeguard Policy Guidebook 2009 (French)](http://siteresources.worldbank.org/INTSAFEPOL/Resources/FrenchCulturalResouces.pdf)</t>
   </si>
   <si>
-    <t>[Sustainability Standards / Policy (re-direct)](http://www.iadb.org/en/topics/sustainability/policies-and-initiatives,1517.html)</t>
-  </si>
-  <si>
-    <t>[Environment and Safeguards Compliance Policy](http://www.iadb.org/document.cfm?id=665902)</t>
-  </si>
-  <si>
-    <t>[Implementation Guidelines for the Environment and Safeguards Policy](http://www.iadb.org/document.cfm?id=35597106) (approved 2007)</t>
-  </si>
-  <si>
-    <t>[Disaster Risk Management Policy](http://www.iadb.org/document.cfm?id=360026)</t>
-  </si>
-  <si>
-    <t>[Disaster Risk Management Policy Guidelines](http://www.iadb.org/document.cfm?id=35597355)</t>
-  </si>
-  <si>
-    <t>[Operational Policy on Indigenous Peoples](http://www.iadb.org/document.cfm?id=865801)</t>
-  </si>
-  <si>
-    <t>[Operating Guidelines for the Indegenous Peoples Policy (IPP)](http://www.iadb.org/document.cfm?id=35598894) (approved 2006)</t>
-  </si>
-  <si>
-    <t>[Involuntary Resettlement Policy](http://www.iadb.org/document.cfm?id=822598)</t>
-  </si>
-  <si>
-    <t>[Involuntary Resettlement in IDB Projects: Principles and Guidelines](http://www.iadb.org/document.cfm?id=362003) (approved 1999)</t>
-  </si>
-  <si>
-    <t>[Access to Information Policy](http://www.iadb.org/en/about-us/information-disclosure-policy,6110.html) (approved May 2010;  effective on January 1, 2011)</t>
-  </si>
-  <si>
-    <t>[OP-765:Operational Policy on Indigenous Peoples (Feb 2006)](http://www.iadb.org/sds/doc/ind-111PolicyE.pdf)</t>
-  </si>
-  <si>
-    <t>[IDB Sustainability Review](http://www.iadb.org/sustainability/template.cfm?Page=54&amp;language=English)</t>
-  </si>
-  <si>
-    <t>[Strategy for Indigenous Development (Feb 2006)](http://www.iadb.org/sds/doc/ind-111StrategyE.pdf)</t>
-  </si>
-  <si>
-    <t>[Environmental and Social Review Procedure](http://www.ifc.org/ifcext/sustainability.nsf/AttachmentsByTitle/pol_ESRP2009/$FILE/ESRP2009.pdf)</t>
-  </si>
-  <si>
-    <t>[Policy on Disclosure of Information](http://www.ifc.org/ifcext/sustainability.nsf/AttachmentsByTitle/pol_Disclosure2006/$FILE/Disclosure2006.pdf)</t>
-  </si>
-  <si>
-    <t>[Environmental and Social Review Procedure Manual](http://www.ifc.org/wps/wcm/connect/topics_ext_content/ifc_external_corporate_site/ifc+sustainability/our+approach/risk+management/environmental+and+social+review+procedure+manual)</t>
-  </si>
-  <si>
     <t>Environmental and Social Review Procedure (April 2013) [PDF]</t>
   </si>
   <si>
@@ -2299,6 +2252,813 @@
   </si>
   <si>
     <t>Stakeholder Engagement: A Good Practice Handbook for Companies Doing Business in Emerging Markets</t>
+  </si>
+  <si>
+    <t>Environmental and Social Review Procedure</t>
+  </si>
+  <si>
+    <t>Environmental and Social Review Procedure Manua</t>
+  </si>
+  <si>
+    <t>Sustainability Framework</t>
+  </si>
+  <si>
+    <t>FPIC</t>
+  </si>
+  <si>
+    <t>consultation &amp; engagement</t>
+  </si>
+  <si>
+    <t>migration</t>
+  </si>
+  <si>
+    <t>retrenchment</t>
+  </si>
+  <si>
+    <t>labour &amp; working conditions</t>
+  </si>
+  <si>
+    <t>displpacement</t>
+  </si>
+  <si>
+    <t>impact assessment</t>
+  </si>
+  <si>
+    <t>disclosure &amp; reporting</t>
+  </si>
+  <si>
+    <t>Policy on Disclosure of Information</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/sustainability/policies-and-initiatives,1517.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=665902</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=35597106</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=360026</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=35597355</t>
+  </si>
+  <si>
+    <t>Disaster Risk Management Policy Guidelines</t>
+  </si>
+  <si>
+    <t>Disaster Risk Management Policy</t>
+  </si>
+  <si>
+    <t>Implementation Guidelines for the Environment and Safeguards Policy</t>
+  </si>
+  <si>
+    <t>Environment and Safeguards Compliance Policy</t>
+  </si>
+  <si>
+    <t>Sustainability Standards / Policy (re-direct)</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=865801</t>
+  </si>
+  <si>
+    <t>Operational Policy on Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>Operating Guidelines for the Indegenous Peoples Policy (IPP)</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=35598894</t>
+  </si>
+  <si>
+    <t>Involuntary Resettlement Policy</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=822598</t>
+  </si>
+  <si>
+    <t>Involuntary Resettlement in IDB Projects: Principles and Guidelines</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=362003</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/information-disclosure-policy,6110.html</t>
+  </si>
+  <si>
+    <t>OP-765:Operational Policy on Indigenous Peoples (Feb 2006)</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/sds/doc/ind-111PolicyE.pdf</t>
+  </si>
+  <si>
+    <t>IDB Sustainability Review</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/sustainability/template.cfm?Page=54&amp;language=English</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/sds/doc/ind-111StrategyE.pdf</t>
+  </si>
+  <si>
+    <t>Strategy for Indigenous Development</t>
+  </si>
+  <si>
+    <t>Strategy on Social Policy for Equity and Productivity</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=35802223</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/education/strategy-on-social-policy-for-equity-and-productivity,3221.html</t>
+  </si>
+  <si>
+    <t>Social Safeguards</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/sustainability/social-safeguards,1518.html</t>
+  </si>
+  <si>
+    <t>Operating Guidelines for the Indigenous Peoples Policy (IPP)</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2631</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2636</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2582</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2584</t>
+  </si>
+  <si>
+    <t>Operational Policy on Gender Equality in Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementation Guidelines for the Operational Policy on Gender Equality in Development </t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=38154638</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/gender-indigenous-peoples-and-african-descendants/operational-policy-on-gender-equality-in-development,2980.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disaster Risk Management Policy Guidelines </t>
+  </si>
+  <si>
+    <t>Greenhouse Gas Emissions (GHG)</t>
+  </si>
+  <si>
+    <t>Coal Fired Power Plants Guidelines</t>
+  </si>
+  <si>
+    <t>Cement Manufacturing Plant Guidelines</t>
+  </si>
+  <si>
+    <t>Landfill Guidelines</t>
+  </si>
+  <si>
+    <t>Liquid and Gaseous Fossil Fuel Power Plant</t>
+  </si>
+  <si>
+    <t>General Operational Policies</t>
+  </si>
+  <si>
+    <t>101 General Information</t>
+  </si>
+  <si>
+    <t>102 Access to Information</t>
+  </si>
+  <si>
+    <t>201 The Country and Subregional Programming Process</t>
+  </si>
+  <si>
+    <t>202 The Bank's Operations Program</t>
+  </si>
+  <si>
+    <t>OPERATIONS PROGRAMING</t>
+  </si>
+  <si>
+    <t>LENDING POLICIES</t>
+  </si>
+  <si>
+    <t>301 Eligible Borrowers</t>
+  </si>
+  <si>
+    <t>302 Project Preparation, Evaluation and Approval</t>
+  </si>
+  <si>
+    <t>303 Guarantees Required from the Borrower</t>
+  </si>
+  <si>
+    <t>304 Operations Administration</t>
+  </si>
+  <si>
+    <t>305 ExPost Evaluation</t>
+  </si>
+  <si>
+    <t>307 Amount of Loan in Foreign Exchange</t>
+  </si>
+  <si>
+    <t>308 Financing of Interest</t>
+  </si>
+  <si>
+    <t>309 Global Loans to Intermediary Financial Institutions - Contributions by Subborrowers</t>
+  </si>
+  <si>
+    <t>310 Financing Increase of Cost Overruns for Operations in Execution</t>
+  </si>
+  <si>
+    <t>311 Eligible Expenditures in Investment Loans</t>
+  </si>
+  <si>
+    <t>TECHNICAL COOPERATION POLICIES</t>
+  </si>
+  <si>
+    <t>400 Technical Cooperation Policy</t>
+  </si>
+  <si>
+    <t>401 Framework for Technical Cooperation</t>
+  </si>
+  <si>
+    <t>402 TC Taxonomy and Forms of Financing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROCUREMENT OF GOODS AND SERVICES </t>
+  </si>
+  <si>
+    <t>Project Procurement</t>
+  </si>
+  <si>
+    <t>SUBREGIONAL FINANCIAL INSTITUTIONS</t>
+  </si>
+  <si>
+    <t>601 Relationship with Subregional Financial Institutions - General Policy</t>
+  </si>
+  <si>
+    <t>602 Cooperation with Other Sources of Financing</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/general-operational-policies,6236.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/idb-financial-programming-process-,6237.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/operational-program-,6238.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/eligible-borrowers-,6709.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/project-preparation-evaluation-and-approval-,6240.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/guarantees-required-from-the-borrower,6708.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/operations-administration-,6241.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/evaluation-of-idb-operational-objectives,6242.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/financing-and-mobilization-of-resources,6243.html</t>
+  </si>
+  <si>
+    <t>306 Forms of Bank Financing and Assistance for the Mobilization of Financial Resources</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/loans-in-foreign-exchange,6244.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/financing-of-interest-,6245.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/global-loans-to-intermediary-financial-institutions-contributions-by-subborrowers,6710.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=37808573</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=37808621</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=39444571</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=39444681</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=39444739</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/projects/project-procurement,8148.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/subregional-financial-institutions,6711.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/cooperation-with-other-sources-of-financing,6256.html</t>
+  </si>
+  <si>
+    <t>Multisectoral Policies</t>
+  </si>
+  <si>
+    <t>703 Environment and Safeguards Compliance</t>
+  </si>
+  <si>
+    <t>704 Natural Disaster Risk Management</t>
+  </si>
+  <si>
+    <t>707 Maintenance and Conservation of Physical Works and Equipment</t>
+  </si>
+  <si>
+    <t>708 Public Utilities (Feb 2014)</t>
+  </si>
+  <si>
+    <t>710 Involuntary Resettlement</t>
+  </si>
+  <si>
+    <t>Economic Infrastructure Sectors</t>
+  </si>
+  <si>
+    <t>733 Energy</t>
+  </si>
+  <si>
+    <t>733-1 Electric Energy</t>
+  </si>
+  <si>
+    <t>Policies for Special Areas</t>
+  </si>
+  <si>
+    <t>761 Gender Equality in Development</t>
+  </si>
+  <si>
+    <t>765 Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>Sector Framework Documents</t>
+  </si>
+  <si>
+    <t>2001 Agriculture and Natural Resource Management</t>
+  </si>
+  <si>
+    <t>2002 Education and Early Childhood Development</t>
+  </si>
+  <si>
+    <t>2003 Integration and Trade</t>
+  </si>
+  <si>
+    <t>2004 Urban Development and Housing</t>
+  </si>
+  <si>
+    <t>2005 Health and Nutrition</t>
+  </si>
+  <si>
+    <t>2006 Labor</t>
+  </si>
+  <si>
+    <t>2007 Transportation</t>
+  </si>
+  <si>
+    <t>2008 Support to SMEs and Financial Access/Supervision</t>
+  </si>
+  <si>
+    <t>2009 Citizen Security and Justice</t>
+  </si>
+  <si>
+    <t>2010 Tourism</t>
+  </si>
+  <si>
+    <t>2011 Social Protection and Poverty</t>
+  </si>
+  <si>
+    <t>2012 Water and Sanitation</t>
+  </si>
+  <si>
+    <t>2013 Innovation, Science and Technology</t>
+  </si>
+  <si>
+    <t>2014 Gender and Diversity</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=35004515</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/maintenance-and-conservation-of-physical-works-and-equipment,6207.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=38198344</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/involuntary-resettlement,6660.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/energy,6219.html</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/electric-energy,6220.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/who-we-are/our-values/environmental-and-social-policy.html%20</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/documents/comms-and-bis/pdf-environmental-and-social-policy-2008.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/publications/policies/environmental-and-social-policy-2008.html</t>
+  </si>
+  <si>
+    <t>Environmental and Social Policy</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/2003-07-01,_Environmental_Policy-_English_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/1996-09-01_Environmental_Policy-_English_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/publications/policies/environmental-and-social-policy.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/publications/policies/environmental-and-social-policy-esp.html</t>
+  </si>
+  <si>
+    <t>Environmental and Social Procedures 2010</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/2008policy.pdf</t>
+  </si>
+  <si>
+    <t>Environmental Policy (EP) 1992</t>
+  </si>
+  <si>
+    <t>Environmental Policy (EP) 1996</t>
+  </si>
+  <si>
+    <t>Enivronmental Policy (EP) 2003</t>
+  </si>
+  <si>
+    <t>Environmental and Social Policy (ESP) 2008</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/documents/comms-and-bis/pdf-environmental-and-social-policy.pdf</t>
+  </si>
+  <si>
+    <t>Environmental and Social Policy (ESP) 2014</t>
+  </si>
+  <si>
+    <t>Public Information Policy</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395236452323&amp;d=&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>Report on the invitation to the public to comment</t>
+  </si>
+  <si>
+    <t>Information request form</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/policies/pip/pip-comment.pdf</t>
+  </si>
+  <si>
+    <t>Evaluation policy</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/strategies-and-policies/public-information-policy.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/evaluation-policy.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241631988&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>Sectoral strategies</t>
+  </si>
+  <si>
+    <t>Country strategies</t>
+  </si>
+  <si>
+    <t>Corporate policies, procedures and strategies</t>
+  </si>
+  <si>
+    <t>Addressing staff grievances</t>
+  </si>
+  <si>
+    <t>Anti-terrorist statement</t>
+  </si>
+  <si>
+    <t>Approval of new governance policies</t>
+  </si>
+  <si>
+    <t>Business Plan and Budget</t>
+  </si>
+  <si>
+    <t>Basic documents of the EBRD</t>
+  </si>
+  <si>
+    <t>Capital Resources Review</t>
+  </si>
+  <si>
+    <t>Common Performance Assessment Report</t>
+  </si>
+  <si>
+    <t>Domiciliation of EBRD clients</t>
+  </si>
+  <si>
+    <t>Enforcement policy and procedures</t>
+  </si>
+  <si>
+    <t>Environmental and social procedures</t>
+  </si>
+  <si>
+    <t>Ethnic minorities and the EBRD</t>
+  </si>
+  <si>
+    <t>Fraud and corruption - definitions and guidelines</t>
+  </si>
+  <si>
+    <t>Governance policies</t>
+  </si>
+  <si>
+    <t>Information Classification (IC)</t>
+  </si>
+  <si>
+    <t>Purchasing policy and procedures</t>
+  </si>
+  <si>
+    <t>Political aspects of the EBRD mandate</t>
+  </si>
+  <si>
+    <t>Procurement policies and rules</t>
+  </si>
+  <si>
+    <t>Project Complaint Mechanism</t>
+  </si>
+  <si>
+    <t>Secure Mail (Switch)</t>
+  </si>
+  <si>
+    <t>Agribusiness strategy</t>
+  </si>
+  <si>
+    <t>Energy strategy</t>
+  </si>
+  <si>
+    <t>Financial Institutions Strategy</t>
+  </si>
+  <si>
+    <t>Information and Communication Technologies Sector Strategy</t>
+  </si>
+  <si>
+    <t>Municipal and Environmental Infrastructure</t>
+  </si>
+  <si>
+    <t>Mining operations policy</t>
+  </si>
+  <si>
+    <t>Micro, small and medium-sized enterprises</t>
+  </si>
+  <si>
+    <t>Property policy</t>
+  </si>
+  <si>
+    <t>Shipping Operations Policy</t>
+  </si>
+  <si>
+    <t>Transport Sector Strategy</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kyrgyz Republic</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>FYR Macedonia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Slovak Republic</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/strategies-and-policies.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/sgri.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395238656263&amp;pagename=EBRD%2FContent%2FContentLayout</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/strategies-and-policies/approval-of-new-governance-policies.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/strategies-and-policies/business-plan-and-budget.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/publications/institutional-documents/basic-documents-of-the-ebrd.html%20</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/capital-resources-review.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395238826157&amp;pagename=EBRD%2FContent%2FContentLayout</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/policies/sector/domiciliation-policy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/epp11.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/sustainability/environmental-procedures.pdf</t>
+  </si>
+  <si>
+    <t>http://www.google.com/url?q=http%3A%2F%2Fwww.ebrd.com%2Fdownloads%2Fabout%2Fethnic.pdf&amp;sa=D&amp;sntz=1&amp;usg=AFQjCNF3vvAIJ7-c87AExXgXs2-A5TrLSg</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/evaluation/1003.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/compas06.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/fraud.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/pages/about/policies/ebrd-information-classification.shtml</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/procurement/ppp.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/aspects.pdf</t>
+  </si>
+  <si>
+    <t>Capital Resources Review 2011-2015</t>
+  </si>
+  <si>
+    <t>Public consultation on the EBRD’s capital review process</t>
+  </si>
+  <si>
+    <t>Report on public consultation</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/documents/comms-and-bis/pdf-basic-documents-of-the-ebrd.pdf</t>
+  </si>
+  <si>
+    <t>Agreement Establishing the European Bank for Reconstruction and Development</t>
+  </si>
+  <si>
+    <t>Chairman’s Report on the Agreement Establishing the European Bank for Reconstruction and Development</t>
+  </si>
+  <si>
+    <t>By-Laws of the European Bank for Reconstruction and Development</t>
+  </si>
+  <si>
+    <t>Rules of Procedure of the Board of Governors</t>
+  </si>
+  <si>
+    <t>Rules of Procedure of the Board of Directors</t>
+  </si>
+  <si>
+    <t>Headquarters Agreement</t>
+  </si>
+  <si>
+    <t>Download the 2014 ESP</t>
+  </si>
+  <si>
+    <t>2014 ESP in other languages</t>
+  </si>
+  <si>
+    <t>ESP Stakeholder Engagement Report</t>
+  </si>
+  <si>
+    <t>ESP Stakeholder Engagement Plan</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395238867768&amp;d=&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/esp-sep.pdf</t>
+  </si>
+  <si>
+    <t>Download the PIP 2014</t>
+  </si>
+  <si>
+    <t>Project Complaint Mechanism Rules of Procedure (PCM RPs) 2014</t>
+  </si>
+  <si>
+    <t>Project Complaint Mechanism Stakeholder Engagement Report</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/2013esp.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/policies/pip/pipe.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/integrity/pcmrules2014.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/integrity/pcm_comments.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/work-with-us/project-finance/project-complaint-mechanism.html</t>
   </si>
 </sst>
 </file>
@@ -5240,7 +6000,9 @@
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5409,8 +6171,8 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
-    <sheetView topLeftCell="G7" zoomScale="90" zoomScaleNormal="90" workbookViewId="1">
-      <selection activeCell="K10" sqref="K10:O10"/>
+    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="1">
+      <selection activeCell="C10" sqref="C10:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7276,46 +8038,72 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B9"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H2" sqref="H2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>646</v>
       </c>
@@ -7327,78 +8115,645 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B14"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1">
-      <selection activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+      <c r="D2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>763</v>
+      </c>
+      <c r="D3" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>762</v>
+      </c>
+      <c r="D4" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+        <v>761</v>
+      </c>
+      <c r="D5" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+      <c r="D6" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+        <v>766</v>
+      </c>
+      <c r="D7" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+      <c r="D8" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>769</v>
+      </c>
+      <c r="D9" t="s">
+        <v>770</v>
+      </c>
+      <c r="J9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+        <v>771</v>
+      </c>
+      <c r="D10" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+      <c r="D11" t="s">
+        <v>773</v>
+      </c>
+      <c r="J11">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+        <v>774</v>
+      </c>
+      <c r="E12" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+        <v>776</v>
+      </c>
+      <c r="D13" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>659</v>
+        <v>779</v>
+      </c>
+      <c r="E14" t="s">
+        <v>778</v>
+      </c>
+      <c r="J14">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>780</v>
+      </c>
+      <c r="D16" t="s">
+        <v>782</v>
+      </c>
+      <c r="E16" t="s">
+        <v>781</v>
+      </c>
+      <c r="J16">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>783</v>
+      </c>
+      <c r="D17" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" t="s">
+        <v>766</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B20" t="s">
+        <v>785</v>
+      </c>
+      <c r="E20" t="s">
+        <v>787</v>
+      </c>
+      <c r="J20">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" t="s">
+        <v>769</v>
+      </c>
+      <c r="E22" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B23" t="s">
+        <v>771</v>
+      </c>
+      <c r="E23" t="s">
+        <v>789</v>
+      </c>
+      <c r="J23">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>790</v>
+      </c>
+      <c r="D25" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>791</v>
+      </c>
+      <c r="E26" t="s">
+        <v>792</v>
+      </c>
+      <c r="J26">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>801</v>
+      </c>
+      <c r="D43" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>802</v>
+      </c>
+      <c r="D44" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>803</v>
+      </c>
+      <c r="D46" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>804</v>
+      </c>
+      <c r="D47" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>807</v>
+      </c>
+      <c r="D49" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>808</v>
+      </c>
+      <c r="D50" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>809</v>
+      </c>
+      <c r="D51" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>810</v>
+      </c>
+      <c r="D52" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>811</v>
+      </c>
+      <c r="D53" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>835</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>812</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>813</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>814</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>815</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>816</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>818</v>
+      </c>
+      <c r="D61" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>819</v>
+      </c>
+      <c r="D62" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>820</v>
+      </c>
+      <c r="D63" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>822</v>
+      </c>
+      <c r="D65" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>824</v>
+      </c>
+      <c r="D67" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>825</v>
+      </c>
+      <c r="D68" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>848</v>
+      </c>
+      <c r="D70" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>849</v>
+      </c>
+      <c r="D71" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>850</v>
+      </c>
+      <c r="D72" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>851</v>
+      </c>
+      <c r="D73" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>852</v>
+      </c>
+      <c r="D74" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>854</v>
+      </c>
+      <c r="D76" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>855</v>
+      </c>
+      <c r="D77" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>873</v>
       </c>
     </row>
   </sheetData>
@@ -7408,16 +8763,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O64"/>
+  <dimension ref="B2:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="1">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7436,10 +8792,10 @@
       </c>
       <c r="H2" s="21"/>
       <c r="I2" t="s">
-        <v>695</v>
+        <v>679</v>
       </c>
       <c r="J2" t="s">
-        <v>696</v>
+        <v>680</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>234</v>
@@ -7459,423 +8815,1281 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>670</v>
+        <v>745</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>670</v>
+        <v>654</v>
       </c>
       <c r="E3" t="s">
-        <v>671</v>
+        <v>655</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>745</v>
+      </c>
       <c r="C4" s="24" t="s">
-        <v>680</v>
+        <v>664</v>
       </c>
       <c r="E4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>745</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>665</v>
+      </c>
+      <c r="E5" t="s">
+        <v>667</v>
+      </c>
+      <c r="I5" t="s">
+        <v>681</v>
+      </c>
+      <c r="J5" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="24" t="s">
-        <v>681</v>
-      </c>
-      <c r="E5" t="s">
-        <v>683</v>
-      </c>
-      <c r="I5" t="s">
-        <v>697</v>
-      </c>
-      <c r="J5" t="s">
-        <v>698</v>
-      </c>
-    </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>745</v>
+      </c>
       <c r="C6" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
       <c r="D6" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
       <c r="E6" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>745</v>
+      </c>
       <c r="C8" t="s">
+        <v>656</v>
+      </c>
+      <c r="E8" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>745</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>669</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>672</v>
-      </c>
-      <c r="E8" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="14" t="s">
-        <v>685</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>688</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>745</v>
+      </c>
       <c r="C10" s="14" t="s">
-        <v>691</v>
+        <v>675</v>
       </c>
       <c r="D10" t="s">
-        <v>693</v>
+        <v>677</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>693</v>
+        <v>677</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>745</v>
+      </c>
       <c r="C11" s="14" t="s">
-        <v>692</v>
+        <v>676</v>
       </c>
       <c r="D11" t="s">
-        <v>694</v>
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>745</v>
+      </c>
       <c r="C12" t="s">
-        <v>668</v>
+        <v>652</v>
       </c>
       <c r="D12" t="s">
-        <v>699</v>
+        <v>683</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>745</v>
+      </c>
       <c r="C14" t="s">
-        <v>686</v>
+        <v>670</v>
       </c>
       <c r="D14" t="s">
+        <v>657</v>
+      </c>
+      <c r="E14" t="s">
         <v>673</v>
       </c>
-      <c r="E14" t="s">
-        <v>689</v>
-      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>745</v>
+      </c>
       <c r="C15" t="s">
-        <v>687</v>
+        <v>671</v>
       </c>
       <c r="D15" t="s">
-        <v>690</v>
+        <v>674</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>745</v>
+      </c>
       <c r="C16" t="s">
         <v>37</v>
       </c>
       <c r="D16" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>745</v>
+      </c>
+      <c r="C18" t="s">
+        <v>663</v>
+      </c>
+      <c r="D18" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>745</v>
+      </c>
+      <c r="C19" t="s">
+        <v>754</v>
+      </c>
+      <c r="D19" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>679</v>
-      </c>
-      <c r="D18" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>661</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="21" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C24" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C25" t="s">
+        <v>648</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C26" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C27" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C28" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C30" t="s">
+        <v>744</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>742</v>
+      </c>
+      <c r="F34" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>741</v>
+      </c>
+      <c r="F35" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>740</v>
+      </c>
+      <c r="F36" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>748</v>
+      </c>
+      <c r="C38" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>748</v>
+      </c>
+      <c r="C40" t="s">
+        <v>739</v>
+      </c>
+      <c r="E40" t="s">
+        <v>691</v>
+      </c>
+      <c r="F40" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>748</v>
+      </c>
+      <c r="C41" t="s">
+        <v>738</v>
+      </c>
+      <c r="F41" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>748</v>
+      </c>
+      <c r="C42" t="s">
+        <v>737</v>
+      </c>
+      <c r="F42" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>748</v>
+      </c>
+      <c r="C43" t="s">
+        <v>736</v>
+      </c>
+      <c r="F43" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>748</v>
+      </c>
+      <c r="C44" t="s">
+        <v>735</v>
+      </c>
+      <c r="F44" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>748</v>
+      </c>
+      <c r="C45" t="s">
+        <v>734</v>
+      </c>
+      <c r="F45" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>748</v>
+      </c>
+      <c r="C46" t="s">
+        <v>733</v>
+      </c>
+      <c r="F46" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>748</v>
+      </c>
+      <c r="C47" t="s">
+        <v>732</v>
+      </c>
+      <c r="F47" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>748</v>
+      </c>
+      <c r="C49" t="s">
+        <v>731</v>
+      </c>
+      <c r="E49" t="s">
+        <v>699</v>
+      </c>
+      <c r="F49" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>746</v>
+      </c>
+      <c r="C51" t="s">
+        <v>717</v>
+      </c>
+      <c r="F51" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="21" spans="3:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>660</v>
-      </c>
-      <c r="D23" s="23" t="s">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>747</v>
+      </c>
+      <c r="C52" t="s">
+        <v>716</v>
+      </c>
+      <c r="F52" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>662</v>
-      </c>
-      <c r="D30" s="23" t="s">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>747</v>
+      </c>
+      <c r="C53" t="s">
+        <v>715</v>
+      </c>
+      <c r="F53" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="32" spans="3:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>758</v>
-      </c>
-      <c r="F34" t="s">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>750</v>
+      </c>
+      <c r="C54" t="s">
+        <v>714</v>
+      </c>
+      <c r="F54" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>757</v>
-      </c>
-      <c r="F35" t="s">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>749</v>
+      </c>
+      <c r="C55" t="s">
+        <v>713</v>
+      </c>
+      <c r="F55" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>756</v>
-      </c>
-      <c r="F36" t="s">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>750</v>
+      </c>
+      <c r="C56" t="s">
+        <v>712</v>
+      </c>
+      <c r="F56" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>755</v>
-      </c>
-      <c r="E40" t="s">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>750</v>
+      </c>
+      <c r="C57" t="s">
+        <v>711</v>
+      </c>
+      <c r="F57" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>752</v>
+      </c>
+      <c r="C58" t="s">
+        <v>710</v>
+      </c>
+      <c r="F58" t="s">
         <v>707</v>
       </c>
-      <c r="F40" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>754</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="I58" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="J58" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>751</v>
+      </c>
+      <c r="C60" t="s">
+        <v>719</v>
+      </c>
+      <c r="F60" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>752</v>
+      </c>
+      <c r="C62" t="s">
+        <v>730</v>
+      </c>
+      <c r="E62" t="s">
+        <v>729</v>
+      </c>
+      <c r="G62" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>753</v>
       </c>
-      <c r="F42" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>752</v>
-      </c>
-      <c r="F43" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>751</v>
-      </c>
-      <c r="F44" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>750</v>
-      </c>
-      <c r="F45" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>749</v>
-      </c>
-      <c r="F46" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>748</v>
-      </c>
-      <c r="F47" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>747</v>
-      </c>
-      <c r="E48" t="s">
-        <v>715</v>
-      </c>
-      <c r="F48" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>733</v>
-      </c>
-      <c r="F50" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>732</v>
-      </c>
-      <c r="F51" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>731</v>
-      </c>
-      <c r="F52" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>730</v>
-      </c>
-      <c r="F53" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>729</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="C64" t="s">
+        <v>721</v>
+      </c>
+      <c r="E64" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>728</v>
-      </c>
-      <c r="F55" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>727</v>
-      </c>
-      <c r="F56" t="s">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>753</v>
+      </c>
+      <c r="C65" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>726</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E65" t="s">
         <v>723</v>
-      </c>
-      <c r="I57" t="s">
-        <v>724</v>
-      </c>
-      <c r="J57" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>735</v>
-      </c>
-      <c r="F59" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>746</v>
-      </c>
-      <c r="E61" t="s">
-        <v>745</v>
-      </c>
-      <c r="G61" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>737</v>
-      </c>
-      <c r="E63" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>738</v>
-      </c>
-      <c r="E64" t="s">
-        <v>739</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B4"/>
+  <dimension ref="B2:N109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="6" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>741</v>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>895</v>
+      </c>
+      <c r="C7" t="s">
+        <v>894</v>
+      </c>
+      <c r="D7" t="s">
+        <v>880</v>
+      </c>
+      <c r="F7" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>893</v>
+      </c>
+      <c r="C8" t="s">
+        <v>881</v>
+      </c>
+      <c r="D8" t="s">
+        <v>882</v>
+      </c>
+      <c r="J8">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>883</v>
+      </c>
+      <c r="D9" t="s">
+        <v>887</v>
+      </c>
+      <c r="F9" t="s">
+        <v>886</v>
+      </c>
+      <c r="J9">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>892</v>
+      </c>
+      <c r="C10" t="s">
+        <v>884</v>
+      </c>
+      <c r="D10" t="s">
+        <v>887</v>
+      </c>
+      <c r="F10" t="s">
+        <v>886</v>
+      </c>
+      <c r="J10">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>891</v>
+      </c>
+      <c r="C11" t="s">
+        <v>885</v>
+      </c>
+      <c r="D11" t="s">
+        <v>887</v>
+      </c>
+      <c r="F11" t="s">
+        <v>886</v>
+      </c>
+      <c r="J11">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>888</v>
+      </c>
+      <c r="C12" t="s">
+        <v>889</v>
+      </c>
+      <c r="D12" t="s">
+        <v>887</v>
+      </c>
+      <c r="J12">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>890</v>
+      </c>
+      <c r="D13" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>998</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F14" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>999</v>
+      </c>
+      <c r="D15" t="s">
+        <v>973</v>
+      </c>
+      <c r="F15" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F16" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F17" t="s">
+        <v>973</v>
+      </c>
+      <c r="J17">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>896</v>
+      </c>
+      <c r="C18" t="s">
+        <v>897</v>
+      </c>
+      <c r="D18" t="s">
+        <v>902</v>
+      </c>
+      <c r="J18">
+        <v>2014</v>
+      </c>
+      <c r="K18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>898</v>
+      </c>
+      <c r="E19" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D21" t="s">
+        <v>902</v>
+      </c>
+      <c r="F21" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>898</v>
+      </c>
+      <c r="C22" t="s">
+        <v>900</v>
+      </c>
+      <c r="D22" t="s">
+        <v>902</v>
+      </c>
+      <c r="F22" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>901</v>
+      </c>
+      <c r="C24" t="s">
+        <v>904</v>
+      </c>
+      <c r="D24" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F26" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F27" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="D30" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>908</v>
+      </c>
+      <c r="C31" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>909</v>
+      </c>
+      <c r="D32" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>910</v>
+      </c>
+      <c r="D33" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>911</v>
+      </c>
+      <c r="D34" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>912</v>
+      </c>
+      <c r="C35" t="s">
+        <v>991</v>
+      </c>
+      <c r="D35" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>913</v>
+      </c>
+      <c r="D42" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="14" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>914</v>
+      </c>
+      <c r="C46" t="s">
+        <v>983</v>
+      </c>
+      <c r="D46" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>915</v>
+      </c>
+      <c r="C47" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>916</v>
+      </c>
+      <c r="C48" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>917</v>
+      </c>
+      <c r="C49" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>883</v>
+      </c>
+      <c r="C50" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>918</v>
+      </c>
+      <c r="C51" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>901</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>919</v>
+      </c>
+      <c r="C53" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>920</v>
+      </c>
+      <c r="D54" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>921</v>
+      </c>
+      <c r="D55" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>922</v>
+      </c>
+      <c r="C56" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>923</v>
+      </c>
+      <c r="C57" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="D64" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="D76" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>969</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7892,12 +10106,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding materials on OPIIC and organizing ERBD
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="12630" windowHeight="7515"/>
-    <workbookView xWindow="4485" yWindow="-30" windowWidth="14805" windowHeight="7590" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-510" yWindow="75" windowWidth="14805" windowHeight="7590" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="1025">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -2197,12 +2197,6 @@
     <t>http://www.globalreporting.org/</t>
   </si>
   <si>
-    <t>[EBRD Environmental and Social Policy and Performance Requirements (2008)](http://www.ebrd.com/about/policies/enviro/policy/2008policy.pdf)</t>
-  </si>
-  <si>
-    <t>[EBRD Guidance Note on Indigenous Peoples (03 Dec 2010)](http://www.ebrd.com/downloads/research/guides/indp.pdf) [(alt link)](http://www.ebrd.com/pages/research/publications/guides/indp.shtml)</t>
-  </si>
-  <si>
     <t>[Environmental and Social Policy Revision: Letter from the President](http://www.opic.gov/doing-business/investment/environment/policy_revision#final_policy_statement)</t>
   </si>
   <si>
@@ -3059,6 +3053,51 @@
   </si>
   <si>
     <t>http://www.ebrd.com/work-with-us/project-finance/project-complaint-mechanism.html</t>
+  </si>
+  <si>
+    <t>Final Environmental and Social Policy Statement (October 15 2010)</t>
+  </si>
+  <si>
+    <t>Dam Review Procedures</t>
+  </si>
+  <si>
+    <t>Environmental and Social Assessment Procedure Manual</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/consolidated_esps.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/content/environmental-and-social-policies</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/docs/dam_review_procedures.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/files/opic-procedures-manual-2012.pdf</t>
+  </si>
+  <si>
+    <t>OPIC Environmental Handbook</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/the-environment</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/docs/opic_env_handbook.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/about/policies/enviro/policy/2008policy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/pages/research/publications/guides/indp.shtml</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/guides/indp.pdf</t>
+  </si>
+  <si>
+    <t>Guidance Note on Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>Environmental and Social Policy and Performance Requirements</t>
   </si>
 </sst>
 </file>
@@ -3105,7 +3144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3202,6 +3241,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3216,7 +3261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3256,6 +3301,11 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3560,9 +3610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9:P9"/>
     </sheetView>
     <sheetView topLeftCell="F1" workbookViewId="1">
       <selection activeCell="J1" sqref="I1:J1048576"/>
@@ -8153,66 +8203,66 @@
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D4" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D6" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D7" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D8" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D9" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="J9">
         <v>1999</v>
@@ -8220,10 +8270,10 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D10" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -8231,7 +8281,7 @@
         <v>663</v>
       </c>
       <c r="D11" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="J11">
         <v>2011</v>
@@ -8239,26 +8289,26 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E12" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D13" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E14" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="J14">
         <v>2006</v>
@@ -8266,13 +8316,13 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>778</v>
+      </c>
+      <c r="D16" t="s">
         <v>780</v>
       </c>
-      <c r="D16" t="s">
-        <v>782</v>
-      </c>
       <c r="E16" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="J16">
         <v>2011</v>
@@ -8280,10 +8330,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D17" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -8291,11 +8341,11 @@
         <v>260</v>
       </c>
       <c r="B19" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -8303,10 +8353,10 @@
         <v>260</v>
       </c>
       <c r="B20" t="s">
+        <v>783</v>
+      </c>
+      <c r="E20" t="s">
         <v>785</v>
-      </c>
-      <c r="E20" t="s">
-        <v>787</v>
       </c>
       <c r="J20">
         <v>2006</v>
@@ -8317,10 +8367,10 @@
         <v>260</v>
       </c>
       <c r="B22" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E22" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -8328,10 +8378,10 @@
         <v>260</v>
       </c>
       <c r="B23" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E23" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="J23">
         <v>1999</v>
@@ -8339,18 +8389,18 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D25" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E26" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="J26">
         <v>2013</v>
@@ -8358,402 +8408,402 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="39" spans="2:4" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D43" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D44" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D46" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D47" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D49" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D50" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D51" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D52" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D53" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D61" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D62" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D63" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D65" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D67" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D68" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D70" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D71" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D72" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D73" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D74" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D76" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D77" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
   </sheetData>
@@ -8815,7 +8865,7 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>654</v>
@@ -8826,7 +8876,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>664</v>
@@ -8837,7 +8887,7 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>665</v>
@@ -8854,7 +8904,7 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C6" t="s">
         <v>658</v>
@@ -8868,7 +8918,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C8" t="s">
         <v>656</v>
@@ -8879,7 +8929,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>669</v>
@@ -8893,7 +8943,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>675</v>
@@ -8910,7 +8960,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>676</v>
@@ -8921,7 +8971,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C12" t="s">
         <v>652</v>
@@ -8932,7 +8982,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C14" t="s">
         <v>670</v>
@@ -8946,7 +8996,7 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C15" t="s">
         <v>671</v>
@@ -8957,7 +9007,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -8968,7 +9018,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C18" t="s">
         <v>663</v>
@@ -8979,10 +9029,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C19" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D19" t="s">
         <v>684</v>
@@ -8991,7 +9041,7 @@
     <row r="21" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C24" t="s">
         <v>647</v>
@@ -8999,7 +9049,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C25" t="s">
         <v>648</v>
@@ -9010,7 +9060,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C26" t="s">
         <v>649</v>
@@ -9018,7 +9068,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C27" t="s">
         <v>650</v>
@@ -9026,7 +9076,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C28" t="s">
         <v>651</v>
@@ -9034,10 +9084,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C30" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>686</v>
@@ -9046,7 +9096,7 @@
     <row r="32" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F34" t="s">
         <v>687</v>
@@ -9054,7 +9104,7 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F35" t="s">
         <v>688</v>
@@ -9062,7 +9112,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F36" t="s">
         <v>689</v>
@@ -9070,7 +9120,7 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C38" t="s">
         <v>653</v>
@@ -9078,10 +9128,10 @@
     </row>
     <row r="40" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C40" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E40" t="s">
         <v>691</v>
@@ -9092,10 +9142,10 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C41" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F41" t="s">
         <v>692</v>
@@ -9103,10 +9153,10 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C42" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F42" t="s">
         <v>693</v>
@@ -9114,10 +9164,10 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C43" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F43" t="s">
         <v>694</v>
@@ -9125,10 +9175,10 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C44" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F44" t="s">
         <v>695</v>
@@ -9136,10 +9186,10 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C45" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F45" t="s">
         <v>696</v>
@@ -9147,10 +9197,10 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C46" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F46" t="s">
         <v>697</v>
@@ -9158,10 +9208,10 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C47" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F47" t="s">
         <v>698</v>
@@ -9169,10 +9219,10 @@
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C49" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E49" t="s">
         <v>699</v>
@@ -9183,7 +9233,7 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C51" t="s">
         <v>717</v>
@@ -9194,7 +9244,7 @@
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C52" t="s">
         <v>716</v>
@@ -9205,7 +9255,7 @@
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C53" t="s">
         <v>715</v>
@@ -9216,7 +9266,7 @@
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C54" t="s">
         <v>714</v>
@@ -9227,7 +9277,7 @@
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C55" t="s">
         <v>713</v>
@@ -9238,7 +9288,7 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C56" t="s">
         <v>712</v>
@@ -9249,7 +9299,7 @@
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C57" t="s">
         <v>711</v>
@@ -9260,7 +9310,7 @@
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C58" t="s">
         <v>710</v>
@@ -9277,7 +9327,7 @@
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C60" t="s">
         <v>719</v>
@@ -9288,21 +9338,21 @@
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C62" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E62" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="G62" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C64" t="s">
         <v>721</v>
@@ -9313,7 +9363,7 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C65" t="s">
         <v>722</v>
@@ -9330,17 +9380,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N109"/>
+  <dimension ref="B2:N119"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView tabSelected="1" workbookViewId="1">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9379,713 +9429,862 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>725</v>
+    <row r="3" spans="2:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="37"/>
+    </row>
+    <row r="4" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="D5" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>906</v>
+      </c>
+      <c r="C6" t="s">
+        <v>969</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>895</v>
-      </c>
-      <c r="C7" t="s">
-        <v>894</v>
+        <v>907</v>
       </c>
       <c r="D7" t="s">
-        <v>880</v>
-      </c>
-      <c r="F7" t="s">
-        <v>887</v>
+        <v>970</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>893</v>
-      </c>
-      <c r="C8" t="s">
-        <v>881</v>
+        <v>908</v>
       </c>
       <c r="D8" t="s">
-        <v>882</v>
-      </c>
-      <c r="J8">
-        <v>2008</v>
+        <v>971</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>883</v>
+        <v>909</v>
       </c>
       <c r="D9" t="s">
-        <v>887</v>
-      </c>
-      <c r="F9" t="s">
-        <v>886</v>
-      </c>
-      <c r="J9">
-        <v>2014</v>
+        <v>972</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>892</v>
+        <v>910</v>
       </c>
       <c r="C10" t="s">
-        <v>884</v>
+        <v>989</v>
       </c>
       <c r="D10" t="s">
-        <v>887</v>
-      </c>
-      <c r="F10" t="s">
-        <v>886</v>
-      </c>
-      <c r="J10">
-        <v>2003</v>
+        <v>973</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>891</v>
-      </c>
-      <c r="C11" t="s">
-        <v>885</v>
-      </c>
-      <c r="D11" t="s">
-        <v>887</v>
-      </c>
-      <c r="F11" t="s">
-        <v>886</v>
-      </c>
-      <c r="J11">
-        <v>1996</v>
+      <c r="B11" s="14" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>888</v>
-      </c>
-      <c r="C12" t="s">
-        <v>889</v>
-      </c>
-      <c r="D12" t="s">
-        <v>887</v>
-      </c>
-      <c r="J12">
-        <v>2010</v>
+      <c r="B12" s="14" t="s">
+        <v>991</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>890</v>
-      </c>
-      <c r="D13" t="s">
-        <v>887</v>
+      <c r="B13" s="14" t="s">
+        <v>992</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>998</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1002</v>
-      </c>
-      <c r="F14" t="s">
-        <v>973</v>
+        <v>993</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>999</v>
-      </c>
-      <c r="D15" t="s">
-        <v>973</v>
-      </c>
-      <c r="F15" t="s">
-        <v>973</v>
+        <v>994</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>911</v>
+      </c>
+      <c r="D17" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>912</v>
+      </c>
+      <c r="C21" t="s">
+        <v>981</v>
+      </c>
+      <c r="D21" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>913</v>
+      </c>
+      <c r="C22" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>914</v>
+      </c>
+      <c r="C23" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>915</v>
+      </c>
+      <c r="C24" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>886</v>
+      </c>
+      <c r="C25" t="s">
+        <v>887</v>
+      </c>
+      <c r="D25" t="s">
+        <v>885</v>
+      </c>
+      <c r="J25">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>881</v>
+      </c>
+      <c r="C26" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="39"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="23" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C29" t="s">
+        <v>887</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J29">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="28" t="s">
+        <v>881</v>
+      </c>
+      <c r="D30" t="s">
+        <v>885</v>
+      </c>
+      <c r="F30" t="s">
+        <v>884</v>
+      </c>
+      <c r="J30">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>996</v>
+      </c>
+      <c r="C31" t="s">
         <v>1000</v>
       </c>
-      <c r="C16" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F16" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
-        <v>1001</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1007</v>
-      </c>
-      <c r="F17" t="s">
-        <v>973</v>
-      </c>
-      <c r="J17">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>896</v>
-      </c>
-      <c r="C18" t="s">
-        <v>897</v>
-      </c>
-      <c r="D18" t="s">
-        <v>902</v>
-      </c>
-      <c r="J18">
-        <v>2014</v>
-      </c>
-      <c r="K18" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>898</v>
-      </c>
-      <c r="E19" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="F31" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>893</v>
+      </c>
+      <c r="C32" t="s">
+        <v>892</v>
+      </c>
+      <c r="D32" t="s">
+        <v>878</v>
+      </c>
+      <c r="F32" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>997</v>
+      </c>
+      <c r="D33" t="s">
+        <v>971</v>
+      </c>
+      <c r="F33" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>891</v>
+      </c>
+      <c r="C34" t="s">
+        <v>879</v>
+      </c>
+      <c r="D34" t="s">
+        <v>880</v>
+      </c>
+      <c r="J34">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C35" t="s">
+        <v>887</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J35">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>890</v>
+      </c>
+      <c r="C36" t="s">
+        <v>882</v>
+      </c>
+      <c r="D36" t="s">
+        <v>885</v>
+      </c>
+      <c r="F36" t="s">
+        <v>884</v>
+      </c>
+      <c r="J36">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>889</v>
+      </c>
+      <c r="C37" t="s">
+        <v>883</v>
+      </c>
+      <c r="D37" t="s">
+        <v>885</v>
+      </c>
+      <c r="F37" t="s">
+        <v>884</v>
+      </c>
+      <c r="J37">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>888</v>
+      </c>
+      <c r="D38" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="39"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>916</v>
+      </c>
+      <c r="C41" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J42">
+        <v>2010</v>
+      </c>
+      <c r="K42" t="s">
+        <v>205</v>
+      </c>
+      <c r="L42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D21" t="s">
-        <v>902</v>
-      </c>
-      <c r="F21" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
-        <v>898</v>
-      </c>
-      <c r="C22" t="s">
-        <v>900</v>
-      </c>
-      <c r="D22" t="s">
-        <v>902</v>
-      </c>
-      <c r="F22" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>901</v>
-      </c>
-      <c r="C24" t="s">
-        <v>904</v>
-      </c>
-      <c r="D24" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1009</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F26" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
-        <v>1006</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F27" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>907</v>
-      </c>
-      <c r="D30" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>908</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C43" s="7" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>917</v>
+      </c>
+      <c r="C44" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>918</v>
+      </c>
+      <c r="D45" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>909</v>
-      </c>
-      <c r="D32" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>910</v>
-      </c>
-      <c r="D33" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>911</v>
-      </c>
-      <c r="D34" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>912</v>
-      </c>
-      <c r="C35" t="s">
-        <v>991</v>
-      </c>
-      <c r="D35" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>913</v>
-      </c>
-      <c r="D42" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="14" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>914</v>
-      </c>
-      <c r="C46" t="s">
+        <v>919</v>
+      </c>
+      <c r="D46" t="s">
         <v>983</v>
       </c>
-      <c r="D46" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="C47" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="C48" t="s">
-        <v>979</v>
+        <v>985</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>917</v>
-      </c>
-      <c r="C49" t="s">
-        <v>980</v>
+        <v>922</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>883</v>
-      </c>
-      <c r="C50" t="s">
-        <v>887</v>
+        <v>923</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>918</v>
-      </c>
-      <c r="C51" t="s">
-        <v>981</v>
+        <v>894</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>901</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>982</v>
+        <v>920</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>919</v>
-      </c>
-      <c r="C53" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>920</v>
-      </c>
-      <c r="D54" t="s">
-        <v>973</v>
+        <v>924</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>921</v>
+      <c r="B55" s="5" t="s">
+        <v>903</v>
       </c>
       <c r="D55" t="s">
-        <v>985</v>
+        <v>968</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>922</v>
-      </c>
-      <c r="C56" t="s">
-        <v>986</v>
+        <v>925</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>923</v>
-      </c>
-      <c r="C57" t="s">
-        <v>987</v>
+        <v>926</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>896</v>
+        <v>929</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>922</v>
+        <v>930</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>926</v>
+        <v>931</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
-        <v>905</v>
-      </c>
-      <c r="D64" t="s">
-        <v>970</v>
+      <c r="B64" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>928</v>
+        <v>934</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>929</v>
+      <c r="B67" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="D67" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>930</v>
+        <v>935</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>931</v>
+        <v>936</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>932</v>
+        <v>937</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>934</v>
+        <v>939</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>936</v>
+        <v>941</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="5" t="s">
-        <v>906</v>
-      </c>
-      <c r="D76" t="s">
-        <v>970</v>
+      <c r="B76" t="s">
+        <v>943</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>937</v>
+        <v>944</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>938</v>
+        <v>945</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>939</v>
+        <v>946</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>940</v>
+        <v>947</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>943</v>
+        <v>950</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>944</v>
+        <v>951</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>945</v>
+        <v>952</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>946</v>
+        <v>953</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>947</v>
+        <v>954</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>950</v>
+        <v>957</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="37"/>
+      <c r="C101" s="37"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+      <c r="J101" s="37"/>
+      <c r="K101" s="37"/>
+      <c r="L101" s="38"/>
+      <c r="M101" s="37"/>
+    </row>
+    <row r="102" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="39"/>
+      <c r="C102" s="39"/>
+      <c r="D102" s="39"/>
+      <c r="E102" s="39"/>
+      <c r="F102" s="39"/>
+      <c r="G102" s="39"/>
+      <c r="H102" s="39"/>
+      <c r="I102" s="39"/>
+      <c r="J102" s="39"/>
+      <c r="K102" s="39"/>
+      <c r="L102" s="40"/>
+      <c r="M102" s="39"/>
+    </row>
+    <row r="104" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B104" s="14" t="s">
+        <v>998</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F104" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="105" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B106" s="14" t="s">
+        <v>999</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F106" t="s">
+        <v>971</v>
+      </c>
+      <c r="J106">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B107" s="14"/>
+    </row>
+    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+      <c r="C108" t="s">
+        <v>895</v>
+      </c>
+      <c r="D108" t="s">
+        <v>900</v>
+      </c>
+      <c r="J108">
+        <v>2014</v>
+      </c>
+      <c r="K108" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>969</v>
-      </c>
+        <v>896</v>
+      </c>
+      <c r="E109" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B111" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D111" t="s">
+        <v>900</v>
+      </c>
+      <c r="F111" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B112" s="14" t="s">
+        <v>896</v>
+      </c>
+      <c r="C112" t="s">
+        <v>898</v>
+      </c>
+      <c r="D112" t="s">
+        <v>900</v>
+      </c>
+      <c r="F112" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>899</v>
+      </c>
+      <c r="C114" t="s">
+        <v>902</v>
+      </c>
+      <c r="D114" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B116" s="14" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F116" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B117" s="14" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F117" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="39"/>
+      <c r="H119" s="39"/>
+      <c r="I119" s="39"/>
+      <c r="J119" s="39"/>
+      <c r="K119" s="39"/>
+      <c r="L119" s="40"/>
+      <c r="M119" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10095,23 +10294,105 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>727</v>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor additions, esp. to IFC
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="12630" windowHeight="7515"/>
-    <workbookView xWindow="-510" yWindow="75" windowWidth="14805" windowHeight="7590" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-510" yWindow="75" windowWidth="14805" windowHeight="7590" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
     <sheet name="ADB_resources" sheetId="4" r:id="rId2"/>
     <sheet name="WB" sheetId="2" r:id="rId3"/>
-    <sheet name="WB_sourcebook" sheetId="5" r:id="rId4"/>
+    <sheet name="WB_resources" sheetId="5" r:id="rId4"/>
     <sheet name="IDB" sheetId="6" r:id="rId5"/>
     <sheet name="IFC" sheetId="3" r:id="rId6"/>
     <sheet name="EBRD" sheetId="7" r:id="rId7"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1036">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -2422,66 +2422,15 @@
     <t>General Operational Policies</t>
   </si>
   <si>
-    <t>101 General Information</t>
-  </si>
-  <si>
-    <t>102 Access to Information</t>
-  </si>
-  <si>
-    <t>201 The Country and Subregional Programming Process</t>
-  </si>
-  <si>
-    <t>202 The Bank's Operations Program</t>
-  </si>
-  <si>
     <t>OPERATIONS PROGRAMING</t>
   </si>
   <si>
     <t>LENDING POLICIES</t>
   </si>
   <si>
-    <t>301 Eligible Borrowers</t>
-  </si>
-  <si>
-    <t>302 Project Preparation, Evaluation and Approval</t>
-  </si>
-  <si>
-    <t>303 Guarantees Required from the Borrower</t>
-  </si>
-  <si>
-    <t>304 Operations Administration</t>
-  </si>
-  <si>
-    <t>305 ExPost Evaluation</t>
-  </si>
-  <si>
-    <t>307 Amount of Loan in Foreign Exchange</t>
-  </si>
-  <si>
-    <t>308 Financing of Interest</t>
-  </si>
-  <si>
-    <t>309 Global Loans to Intermediary Financial Institutions - Contributions by Subborrowers</t>
-  </si>
-  <si>
-    <t>310 Financing Increase of Cost Overruns for Operations in Execution</t>
-  </si>
-  <si>
-    <t>311 Eligible Expenditures in Investment Loans</t>
-  </si>
-  <si>
     <t>TECHNICAL COOPERATION POLICIES</t>
   </si>
   <si>
-    <t>400 Technical Cooperation Policy</t>
-  </si>
-  <si>
-    <t>401 Framework for Technical Cooperation</t>
-  </si>
-  <si>
-    <t>402 TC Taxonomy and Forms of Financing</t>
-  </si>
-  <si>
     <t xml:space="preserve">PROCUREMENT OF GOODS AND SERVICES </t>
   </si>
   <si>
@@ -2491,12 +2440,6 @@
     <t>SUBREGIONAL FINANCIAL INSTITUTIONS</t>
   </si>
   <si>
-    <t>601 Relationship with Subregional Financial Institutions - General Policy</t>
-  </si>
-  <si>
-    <t>602 Cooperation with Other Sources of Financing</t>
-  </si>
-  <si>
     <t>http://www.iadb.org/en/about-us/general-operational-policies,6236.html</t>
   </si>
   <si>
@@ -2524,9 +2467,6 @@
     <t>http://www.iadb.org/en/about-us/financing-and-mobilization-of-resources,6243.html</t>
   </si>
   <si>
-    <t>306 Forms of Bank Financing and Assistance for the Mobilization of Financial Resources</t>
-  </si>
-  <si>
     <t>http://www.iadb.org/en/about-us/loans-in-foreign-exchange,6244.html</t>
   </si>
   <si>
@@ -2563,84 +2503,15 @@
     <t>Multisectoral Policies</t>
   </si>
   <si>
-    <t>703 Environment and Safeguards Compliance</t>
-  </si>
-  <si>
-    <t>704 Natural Disaster Risk Management</t>
-  </si>
-  <si>
-    <t>707 Maintenance and Conservation of Physical Works and Equipment</t>
-  </si>
-  <si>
-    <t>708 Public Utilities (Feb 2014)</t>
-  </si>
-  <si>
-    <t>710 Involuntary Resettlement</t>
-  </si>
-  <si>
     <t>Economic Infrastructure Sectors</t>
   </si>
   <si>
-    <t>733 Energy</t>
-  </si>
-  <si>
-    <t>733-1 Electric Energy</t>
-  </si>
-  <si>
     <t>Policies for Special Areas</t>
   </si>
   <si>
-    <t>761 Gender Equality in Development</t>
-  </si>
-  <si>
-    <t>765 Indigenous Peoples</t>
-  </si>
-  <si>
     <t>Sector Framework Documents</t>
   </si>
   <si>
-    <t>2001 Agriculture and Natural Resource Management</t>
-  </si>
-  <si>
-    <t>2002 Education and Early Childhood Development</t>
-  </si>
-  <si>
-    <t>2003 Integration and Trade</t>
-  </si>
-  <si>
-    <t>2004 Urban Development and Housing</t>
-  </si>
-  <si>
-    <t>2005 Health and Nutrition</t>
-  </si>
-  <si>
-    <t>2006 Labor</t>
-  </si>
-  <si>
-    <t>2007 Transportation</t>
-  </si>
-  <si>
-    <t>2008 Support to SMEs and Financial Access/Supervision</t>
-  </si>
-  <si>
-    <t>2009 Citizen Security and Justice</t>
-  </si>
-  <si>
-    <t>2010 Tourism</t>
-  </si>
-  <si>
-    <t>2011 Social Protection and Poverty</t>
-  </si>
-  <si>
-    <t>2012 Water and Sanitation</t>
-  </si>
-  <si>
-    <t>2013 Innovation, Science and Technology</t>
-  </si>
-  <si>
-    <t>2014 Gender and Diversity</t>
-  </si>
-  <si>
     <t>http://www.iadb.org/document.cfm?id=35004515</t>
   </si>
   <si>
@@ -3098,6 +2969,168 @@
   </si>
   <si>
     <t>Environmental and Social Policy and Performance Requirements</t>
+  </si>
+  <si>
+    <t>733-1</t>
+  </si>
+  <si>
+    <t>Operations Programing</t>
+  </si>
+  <si>
+    <t>Lending Policies</t>
+  </si>
+  <si>
+    <t>Technical Cooperation Policies</t>
+  </si>
+  <si>
+    <t>grievence redress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procurement Of Goods And Services </t>
+  </si>
+  <si>
+    <t>Subregional Financial Institutions</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>Access to Information</t>
+  </si>
+  <si>
+    <t>The Country and Subregional Programming Process</t>
+  </si>
+  <si>
+    <t>The Bank's Operations Program</t>
+  </si>
+  <si>
+    <t>Eligible Borrowers</t>
+  </si>
+  <si>
+    <t>Project Preparation, Evaluation and Approval</t>
+  </si>
+  <si>
+    <t>Guarantees Required from the Borrower</t>
+  </si>
+  <si>
+    <t>Operations Administration</t>
+  </si>
+  <si>
+    <t>ExPost Evaluation</t>
+  </si>
+  <si>
+    <t>Forms of Bank Financing and Assistance for the Mobilization of Financial Resources</t>
+  </si>
+  <si>
+    <t>Amount of Loan in Foreign Exchange</t>
+  </si>
+  <si>
+    <t>Financing of Interest</t>
+  </si>
+  <si>
+    <t>Global Loans to Intermediary Financial Institutions - Contributions by Subborrowers</t>
+  </si>
+  <si>
+    <t>Financing Increase of Cost Overruns for Operations in Execution</t>
+  </si>
+  <si>
+    <t>Eligible Expenditures in Investment Loans</t>
+  </si>
+  <si>
+    <t>Technical Cooperation Policy</t>
+  </si>
+  <si>
+    <t>Framework for Technical Cooperation</t>
+  </si>
+  <si>
+    <t>TC Taxonomy and Forms of Financing</t>
+  </si>
+  <si>
+    <t>Relationship with Subregional Financial Institutions - General Policy</t>
+  </si>
+  <si>
+    <t>Cooperation with Other Sources of Financing</t>
+  </si>
+  <si>
+    <t>Environment and Safeguards Compliance</t>
+  </si>
+  <si>
+    <t>Gender and Diversity</t>
+  </si>
+  <si>
+    <t>Innovation, Science and Technology</t>
+  </si>
+  <si>
+    <t>Water and Sanitation</t>
+  </si>
+  <si>
+    <t>Social Protection and Poverty</t>
+  </si>
+  <si>
+    <t>Tourism</t>
+  </si>
+  <si>
+    <t>Citizen Security and Justice</t>
+  </si>
+  <si>
+    <t>Support to SMEs and Financial Access/Supervision</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Health and Nutrition</t>
+  </si>
+  <si>
+    <t>Urban Development and Housing</t>
+  </si>
+  <si>
+    <t>Integration and Trade</t>
+  </si>
+  <si>
+    <t>Education and Early Childhood Development</t>
+  </si>
+  <si>
+    <t>Agriculture and Natural Resource Management</t>
+  </si>
+  <si>
+    <t>Gender Equality in Development</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Electric Energy</t>
+  </si>
+  <si>
+    <t>Public Utilities (Feb 2014)</t>
+  </si>
+  <si>
+    <t>Maintenance and Conservation of Physical Works and Equipment</t>
+  </si>
+  <si>
+    <t>Natural Disaster Risk Management</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=1481950</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=35597106</t>
+  </si>
+  <si>
+    <t>Background paper on New Access to Information Policy</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=35167427</t>
+  </si>
+  <si>
+    <t>Implementation Plan (September 2010)</t>
+  </si>
+  <si>
+    <t>Information Disclosure Policy Implementation Instructions (Revised December 2009)</t>
   </si>
 </sst>
 </file>
@@ -6221,8 +6254,8 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
-    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="1">
-      <selection activeCell="C10" sqref="C10:O10"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="1">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8092,7 +8125,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1">
-      <selection activeCell="H2" sqref="H2:J2"/>
+      <selection activeCell="C10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8165,649 +8198,939 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+    <row r="1" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="21"/>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="21" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
         <v>762</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>761</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>754</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>760</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>759</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>758</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>764</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>765</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>767</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>768</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1999</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>769</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>770</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>663</v>
       </c>
       <c r="D11" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E11" t="s">
         <v>771</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2011</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="14" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="14" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="14" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>772</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F15" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>774</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E16" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>777</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F17" t="s">
         <v>776</v>
       </c>
-      <c r="J14">
+      <c r="K17">
         <v>2006</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>778</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E19" t="s">
         <v>780</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F19" t="s">
         <v>779</v>
       </c>
-      <c r="J16">
+      <c r="K19">
         <v>2011</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>781</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E20" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C22" t="s">
         <v>764</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="7" t="s">
+      <c r="E22" s="5"/>
+      <c r="F22" s="7" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C23" t="s">
         <v>783</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F23" t="s">
         <v>785</v>
       </c>
-      <c r="J20">
+      <c r="K23">
         <v>2006</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C25" t="s">
         <v>767</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F25" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C26" t="s">
         <v>769</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F26" t="s">
         <v>787</v>
       </c>
-      <c r="J23">
+      <c r="K26">
         <v>1999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>788</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E28" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>789</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F29" t="s">
         <v>790</v>
       </c>
-      <c r="J26">
+      <c r="K29">
         <v>2013</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="D31" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="F32" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="39" spans="2:4" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="42" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>798</v>
+      </c>
+      <c r="B46">
+        <v>101</v>
+      </c>
+      <c r="C46" t="s">
+        <v>989</v>
+      </c>
+      <c r="E46" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>798</v>
+      </c>
+      <c r="B47">
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>990</v>
+      </c>
+      <c r="E47" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>799</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>983</v>
+      </c>
+      <c r="B49">
+        <v>201</v>
+      </c>
+      <c r="C49" t="s">
+        <v>991</v>
+      </c>
+      <c r="E49" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>983</v>
+      </c>
+      <c r="B50">
+        <v>202</v>
+      </c>
+      <c r="C50" t="s">
+        <v>992</v>
+      </c>
+      <c r="E50" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>984</v>
+      </c>
+      <c r="B52">
+        <v>301</v>
+      </c>
+      <c r="C52" t="s">
+        <v>993</v>
+      </c>
+      <c r="E52" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>984</v>
+      </c>
+      <c r="B53">
+        <v>302</v>
+      </c>
+      <c r="C53" t="s">
+        <v>994</v>
+      </c>
+      <c r="E53" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>984</v>
+      </c>
+      <c r="B54">
+        <v>303</v>
+      </c>
+      <c r="C54" t="s">
+        <v>995</v>
+      </c>
+      <c r="E54" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>984</v>
+      </c>
+      <c r="B55">
+        <v>304</v>
+      </c>
+      <c r="C55" t="s">
+        <v>996</v>
+      </c>
+      <c r="E55" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>984</v>
+      </c>
+      <c r="B56">
+        <v>305</v>
+      </c>
+      <c r="C56" t="s">
+        <v>997</v>
+      </c>
+      <c r="E56" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>984</v>
+      </c>
+      <c r="B57">
+        <v>306</v>
+      </c>
+      <c r="C57" t="s">
+        <v>998</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>984</v>
+      </c>
+      <c r="B58">
+        <v>307</v>
+      </c>
+      <c r="C58" t="s">
+        <v>999</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>984</v>
+      </c>
+      <c r="B59">
+        <v>308</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>984</v>
+      </c>
+      <c r="B60">
+        <v>309</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>984</v>
+      </c>
+      <c r="B61">
+        <v>310</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>984</v>
+      </c>
+      <c r="B62">
+        <v>311</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>985</v>
+      </c>
+      <c r="B64">
+        <v>400</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E64" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>985</v>
+      </c>
+      <c r="B65">
+        <v>401</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E65" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>985</v>
+      </c>
+      <c r="B66">
+        <v>402</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E66" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>987</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" t="s">
+        <v>803</v>
+      </c>
+      <c r="E68" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>988</v>
+      </c>
+      <c r="B70">
+        <v>601</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E70" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>988</v>
+      </c>
+      <c r="B71">
+        <v>602</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E71" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>800</v>
-      </c>
-      <c r="D44" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>801</v>
-      </c>
-      <c r="D46" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>988</v>
+      </c>
+      <c r="C72" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>802</v>
-      </c>
-      <c r="D47" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>988</v>
+      </c>
+      <c r="B73">
+        <v>703</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E73" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>988</v>
+      </c>
+      <c r="B74">
+        <v>704</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E74" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>988</v>
+      </c>
+      <c r="B75">
+        <v>707</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E75" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>988</v>
+      </c>
+      <c r="B76">
+        <v>708</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E76" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>988</v>
+      </c>
+      <c r="B77">
+        <v>710</v>
+      </c>
+      <c r="C77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>805</v>
-      </c>
-      <c r="D49" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>826</v>
+      </c>
+      <c r="B79">
+        <v>733</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E79" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>826</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E80" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>806</v>
-      </c>
-      <c r="D50" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>827</v>
+      </c>
+      <c r="B82">
+        <v>761</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>827</v>
+      </c>
+      <c r="B83">
+        <v>765</v>
+      </c>
+      <c r="C83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>807</v>
-      </c>
-      <c r="D51" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>808</v>
-      </c>
-      <c r="D52" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>809</v>
-      </c>
-      <c r="D53" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>833</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>810</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>811</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>812</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>813</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>814</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>816</v>
-      </c>
-      <c r="D61" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>817</v>
-      </c>
-      <c r="D62" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>818</v>
-      </c>
-      <c r="D63" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>820</v>
-      </c>
-      <c r="D65" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>822</v>
-      </c>
-      <c r="D67" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>823</v>
-      </c>
-      <c r="D68" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>846</v>
-      </c>
-      <c r="D70" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>847</v>
-      </c>
-      <c r="D71" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>848</v>
-      </c>
-      <c r="D72" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>849</v>
-      </c>
-      <c r="D73" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>850</v>
-      </c>
-      <c r="D74" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>852</v>
-      </c>
-      <c r="D76" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>853</v>
-      </c>
-      <c r="D77" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>871</v>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>828</v>
+      </c>
+      <c r="B85">
+        <v>2001</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>828</v>
+      </c>
+      <c r="B86">
+        <v>2002</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>828</v>
+      </c>
+      <c r="B87">
+        <v>2003</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>828</v>
+      </c>
+      <c r="B88">
+        <v>2004</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>828</v>
+      </c>
+      <c r="B89">
+        <v>2005</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>828</v>
+      </c>
+      <c r="B90">
+        <v>2006</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>828</v>
+      </c>
+      <c r="B91">
+        <v>2007</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>828</v>
+      </c>
+      <c r="B92">
+        <v>2008</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>828</v>
+      </c>
+      <c r="B93">
+        <v>2009</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>828</v>
+      </c>
+      <c r="B94">
+        <v>2010</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>828</v>
+      </c>
+      <c r="B95">
+        <v>2011</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>828</v>
+      </c>
+      <c r="B96">
+        <v>2012</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>828</v>
+      </c>
+      <c r="B97">
+        <v>2013</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>828</v>
+      </c>
+      <c r="B98">
+        <v>2014</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1010</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8818,16 +9141,19 @@
     <sheetView workbookViewId="0"/>
     <sheetView zoomScaleNormal="100" workbookViewId="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C2" s="21" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" s="21" t="s">
         <v>152</v>
       </c>
@@ -9095,6 +9421,9 @@
     </row>
     <row r="32" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>745</v>
+      </c>
       <c r="C34" t="s">
         <v>740</v>
       </c>
@@ -9103,6 +9432,9 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>745</v>
+      </c>
       <c r="C35" t="s">
         <v>739</v>
       </c>
@@ -9111,6 +9443,9 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>986</v>
+      </c>
       <c r="C36" t="s">
         <v>738</v>
       </c>
@@ -9380,12 +9715,12 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N119"/>
+  <dimension ref="B2:N116"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9446,152 +9781,152 @@
     <row r="4" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>905</v>
+        <v>862</v>
       </c>
       <c r="D5" t="s">
-        <v>968</v>
+        <v>925</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>906</v>
+        <v>863</v>
       </c>
       <c r="C6" t="s">
-        <v>969</v>
+        <v>926</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>907</v>
+        <v>864</v>
       </c>
       <c r="D7" t="s">
-        <v>970</v>
+        <v>927</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>908</v>
+        <v>865</v>
       </c>
       <c r="D8" t="s">
-        <v>971</v>
+        <v>928</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>909</v>
+        <v>866</v>
       </c>
       <c r="D9" t="s">
-        <v>972</v>
+        <v>929</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>910</v>
+        <v>867</v>
       </c>
       <c r="C10" t="s">
-        <v>989</v>
+        <v>946</v>
       </c>
       <c r="D10" t="s">
-        <v>973</v>
+        <v>930</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>990</v>
+        <v>947</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>991</v>
+        <v>948</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>992</v>
+        <v>949</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>993</v>
+        <v>950</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>994</v>
+        <v>951</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>995</v>
+        <v>952</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>911</v>
+        <v>868</v>
       </c>
       <c r="D17" t="s">
-        <v>974</v>
+        <v>931</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>986</v>
+        <v>943</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>987</v>
+        <v>944</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>988</v>
+        <v>945</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>912</v>
+        <v>869</v>
       </c>
       <c r="C21" t="s">
-        <v>981</v>
+        <v>938</v>
       </c>
       <c r="D21" t="s">
-        <v>975</v>
+        <v>932</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>913</v>
+        <v>870</v>
       </c>
       <c r="C22" t="s">
-        <v>976</v>
+        <v>933</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>914</v>
+        <v>871</v>
       </c>
       <c r="C23" t="s">
-        <v>977</v>
+        <v>934</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>915</v>
+        <v>872</v>
       </c>
       <c r="C24" t="s">
-        <v>978</v>
+        <v>935</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>886</v>
+        <v>843</v>
       </c>
       <c r="C25" t="s">
-        <v>887</v>
+        <v>844</v>
       </c>
       <c r="D25" t="s">
-        <v>885</v>
+        <v>842</v>
       </c>
       <c r="J25">
         <v>2010</v>
@@ -9599,10 +9934,10 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>881</v>
+        <v>838</v>
       </c>
       <c r="C26" t="s">
-        <v>885</v>
+        <v>842</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -9632,13 +9967,13 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="23" t="s">
-        <v>1024</v>
+        <v>981</v>
       </c>
       <c r="C29" t="s">
-        <v>887</v>
+        <v>844</v>
       </c>
       <c r="F29" t="s">
-        <v>1020</v>
+        <v>977</v>
       </c>
       <c r="J29">
         <v>2008</v>
@@ -9646,645 +9981,677 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="28" t="s">
-        <v>881</v>
+        <v>838</v>
       </c>
       <c r="D30" t="s">
-        <v>885</v>
+        <v>842</v>
       </c>
       <c r="F30" t="s">
-        <v>884</v>
+        <v>841</v>
       </c>
       <c r="J30">
         <v>2014</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>996</v>
+      <c r="B31" t="s">
+        <v>850</v>
       </c>
       <c r="C31" t="s">
-        <v>1000</v>
+        <v>849</v>
+      </c>
+      <c r="D31" t="s">
+        <v>835</v>
       </c>
       <c r="F31" t="s">
-        <v>971</v>
+        <v>842</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>893</v>
+      <c r="B32" s="14" t="s">
+        <v>953</v>
       </c>
       <c r="C32" t="s">
-        <v>892</v>
-      </c>
-      <c r="D32" t="s">
-        <v>878</v>
+        <v>957</v>
       </c>
       <c r="F32" t="s">
-        <v>885</v>
+        <v>928</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>997</v>
-      </c>
-      <c r="D33" t="s">
-        <v>971</v>
+        <v>956</v>
+      </c>
+      <c r="C33" t="s">
+        <v>962</v>
       </c>
       <c r="F33" t="s">
-        <v>971</v>
+        <v>928</v>
+      </c>
+      <c r="J33">
+        <v>1992</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>891</v>
+      <c r="B34" s="11" t="s">
+        <v>955</v>
       </c>
       <c r="C34" t="s">
-        <v>879</v>
-      </c>
-      <c r="D34" t="s">
-        <v>880</v>
-      </c>
-      <c r="J34">
-        <v>2008</v>
+        <v>958</v>
+      </c>
+      <c r="F34" t="s">
+        <v>928</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>1024</v>
-      </c>
-      <c r="C35" t="s">
-        <v>887</v>
+        <v>954</v>
+      </c>
+      <c r="D35" t="s">
+        <v>928</v>
       </c>
       <c r="F35" t="s">
-        <v>1020</v>
-      </c>
-      <c r="J35">
-        <v>2008</v>
+        <v>928</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>890</v>
+        <v>848</v>
       </c>
       <c r="C36" t="s">
-        <v>882</v>
+        <v>836</v>
       </c>
       <c r="D36" t="s">
-        <v>885</v>
-      </c>
-      <c r="F36" t="s">
-        <v>884</v>
+        <v>837</v>
       </c>
       <c r="J36">
-        <v>2003</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>889</v>
+      <c r="B37" s="14" t="s">
+        <v>981</v>
       </c>
       <c r="C37" t="s">
-        <v>883</v>
-      </c>
-      <c r="D37" t="s">
-        <v>885</v>
+        <v>844</v>
       </c>
       <c r="F37" t="s">
-        <v>884</v>
+        <v>977</v>
       </c>
       <c r="J37">
-        <v>1996</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>888</v>
+        <v>847</v>
+      </c>
+      <c r="C38" t="s">
+        <v>839</v>
       </c>
       <c r="D38" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="39"/>
+        <v>842</v>
+      </c>
+      <c r="F38" t="s">
+        <v>841</v>
+      </c>
+      <c r="J38">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>846</v>
+      </c>
+      <c r="C39" t="s">
+        <v>840</v>
+      </c>
+      <c r="D39" t="s">
+        <v>842</v>
+      </c>
+      <c r="F39" t="s">
+        <v>841</v>
+      </c>
+      <c r="J39">
+        <v>1996</v>
+      </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>916</v>
-      </c>
-      <c r="C41" t="s">
-        <v>979</v>
-      </c>
+      <c r="B40" t="s">
+        <v>845</v>
+      </c>
+      <c r="D40" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="39"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
-        <v>1023</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1022</v>
-      </c>
-      <c r="D42" t="s">
-        <v>1021</v>
-      </c>
-      <c r="J42">
-        <v>2010</v>
-      </c>
-      <c r="K42" t="s">
-        <v>205</v>
-      </c>
-      <c r="L42">
-        <v>3</v>
-      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>899</v>
-      </c>
-      <c r="C43" s="7" t="s">
+        <v>873</v>
+      </c>
+      <c r="C43" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
         <v>980</v>
       </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>917</v>
-      </c>
       <c r="C44" t="s">
-        <v>982</v>
+        <v>979</v>
+      </c>
+      <c r="D44" t="s">
+        <v>978</v>
+      </c>
+      <c r="J44">
+        <v>2010</v>
+      </c>
+      <c r="K44" t="s">
+        <v>205</v>
+      </c>
+      <c r="L44">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>918</v>
-      </c>
-      <c r="D45" t="s">
-        <v>971</v>
+        <v>856</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>919</v>
+      <c r="B46" s="14" t="s">
+        <v>856</v>
+      </c>
+      <c r="C46" t="s">
+        <v>859</v>
       </c>
       <c r="D46" t="s">
-        <v>983</v>
+        <v>858</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>920</v>
+        <v>874</v>
       </c>
       <c r="C47" t="s">
-        <v>984</v>
+        <v>939</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>875</v>
+      </c>
+      <c r="D48" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>876</v>
+      </c>
+      <c r="D49" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>877</v>
+      </c>
+      <c r="C50" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>878</v>
+      </c>
+      <c r="C51" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="14" t="s">
+        <v>960</v>
+      </c>
+      <c r="C54" t="s">
+        <v>964</v>
+      </c>
+      <c r="D54" t="s">
+        <v>966</v>
+      </c>
+      <c r="F54" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>961</v>
+      </c>
+      <c r="C55" t="s">
+        <v>965</v>
+      </c>
+      <c r="F55" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="39"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="39"/>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>851</v>
+      </c>
+      <c r="C59" t="s">
+        <v>852</v>
+      </c>
+      <c r="D59" t="s">
+        <v>857</v>
+      </c>
+      <c r="J59">
+        <v>2014</v>
+      </c>
+      <c r="K59" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>853</v>
+      </c>
+      <c r="E60" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B62" s="14" t="s">
+        <v>959</v>
+      </c>
+      <c r="C62" t="s">
+        <v>963</v>
+      </c>
+      <c r="D62" t="s">
+        <v>857</v>
+      </c>
+      <c r="F62" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="14" t="s">
+        <v>853</v>
+      </c>
+      <c r="C63" t="s">
+        <v>855</v>
+      </c>
+      <c r="D63" t="s">
+        <v>857</v>
+      </c>
+      <c r="F63" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="39"/>
+      <c r="J64" s="39"/>
+      <c r="K64" s="39"/>
+      <c r="L64" s="40"/>
+      <c r="M64" s="39"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="D69" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="D81" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
         <v>921</v>
       </c>
-      <c r="C48" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
         <v>923</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
-        <v>903</v>
-      </c>
-      <c r="D55" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="5" t="s">
-        <v>904</v>
-      </c>
-      <c r="D67" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="101" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="37"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="37"/>
-      <c r="H101" s="37"/>
-      <c r="I101" s="37"/>
-      <c r="J101" s="37"/>
-      <c r="K101" s="37"/>
-      <c r="L101" s="38"/>
-      <c r="M101" s="37"/>
-    </row>
-    <row r="102" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="39"/>
-      <c r="C102" s="39"/>
-      <c r="D102" s="39"/>
-      <c r="E102" s="39"/>
-      <c r="F102" s="39"/>
-      <c r="G102" s="39"/>
-      <c r="H102" s="39"/>
-      <c r="I102" s="39"/>
-      <c r="J102" s="39"/>
-      <c r="K102" s="39"/>
-      <c r="L102" s="40"/>
-      <c r="M102" s="39"/>
-    </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B104" s="14" t="s">
-        <v>998</v>
-      </c>
-      <c r="C104" t="s">
-        <v>1001</v>
-      </c>
-      <c r="F104" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="105" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B106" s="14" t="s">
-        <v>999</v>
-      </c>
-      <c r="C106" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F106" t="s">
-        <v>971</v>
-      </c>
-      <c r="J106">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B107" s="14"/>
-    </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>894</v>
-      </c>
-      <c r="C108" t="s">
-        <v>895</v>
-      </c>
-      <c r="D108" t="s">
-        <v>900</v>
-      </c>
-      <c r="J108">
-        <v>2014</v>
-      </c>
-      <c r="K108" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>896</v>
-      </c>
-      <c r="E109" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B111" s="14" t="s">
-        <v>1002</v>
-      </c>
-      <c r="C111" t="s">
-        <v>1006</v>
-      </c>
-      <c r="D111" t="s">
-        <v>900</v>
-      </c>
-      <c r="F111" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B112" s="14" t="s">
-        <v>896</v>
-      </c>
-      <c r="C112" t="s">
-        <v>898</v>
-      </c>
-      <c r="D112" t="s">
-        <v>900</v>
-      </c>
-      <c r="F112" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="114" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>899</v>
-      </c>
-      <c r="C114" t="s">
-        <v>902</v>
-      </c>
-      <c r="D114" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B116" s="14" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C116" t="s">
-        <v>1007</v>
-      </c>
-      <c r="D116" t="s">
-        <v>1009</v>
-      </c>
-      <c r="F116" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B117" s="14" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C117" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F117" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="119" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="39"/>
-      <c r="I119" s="39"/>
-      <c r="J119" s="39"/>
-      <c r="K119" s="39"/>
-      <c r="L119" s="40"/>
-      <c r="M119" s="39"/>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="115" spans="2:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="37"/>
+      <c r="C115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="37"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="37"/>
+      <c r="K115" s="37"/>
+      <c r="L115" s="38"/>
+      <c r="M115" s="37"/>
+    </row>
+    <row r="116" spans="2:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="39"/>
+      <c r="C116" s="39"/>
+      <c r="D116" s="39"/>
+      <c r="E116" s="39"/>
+      <c r="F116" s="39"/>
+      <c r="G116" s="39"/>
+      <c r="H116" s="39"/>
+      <c r="I116" s="39"/>
+      <c r="J116" s="39"/>
+      <c r="K116" s="39"/>
+      <c r="L116" s="40"/>
+      <c r="M116" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10353,46 +10720,46 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1010</v>
+        <v>967</v>
       </c>
       <c r="C6" t="s">
-        <v>1013</v>
+        <v>970</v>
       </c>
       <c r="D6" t="s">
-        <v>1014</v>
+        <v>971</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1011</v>
+        <v>968</v>
       </c>
       <c r="C7" t="s">
-        <v>1015</v>
+        <v>972</v>
       </c>
       <c r="D7" t="s">
-        <v>1014</v>
+        <v>971</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1012</v>
+        <v>969</v>
       </c>
       <c r="C8" t="s">
-        <v>1016</v>
+        <v>973</v>
       </c>
       <c r="D8" t="s">
-        <v>1014</v>
+        <v>971</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>1017</v>
+        <v>974</v>
       </c>
       <c r="C10" t="s">
-        <v>1019</v>
+        <v>976</v>
       </c>
       <c r="D10" t="s">
-        <v>1018</v>
+        <v>975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filling in URL data for IDB
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="12630" windowHeight="7515"/>
-    <workbookView xWindow="-510" yWindow="75" windowWidth="14805" windowHeight="7590" activeTab="4"/>
+    <workbookView xWindow="-510" yWindow="75" windowWidth="14805" windowHeight="7590" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,11 @@
     <sheet name="WB" sheetId="2" r:id="rId3"/>
     <sheet name="WB_resources" sheetId="5" r:id="rId4"/>
     <sheet name="IDB" sheetId="6" r:id="rId5"/>
-    <sheet name="IFC" sheetId="3" r:id="rId6"/>
-    <sheet name="EBRD" sheetId="7" r:id="rId7"/>
-    <sheet name="OPIC" sheetId="8" r:id="rId8"/>
+    <sheet name="IDB_resources" sheetId="9" r:id="rId6"/>
+    <sheet name="IFC" sheetId="3" r:id="rId7"/>
+    <sheet name="IFC_resources" sheetId="10" r:id="rId8"/>
+    <sheet name="EBRD" sheetId="7" r:id="rId9"/>
+    <sheet name="OPIC" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="1082">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -3131,6 +3133,144 @@
   </si>
   <si>
     <t>Information Disclosure Policy Implementation Instructions (Revised December 2009)</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=35004515</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=360026</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=1442307</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=2032081</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=822598</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=362003</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=35428399</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/research-and-data/regional-policy-dialogue/disaster-risk-management-network,17733.html</t>
+  </si>
+  <si>
+    <t>Disaster Risk Management Network: Regional Policy Dialogue</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/natural-disasters/disaster-risk-indicators/disaster-risk-indicators,1456.html</t>
+  </si>
+  <si>
+    <t>Disaster Risk Indicators</t>
+  </si>
+  <si>
+    <t>Sustainability and Safeguards Policies</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/sustainability/sustainability-and-safeguards-policies,1515.html</t>
+  </si>
+  <si>
+    <t>Helping Latin America and the Caribbean manage natural disaster risks</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/natural-disasters/natural-disasters,1441.html</t>
+  </si>
+  <si>
+    <t>Climate Change and Disaster Risk Management</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/environment/climate-change-and-disaster-risk-management,2689.html</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=36344547</t>
+  </si>
+  <si>
+    <t>Agricultural Greenhouse Gas Emissions in Latin America and the Caribbean Current Situation, Future Trends and One Policy Experiment</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=35584254</t>
+  </si>
+  <si>
+    <t>http://www10.iadb.org/intal/intalcdi/PE/2013/12483.pdf</t>
+  </si>
+  <si>
+    <t>Migration Strategies and Accounting Methods for Greenhouse Gas Emissions from Transportation</t>
+  </si>
+  <si>
+    <t>https://commdev.org/userfiles/IFC_Sustainability_Framework.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/Topics_Ext_Content/IFC_External_Corporate_Site/CB_Home/Measuring+Reporting/</t>
+  </si>
+  <si>
+    <t>IFC Climate Business Measuring and Reporting</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/6923?locale-attribute=en</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/corporate-social-responsibility/corporate-environmental-social-responsibility-csr-program/idbs-greenhouse-gas-emissions,1637.html</t>
+  </si>
+  <si>
+    <t>Our Footprint: IDB's Greenhouse Gas Emissions</t>
+  </si>
+  <si>
+    <t>Inventory Data</t>
+  </si>
+  <si>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=37077851</t>
+  </si>
+  <si>
+    <t>Greenhouse Gas Assessment Emissions Methodology</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=2242924</t>
+  </si>
+  <si>
+    <t>Coal Fired Power Plants Guidelines: An Approach to Reconciling the Financing of Coal-Fired Power Plants with Climate Change Objectives</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=37249415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liquid and Gaseous Fossil Fuel Power Plant Guidelines: An Approach to Reconciling the Financing of Fossil Fuel Power Plants with Climate Change Objectives </t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=37929911</t>
+  </si>
+  <si>
+    <t>Greenhouse Gas Emissions from New Petrochemical Plants: Background Information Paper for the Elaboration of Technical Notes and Guidelines for IDB Projects</t>
+  </si>
+  <si>
+    <t>Environmental Safeguards: Policies and Guidelines</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/topics/sustainability/environmental-safeguards,1517.html</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2576</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2574</t>
+  </si>
+  <si>
+    <t>http://publications.iadb.org/handle/11319/2503</t>
+  </si>
+  <si>
+    <t>http://idbdocs.iadb.org/wsdocs/getdocument.aspx?docnum=36422007</t>
+  </si>
+  <si>
+    <t>Landfill Guidelines: An Approach to Support Climate Change-Friendly Landfill Investments</t>
+  </si>
+  <si>
+    <t>http://saludmesoamerica2015.org/en/publications/publications,4126.html?docType=Policies,%20Strategies%20%26%20Guidelines&amp;docTypeID=PoliciesSG&amp;searchLang=&amp;topic=Electricity%20%3BCITI&amp;country=&amp;keywords=landfill&amp;selectList=All&amp;topicDetail=0&amp;tagDetail=0&amp;dept=&amp;jelcodeDetail=0&amp;publicationCover=0</t>
   </si>
 </sst>
 </file>
@@ -3294,7 +3434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3339,6 +3479,9 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6076,6 +6219,114 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>967</v>
+      </c>
+      <c r="C6" t="s">
+        <v>970</v>
+      </c>
+      <c r="D6" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>968</v>
+      </c>
+      <c r="C7" t="s">
+        <v>972</v>
+      </c>
+      <c r="D7" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>969</v>
+      </c>
+      <c r="C8" t="s">
+        <v>973</v>
+      </c>
+      <c r="D8" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>974</v>
+      </c>
+      <c r="C10" t="s">
+        <v>976</v>
+      </c>
+      <c r="D10" t="s">
+        <v>975</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D39"/>
@@ -8198,12 +8449,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView tabSelected="1" workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8262,6 +8513,9 @@
       <c r="C5" t="s">
         <v>759</v>
       </c>
+      <c r="D5" t="s">
+        <v>1036</v>
+      </c>
       <c r="E5" t="s">
         <v>756</v>
       </c>
@@ -8270,6 +8524,9 @@
       <c r="C6" t="s">
         <v>758</v>
       </c>
+      <c r="D6" t="s">
+        <v>1037</v>
+      </c>
       <c r="E6" t="s">
         <v>757</v>
       </c>
@@ -8394,8 +8651,12 @@
       <c r="C22" t="s">
         <v>764</v>
       </c>
+      <c r="D22" t="s">
+        <v>1039</v>
+      </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
         <v>784</v>
       </c>
     </row>
@@ -8406,7 +8667,13 @@
       <c r="C23" t="s">
         <v>783</v>
       </c>
+      <c r="D23" t="s">
+        <v>1038</v>
+      </c>
       <c r="F23" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G23" t="s">
         <v>785</v>
       </c>
       <c r="K23">
@@ -8442,668 +8709,646 @@
       <c r="C28" t="s">
         <v>788</v>
       </c>
+      <c r="D28" t="s">
+        <v>1040</v>
+      </c>
       <c r="E28" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="C29" s="14" t="s">
+        <v>788</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>789</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>790</v>
       </c>
-      <c r="K29">
+      <c r="K30">
         <v>2013</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="C31" s="14" t="s">
+        <v>789</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>761</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>760</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F34" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="30" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="D35" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="F36" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="2:10" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="14" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="28" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="28" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="30" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="30" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="F48" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+      <c r="F49" s="30" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="G50" s="11" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="F51" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>798</v>
       </c>
-      <c r="B46">
+      <c r="B57">
         <v>101</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C57" t="s">
         <v>989</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E57" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>798</v>
       </c>
-      <c r="B47">
+      <c r="B58">
         <v>102</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C58" t="s">
         <v>990</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E58" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>983</v>
       </c>
-      <c r="B49">
+      <c r="B60">
         <v>201</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C60" t="s">
         <v>991</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E60" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>983</v>
       </c>
-      <c r="B50">
+      <c r="B61">
         <v>202</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C61" t="s">
         <v>992</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E61" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>984</v>
       </c>
-      <c r="B52">
+      <c r="B63">
         <v>301</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C63" t="s">
         <v>993</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E63" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>984</v>
       </c>
-      <c r="B53">
+      <c r="B64">
         <v>302</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C64" t="s">
         <v>994</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E64" t="s">
         <v>809</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>984</v>
-      </c>
-      <c r="B54">
-        <v>303</v>
-      </c>
-      <c r="C54" t="s">
-        <v>995</v>
-      </c>
-      <c r="E54" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>984</v>
-      </c>
-      <c r="B55">
-        <v>304</v>
-      </c>
-      <c r="C55" t="s">
-        <v>996</v>
-      </c>
-      <c r="E55" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>984</v>
-      </c>
-      <c r="B56">
-        <v>305</v>
-      </c>
-      <c r="C56" t="s">
-        <v>997</v>
-      </c>
-      <c r="E56" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>984</v>
-      </c>
-      <c r="B57">
-        <v>306</v>
-      </c>
-      <c r="C57" t="s">
-        <v>998</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>984</v>
-      </c>
-      <c r="B58">
-        <v>307</v>
-      </c>
-      <c r="C58" t="s">
-        <v>999</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>984</v>
-      </c>
-      <c r="B59">
-        <v>308</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>984</v>
-      </c>
-      <c r="B60">
-        <v>309</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>984</v>
-      </c>
-      <c r="B61">
-        <v>310</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>984</v>
-      </c>
-      <c r="B62">
-        <v>311</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>985</v>
-      </c>
-      <c r="B64">
-        <v>400</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1004</v>
-      </c>
-      <c r="E64" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B65">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="C65" t="s">
-        <v>1005</v>
+        <v>995</v>
       </c>
       <c r="E65" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B66">
-        <v>402</v>
+        <v>304</v>
       </c>
       <c r="C66" t="s">
-        <v>1006</v>
+        <v>996</v>
       </c>
       <c r="E66" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>984</v>
+      </c>
+      <c r="B67">
+        <v>305</v>
+      </c>
       <c r="C67" t="s">
-        <v>802</v>
+        <v>997</v>
+      </c>
+      <c r="E67" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>987</v>
-      </c>
-      <c r="B68" s="8"/>
+        <v>984</v>
+      </c>
+      <c r="B68">
+        <v>306</v>
+      </c>
       <c r="C68" t="s">
-        <v>803</v>
-      </c>
-      <c r="E68" t="s">
-        <v>822</v>
+        <v>998</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>984</v>
+      </c>
+      <c r="B69">
+        <v>307</v>
+      </c>
       <c r="C69" t="s">
-        <v>804</v>
+        <v>999</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="B70">
-        <v>601</v>
+        <v>308</v>
       </c>
       <c r="C70" t="s">
-        <v>1007</v>
-      </c>
-      <c r="E70" t="s">
-        <v>823</v>
+        <v>1000</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="B71">
-        <v>602</v>
+        <v>309</v>
       </c>
       <c r="C71" t="s">
-        <v>1008</v>
-      </c>
-      <c r="E71" t="s">
-        <v>824</v>
+        <v>1001</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>988</v>
+        <v>984</v>
+      </c>
+      <c r="B72">
+        <v>310</v>
       </c>
       <c r="C72" t="s">
-        <v>825</v>
+        <v>1002</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="B73">
-        <v>703</v>
+        <v>311</v>
       </c>
       <c r="C73" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E73" t="s">
-        <v>754</v>
+        <v>1003</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>988</v>
-      </c>
-      <c r="B74">
-        <v>704</v>
-      </c>
       <c r="C74" t="s">
-        <v>1029</v>
-      </c>
-      <c r="E74" t="s">
-        <v>829</v>
+        <v>801</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B75">
-        <v>707</v>
+        <v>400</v>
       </c>
       <c r="C75" t="s">
-        <v>1028</v>
+        <v>1004</v>
       </c>
       <c r="E75" t="s">
-        <v>830</v>
+        <v>819</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B76">
-        <v>708</v>
+        <v>401</v>
       </c>
       <c r="C76" t="s">
-        <v>1027</v>
+        <v>1005</v>
       </c>
       <c r="E76" t="s">
-        <v>831</v>
+        <v>820</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B77">
-        <v>710</v>
+        <v>402</v>
       </c>
       <c r="C77" t="s">
-        <v>161</v>
+        <v>1006</v>
       </c>
       <c r="E77" t="s">
-        <v>832</v>
+        <v>821</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>987</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" t="s">
+        <v>803</v>
+      </c>
+      <c r="E79" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>988</v>
+      </c>
+      <c r="B81">
+        <v>601</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E81" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>988</v>
+      </c>
+      <c r="B82">
+        <v>602</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E82" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>988</v>
+      </c>
+      <c r="C83" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>988</v>
+      </c>
+      <c r="B84">
+        <v>703</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E84" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>988</v>
+      </c>
+      <c r="B85">
+        <v>704</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E85" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>988</v>
+      </c>
+      <c r="B86">
+        <v>707</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E86" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>988</v>
+      </c>
+      <c r="B87">
+        <v>708</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E87" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>988</v>
+      </c>
+      <c r="B88">
+        <v>710</v>
+      </c>
+      <c r="C88" t="s">
+        <v>161</v>
+      </c>
+      <c r="E88" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>826</v>
       </c>
-      <c r="B79">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>826</v>
+      </c>
+      <c r="B90">
         <v>733</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C90" t="s">
         <v>1025</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E90" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>826</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>982</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C91" t="s">
         <v>1026</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E91" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>827</v>
       </c>
-      <c r="B82">
+      <c r="B93">
         <v>761</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C93" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>827</v>
       </c>
-      <c r="B83">
+      <c r="B94">
         <v>765</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C94" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>828</v>
-      </c>
-      <c r="B85">
-        <v>2001</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>828</v>
-      </c>
-      <c r="B86">
-        <v>2002</v>
-      </c>
-      <c r="C86" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>828</v>
-      </c>
-      <c r="B87">
-        <v>2003</v>
-      </c>
-      <c r="C87" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>828</v>
-      </c>
-      <c r="B88">
-        <v>2004</v>
-      </c>
-      <c r="C88" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>828</v>
-      </c>
-      <c r="B89">
-        <v>2005</v>
-      </c>
-      <c r="C89" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>828</v>
-      </c>
-      <c r="B90">
-        <v>2006</v>
-      </c>
-      <c r="C90" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>828</v>
-      </c>
-      <c r="B91">
-        <v>2007</v>
-      </c>
-      <c r="C91" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>828</v>
-      </c>
-      <c r="B92">
-        <v>2008</v>
-      </c>
-      <c r="C92" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>828</v>
-      </c>
-      <c r="B93">
-        <v>2009</v>
-      </c>
-      <c r="C93" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>828</v>
-      </c>
-      <c r="B94">
-        <v>2010</v>
-      </c>
-      <c r="C94" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>828</v>
-      </c>
-      <c r="B95">
-        <v>2011</v>
-      </c>
-      <c r="C95" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>828</v>
       </c>
       <c r="B96">
-        <v>2012</v>
+        <v>2001</v>
       </c>
       <c r="C96" t="s">
-        <v>1012</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -9111,10 +9356,10 @@
         <v>828</v>
       </c>
       <c r="B97">
-        <v>2013</v>
+        <v>2002</v>
       </c>
       <c r="C97" t="s">
-        <v>1011</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -9122,9 +9367,130 @@
         <v>828</v>
       </c>
       <c r="B98">
+        <v>2003</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>828</v>
+      </c>
+      <c r="B99">
+        <v>2004</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>828</v>
+      </c>
+      <c r="B100">
+        <v>2005</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>828</v>
+      </c>
+      <c r="B101">
+        <v>2006</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>828</v>
+      </c>
+      <c r="B102">
+        <v>2007</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>828</v>
+      </c>
+      <c r="B103">
+        <v>2008</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>828</v>
+      </c>
+      <c r="B104">
+        <v>2009</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>828</v>
+      </c>
+      <c r="B105">
+        <v>2010</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>828</v>
+      </c>
+      <c r="B106">
+        <v>2011</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>828</v>
+      </c>
+      <c r="B107">
+        <v>2012</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>828</v>
+      </c>
+      <c r="B108">
+        <v>2013</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>828</v>
+      </c>
+      <c r="B109">
         <v>2014</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C109" t="s">
         <v>1010</v>
       </c>
     </row>
@@ -9136,12 +9502,134 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O65"/>
+  <dimension ref="C2:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="30" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView zoomScaleNormal="100" workbookViewId="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9201,14 +9689,11 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>743</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>664</v>
-      </c>
-      <c r="E4" t="s">
-        <v>666</v>
+      <c r="C4" s="8" t="s">
+        <v>654</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -9216,69 +9701,63 @@
         <v>743</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E5" t="s">
-        <v>667</v>
-      </c>
-      <c r="I5" t="s">
-        <v>681</v>
-      </c>
-      <c r="J5" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>743</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="24" t="s">
+        <v>665</v>
+      </c>
+      <c r="E6" t="s">
+        <v>667</v>
+      </c>
+      <c r="I6" t="s">
+        <v>681</v>
+      </c>
+      <c r="J6" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>743</v>
+      </c>
+      <c r="C7" t="s">
         <v>658</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>659</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>661</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>743</v>
-      </c>
-      <c r="C8" t="s">
-        <v>656</v>
-      </c>
-      <c r="E8" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>743</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>669</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>672</v>
-      </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="C9" t="s">
+        <v>656</v>
+      </c>
+      <c r="E9" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>743</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>675</v>
-      </c>
-      <c r="D10" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -9289,35 +9768,38 @@
         <v>743</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D11" t="s">
-        <v>678</v>
-      </c>
+        <v>677</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>677</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>743</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="D12" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>743</v>
+      </c>
+      <c r="C13" t="s">
         <v>652</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>743</v>
-      </c>
-      <c r="C14" t="s">
-        <v>670</v>
-      </c>
-      <c r="D14" t="s">
-        <v>657</v>
-      </c>
-      <c r="E14" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -9325,10 +9807,13 @@
         <v>743</v>
       </c>
       <c r="C15" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D15" t="s">
-        <v>674</v>
+        <v>657</v>
+      </c>
+      <c r="E15" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -9336,21 +9821,21 @@
         <v>743</v>
       </c>
       <c r="C16" t="s">
+        <v>671</v>
+      </c>
+      <c r="D16" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>668</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>743</v>
-      </c>
-      <c r="C18" t="s">
-        <v>663</v>
-      </c>
-      <c r="D18" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -9358,30 +9843,30 @@
         <v>743</v>
       </c>
       <c r="C19" t="s">
+        <v>663</v>
+      </c>
+      <c r="D19" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>743</v>
+      </c>
+      <c r="C20" t="s">
         <v>752</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="21" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>741</v>
-      </c>
-      <c r="C24" t="s">
-        <v>647</v>
-      </c>
-    </row>
+    <row r="22" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>741</v>
       </c>
       <c r="C25" t="s">
-        <v>648</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>685</v>
+        <v>647</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -9389,7 +9874,10 @@
         <v>741</v>
       </c>
       <c r="C26" t="s">
-        <v>649</v>
+        <v>648</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -9397,7 +9885,7 @@
         <v>741</v>
       </c>
       <c r="C27" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -9405,85 +9893,82 @@
         <v>741</v>
       </c>
       <c r="C28" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="C29" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
         <v>741</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>742</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D31" s="23" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="32" spans="2:4" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>745</v>
-      </c>
-      <c r="C34" t="s">
-        <v>740</v>
-      </c>
-      <c r="F34" t="s">
-        <v>687</v>
-      </c>
-    </row>
+    <row r="33" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>745</v>
       </c>
       <c r="C35" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F35" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>745</v>
+      </c>
+      <c r="C36" t="s">
+        <v>739</v>
+      </c>
+      <c r="F36" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>986</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>738</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>746</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>746</v>
-      </c>
-      <c r="C40" t="s">
-        <v>737</v>
-      </c>
-      <c r="E40" t="s">
-        <v>691</v>
-      </c>
-      <c r="F40" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>746</v>
       </c>
       <c r="C41" t="s">
-        <v>736</v>
+        <v>737</v>
+      </c>
+      <c r="E41" t="s">
+        <v>691</v>
       </c>
       <c r="F41" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -9491,10 +9976,10 @@
         <v>746</v>
       </c>
       <c r="C42" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F42" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -9502,10 +9987,10 @@
         <v>746</v>
       </c>
       <c r="C43" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="F43" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -9513,10 +9998,10 @@
         <v>746</v>
       </c>
       <c r="C44" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="F44" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -9524,10 +10009,10 @@
         <v>746</v>
       </c>
       <c r="C45" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F45" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -9535,10 +10020,10 @@
         <v>746</v>
       </c>
       <c r="C46" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F46" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -9546,46 +10031,46 @@
         <v>746</v>
       </c>
       <c r="C47" t="s">
+        <v>731</v>
+      </c>
+      <c r="F47" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>746</v>
+      </c>
+      <c r="C48" t="s">
         <v>730</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>746</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>729</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>699</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>699</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>744</v>
-      </c>
-      <c r="C51" t="s">
-        <v>717</v>
-      </c>
-      <c r="F51" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C52" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F52" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -9593,43 +10078,43 @@
         <v>745</v>
       </c>
       <c r="C53" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F53" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="C54" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="F54" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C55" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="F55" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C56" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="F56" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -9637,63 +10122,63 @@
         <v>748</v>
       </c>
       <c r="C57" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="F57" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>748</v>
+      </c>
+      <c r="C58" t="s">
+        <v>711</v>
+      </c>
+      <c r="F58" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>750</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>710</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>707</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I59" t="s">
         <v>708</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J59" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>749</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>719</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>750</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>728</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>727</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G63" t="s">
         <v>726</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>751</v>
-      </c>
-      <c r="C64" t="s">
-        <v>721</v>
-      </c>
-      <c r="E64" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
@@ -9701,9 +10186,20 @@
         <v>751</v>
       </c>
       <c r="C65" t="s">
+        <v>721</v>
+      </c>
+      <c r="E65" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>751</v>
+      </c>
+      <c r="C66" t="s">
         <v>722</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>723</v>
       </c>
     </row>
@@ -9713,14 +10209,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B8" sqref="B7:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="28" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N116"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10657,112 +11221,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>236</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>967</v>
-      </c>
-      <c r="C6" t="s">
-        <v>970</v>
-      </c>
-      <c r="D6" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>968</v>
-      </c>
-      <c r="C7" t="s">
-        <v>972</v>
-      </c>
-      <c r="D7" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>969</v>
-      </c>
-      <c r="C8" t="s">
-        <v>973</v>
-      </c>
-      <c r="D8" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>974</v>
-      </c>
-      <c r="C10" t="s">
-        <v>976</v>
-      </c>
-      <c r="D10" t="s">
-        <v>975</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding country strategy URLs for EBRD
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1179">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -3460,6 +3460,108 @@
   </si>
   <si>
     <t>http://www.ebrd.com/downloads/policies/sector/property.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/what-we-do/strategies-and-policies.html#collapseOne1395238894262</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/albania.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/armenia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/azerbaijan-country-strategy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/belarus.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/bosnia2014.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/documents/strategy-and-policy-coordination/strategy-for-bulgaria.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/croatia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395243085650&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/estonia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/georgia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/hungary.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395238389551&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/kazakhstan-strategy-2013.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/kosovo-strategy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241627745&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/latvia_strategy_2_111207.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/lithuania.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/macedonia-strategy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/moldova.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/mongolia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/montenegro.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395243032404&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/poland.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/romania.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/russia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/serbia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/slovak.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/slovenia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/tajikistan.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/turkey.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/turkmenistan.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/ukraine_country_strategy_2011_2014.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/country/strategy/uzbekistan.pdf</t>
   </si>
 </sst>
 </file>
@@ -11318,8 +11420,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="1">
-      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C88" sqref="A88:XFD88"/>
+      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12208,172 +12310,271 @@
         <v>852</v>
       </c>
       <c r="E91" t="s">
-        <v>916</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="92" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>883</v>
       </c>
+      <c r="D92" t="s">
+        <v>1146</v>
+      </c>
     </row>
     <row r="93" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>884</v>
       </c>
+      <c r="D93" t="s">
+        <v>1147</v>
+      </c>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>885</v>
       </c>
+      <c r="D94" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="95" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>886</v>
       </c>
+      <c r="D95" t="s">
+        <v>1149</v>
+      </c>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
         <v>887</v>
       </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>888</v>
       </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="7" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>890</v>
       </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
         <v>891</v>
       </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
         <v>900</v>
       </c>
-    </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
         <v>901</v>
       </c>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
         <v>903</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1166</v>
       </c>
     </row>
     <row r="113" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
         <v>904</v>
       </c>
+      <c r="D113" t="s">
+        <v>1167</v>
+      </c>
     </row>
     <row r="114" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
         <v>905</v>
       </c>
+      <c r="D114" t="s">
+        <v>1168</v>
+      </c>
     </row>
     <row r="115" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
         <v>906</v>
       </c>
+      <c r="D115" t="s">
+        <v>1169</v>
+      </c>
     </row>
     <row r="116" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
         <v>907</v>
       </c>
+      <c r="D116" t="s">
+        <v>1170</v>
+      </c>
     </row>
     <row r="117" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
         <v>908</v>
       </c>
+      <c r="D117" t="s">
+        <v>1171</v>
+      </c>
     </row>
     <row r="118" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
         <v>909</v>
       </c>
+      <c r="D118" t="s">
+        <v>1172</v>
+      </c>
     </row>
     <row r="119" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
         <v>910</v>
       </c>
+      <c r="D119" t="s">
+        <v>1173</v>
+      </c>
     </row>
     <row r="120" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
         <v>911</v>
       </c>
+      <c r="D120" t="s">
+        <v>1174</v>
+      </c>
     </row>
     <row r="121" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
         <v>912</v>
       </c>
+      <c r="D121" t="s">
+        <v>1175</v>
+      </c>
     </row>
     <row r="122" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
         <v>913</v>
       </c>
+      <c r="D122" t="s">
+        <v>1176</v>
+      </c>
     </row>
     <row r="123" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
         <v>914</v>
       </c>
+      <c r="D123" t="s">
+        <v>1177</v>
+      </c>
     </row>
     <row r="124" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
         <v>915</v>
+      </c>
+      <c r="D124" t="s">
+        <v>1178</v>
       </c>
     </row>
     <row r="125" spans="3:14" s="16" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished adding most links; time to organize
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="12630" windowHeight="5100"/>
-    <workbookView xWindow="-510" yWindow="75" windowWidth="14325" windowHeight="5070" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="9615" windowHeight="5100"/>
+    <workbookView xWindow="-510" yWindow="75" windowWidth="10245" windowHeight="5070" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="IFC" sheetId="3" r:id="rId7"/>
     <sheet name="IFC_resources" sheetId="10" r:id="rId8"/>
     <sheet name="EBRD" sheetId="7" r:id="rId9"/>
-    <sheet name="OPIC" sheetId="8" r:id="rId10"/>
+    <sheet name="EBRD_resources" sheetId="11" r:id="rId10"/>
+    <sheet name="OPIC" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="1215">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -3562,6 +3563,114 @@
   </si>
   <si>
     <t>http://www.ebrd.com/downloads/country/strategy/uzbekistan.pdf</t>
+  </si>
+  <si>
+    <t>Environmental and Social Advisory Council</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/who-we-are/our-values/environmental-and-social-advisory-council.html%20</t>
+  </si>
+  <si>
+    <t>Performance Requirements and Guidance</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/who-we-are/our-values/environmental-and-social-policy/performance-requirements.html%20</t>
+  </si>
+  <si>
+    <t>PR 1: Assessment and Management of Environmental and Social Impacts and Issues</t>
+  </si>
+  <si>
+    <t>PR 2: Labour and Working Conditions</t>
+  </si>
+  <si>
+    <t>PR 3: Resource Efficiency and Pollution Prevention and Control</t>
+  </si>
+  <si>
+    <t>PR 4: Health and Safety</t>
+  </si>
+  <si>
+    <t>PR 5: Land Acquisition, Involuntary Resettlement and Economic Displacement</t>
+  </si>
+  <si>
+    <t>PR 6: Biodiversity Conservation and Sustainable Management of Living Natural Resources</t>
+  </si>
+  <si>
+    <t>PR 7: Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>PR 8: Cultural Heritage</t>
+  </si>
+  <si>
+    <t>PR 9: Financial Intermediaries</t>
+  </si>
+  <si>
+    <t>PR 10: Information Disclosure and Stakeholder Engagement</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241534189&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241534659&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241534732&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241534816&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241535028&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241535083&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241535137&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241535196&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241535263&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241535351&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395238867768&amp;pagename=EBRD%2FContent%2FDownloadDocument</t>
+  </si>
+  <si>
+    <t>How to implement our performance requirements</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/who-we-are/our-values/environmental-and-social-policy/implementation.html%20</t>
+  </si>
+  <si>
+    <t>Implementation tools for financial intermediaries</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/who-we-are/our-values/environmental-and-social-policy/tools-for-financial-intermediaries.html%20</t>
+  </si>
+  <si>
+    <t>Environmental and Social Sustainability overview</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/who-we-are/our-values/environmental-and-social-sustainability.html</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/ethnic.pdf</t>
+  </si>
+  <si>
+    <t>Political aspects of the mandate of the European Bank in relation to ethnic minorities</t>
+  </si>
+  <si>
+    <t>Project Complaint Mechanism (PCM) user guide</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/documents/comms-and-bis/pdf-pcm-user-guide.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/publications/guides/pcm-user-guide.html</t>
   </si>
 </sst>
 </file>
@@ -3569,7 +3678,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -3734,7 +3843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3782,8 +3891,9 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6523,6 +6633,123 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="44" t="s">
+        <v>673</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>674</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="N3" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10579,7 +10806,9 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10713,7 +10942,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="42" t="s">
         <v>1054</v>
       </c>
@@ -11416,12 +11645,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O126"/>
+  <dimension ref="C2:O137"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="1">
-      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11688,6 +11917,9 @@
       <c r="C30" s="28" t="s">
         <v>829</v>
       </c>
+      <c r="D30" t="s">
+        <v>1203</v>
+      </c>
       <c r="E30" t="s">
         <v>833</v>
       </c>
@@ -11843,767 +12075,871 @@
       <c r="M41" s="40"/>
       <c r="N41" s="39"/>
     </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="42" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>1193</v>
+      </c>
+      <c r="M42" s="45"/>
+    </row>
+    <row r="43" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>1194</v>
+      </c>
+      <c r="M43" s="45"/>
+    </row>
+    <row r="44" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="18" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>1195</v>
+      </c>
+      <c r="M44" s="45"/>
+    </row>
+    <row r="45" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>1196</v>
+      </c>
+      <c r="M45" s="45"/>
+    </row>
+    <row r="46" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="18" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>1197</v>
+      </c>
+      <c r="M46" s="45"/>
+    </row>
+    <row r="47" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>1198</v>
+      </c>
+      <c r="M47" s="45"/>
+    </row>
+    <row r="48" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="18" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>1199</v>
+      </c>
+      <c r="M48" s="45"/>
+    </row>
+    <row r="49" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>1200</v>
+      </c>
+      <c r="M49" s="45"/>
+    </row>
+    <row r="50" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="18" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>1201</v>
+      </c>
+      <c r="M50" s="45"/>
+    </row>
+    <row r="51" spans="3:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="18" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>1202</v>
+      </c>
+      <c r="M51" s="45"/>
+    </row>
+    <row r="52" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="40"/>
+      <c r="N52" s="39"/>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>864</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D54" t="s">
         <v>927</v>
-      </c>
-    </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C44" s="14" t="s">
-        <v>970</v>
-      </c>
-      <c r="D44" t="s">
-        <v>969</v>
-      </c>
-      <c r="E44" t="s">
-        <v>968</v>
-      </c>
-      <c r="K44">
-        <v>2010</v>
-      </c>
-      <c r="L44" t="s">
-        <v>205</v>
-      </c>
-      <c r="M44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>847</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C46" s="14" t="s">
-        <v>847</v>
-      </c>
-      <c r="D46" t="s">
-        <v>850</v>
-      </c>
-      <c r="E46" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>865</v>
-      </c>
-      <c r="D47" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>866</v>
-      </c>
-      <c r="E48" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="49" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>867</v>
-      </c>
-      <c r="E49" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="50" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>868</v>
-      </c>
-      <c r="D50" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="51" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>869</v>
-      </c>
-      <c r="D51" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="52" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="53" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="54" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C54" s="14" t="s">
-        <v>951</v>
-      </c>
-      <c r="D54" t="s">
-        <v>955</v>
-      </c>
-      <c r="E54" t="s">
-        <v>957</v>
-      </c>
-      <c r="G54" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="55" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C55" s="14" t="s">
-        <v>952</v>
+        <v>970</v>
       </c>
       <c r="D55" t="s">
-        <v>956</v>
-      </c>
-      <c r="G55" t="s">
-        <v>919</v>
+        <v>969</v>
+      </c>
+      <c r="E55" t="s">
+        <v>968</v>
+      </c>
+      <c r="K55">
+        <v>2010</v>
+      </c>
+      <c r="L55" t="s">
+        <v>205</v>
+      </c>
+      <c r="M55">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>842</v>
+        <v>847</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>928</v>
       </c>
     </row>
     <row r="57" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-    </row>
-    <row r="58" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="40"/>
-      <c r="N58" s="39"/>
+      <c r="C57" s="14" t="s">
+        <v>847</v>
+      </c>
+      <c r="D57" t="s">
+        <v>850</v>
+      </c>
+      <c r="E57" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>865</v>
+      </c>
+      <c r="D58" t="s">
+        <v>930</v>
+      </c>
     </row>
     <row r="59" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>842</v>
-      </c>
-      <c r="D59" t="s">
-        <v>843</v>
+        <v>866</v>
       </c>
       <c r="E59" t="s">
-        <v>848</v>
-      </c>
-      <c r="K59">
-        <v>2014</v>
-      </c>
-      <c r="L59" t="s">
-        <v>210</v>
+        <v>919</v>
       </c>
     </row>
     <row r="60" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>844</v>
-      </c>
-      <c r="F60" t="s">
-        <v>846</v>
+        <v>867</v>
+      </c>
+      <c r="E60" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="61" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
+        <v>868</v>
+      </c>
+      <c r="D61" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>869</v>
+      </c>
+      <c r="D62" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="64" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C65" s="14" t="s">
+        <v>951</v>
+      </c>
+      <c r="D65" t="s">
+        <v>955</v>
+      </c>
+      <c r="E65" t="s">
+        <v>957</v>
+      </c>
+      <c r="G65" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="66" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C66" s="14" t="s">
+        <v>952</v>
+      </c>
+      <c r="D66" t="s">
+        <v>956</v>
+      </c>
+      <c r="G66" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="67" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+    </row>
+    <row r="69" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="39"/>
+      <c r="J69" s="39"/>
+      <c r="K69" s="39"/>
+      <c r="L69" s="39"/>
+      <c r="M69" s="40"/>
+      <c r="N69" s="39"/>
+    </row>
+    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>842</v>
+      </c>
+      <c r="D70" t="s">
+        <v>843</v>
+      </c>
+      <c r="E70" t="s">
+        <v>848</v>
+      </c>
+      <c r="K70">
+        <v>2014</v>
+      </c>
+      <c r="L70" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>844</v>
+      </c>
+      <c r="F71" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C62" s="14" t="s">
+    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C73" s="14" t="s">
         <v>950</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D73" t="s">
         <v>954</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E73" t="s">
         <v>848</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G73" t="s">
         <v>919</v>
       </c>
-      <c r="K62">
+      <c r="K73">
         <v>2014</v>
       </c>
     </row>
-    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C63" s="14" t="s">
+    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C74" s="14" t="s">
         <v>844</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D74" t="s">
         <v>846</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E74" t="s">
         <v>848</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G74" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="64" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
-      <c r="M64" s="40"/>
-      <c r="N64" s="39"/>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+    <row r="75" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="39"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="39"/>
+      <c r="L75" s="39"/>
+      <c r="M75" s="40"/>
+      <c r="N75" s="39"/>
+    </row>
+    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+    </row>
+    <row r="77" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C69" s="5" t="s">
+    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C80" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E80" t="s">
         <v>916</v>
-      </c>
-    </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>873</v>
-      </c>
-      <c r="D70" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C71" s="23" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D71" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C72" s="23" t="s">
-        <v>1112</v>
-      </c>
-      <c r="F72" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C73" s="23" t="s">
-        <v>1113</v>
-      </c>
-      <c r="E73" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>874</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>1127</v>
-      </c>
-      <c r="E74" t="s">
-        <v>1126</v>
-      </c>
-      <c r="F74" s="16"/>
-      <c r="G74" t="s">
-        <v>1131</v>
-      </c>
-      <c r="I74" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C75" s="23" t="s">
-        <v>1116</v>
-      </c>
-      <c r="F75" t="s">
-        <v>1128</v>
-      </c>
-      <c r="G75" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C76" s="23" t="s">
-        <v>1129</v>
-      </c>
-      <c r="D76" s="30" t="s">
-        <v>1130</v>
-      </c>
-      <c r="F76" s="16"/>
-    </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>875</v>
-      </c>
-      <c r="D77" t="s">
-        <v>1133</v>
-      </c>
-      <c r="E77" t="s">
-        <v>1114</v>
-      </c>
-      <c r="G77" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C78" s="23" t="s">
-        <v>1112</v>
-      </c>
-      <c r="F78" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>876</v>
-      </c>
-      <c r="E79" t="s">
-        <v>1134</v>
-      </c>
-      <c r="G79" t="s">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C80" s="23" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="D81" t="s">
-        <v>1137</v>
-      </c>
-      <c r="G81" t="s">
-        <v>1131</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="82" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C82" s="23" t="s">
-        <v>844</v>
+        <v>1111</v>
       </c>
       <c r="D82" t="s">
-        <v>1136</v>
-      </c>
-      <c r="G82" t="s">
-        <v>1131</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="83" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>878</v>
-      </c>
-      <c r="D83" t="s">
-        <v>1138</v>
-      </c>
-      <c r="I83" t="s">
-        <v>1140</v>
+      <c r="C83" s="23" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1124</v>
       </c>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C84" s="23" t="s">
-        <v>1117</v>
-      </c>
-      <c r="F84" t="s">
-        <v>1141</v>
+        <v>1113</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1125</v>
       </c>
     </row>
     <row r="85" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>879</v>
-      </c>
-      <c r="D85" t="s">
-        <v>1142</v>
-      </c>
+        <v>874</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F85" s="16"/>
       <c r="G85" t="s">
         <v>1131</v>
       </c>
+      <c r="I85" t="s">
+        <v>1139</v>
+      </c>
     </row>
     <row r="86" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C86" s="23" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F86" t="s">
-        <v>1143</v>
+        <v>1128</v>
+      </c>
+      <c r="G86" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="87" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
-        <v>880</v>
-      </c>
-      <c r="D87" t="s">
-        <v>1144</v>
-      </c>
+      <c r="C87" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F87" s="16"/>
     </row>
     <row r="88" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="D88" t="s">
-        <v>1119</v>
+        <v>1133</v>
       </c>
       <c r="E88" t="s">
-        <v>1118</v>
+        <v>1114</v>
+      </c>
+      <c r="G88" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>882</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1120</v>
+      <c r="C89" s="23" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="90" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>876</v>
+      </c>
+      <c r="E90" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G90" t="s">
+        <v>1135</v>
       </c>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C91" s="5" t="s">
-        <v>852</v>
-      </c>
-      <c r="E91" t="s">
-        <v>1145</v>
+      <c r="C91" s="23" t="s">
+        <v>1115</v>
       </c>
     </row>
     <row r="92" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D92" t="s">
-        <v>1146</v>
+        <v>1137</v>
+      </c>
+      <c r="G92" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="93" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
-        <v>884</v>
+      <c r="C93" s="23" t="s">
+        <v>844</v>
       </c>
       <c r="D93" t="s">
-        <v>1147</v>
+        <v>1136</v>
+      </c>
+      <c r="G93" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="D94" t="s">
-        <v>1148</v>
+        <v>1138</v>
+      </c>
+      <c r="I94" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="95" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>886</v>
-      </c>
-      <c r="D95" t="s">
-        <v>1149</v>
+      <c r="C95" s="23" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1141</v>
       </c>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
+        <v>879</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G96" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C97" s="23" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>880</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>881</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E99" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>882</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C102" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="E102" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>883</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>884</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>885</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>886</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
         <v>887</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D107" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
         <v>888</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D108" t="s">
         <v>1151</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
         <v>889</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D109" s="7" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
         <v>890</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D110" t="s">
         <v>1153</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
         <v>891</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D111" t="s">
         <v>1154</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
         <v>892</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D112" t="s">
         <v>1155</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
         <v>893</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D113" t="s">
         <v>1156</v>
       </c>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
         <v>894</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D114" t="s">
         <v>1157</v>
       </c>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
         <v>895</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D115" t="s">
         <v>1158</v>
       </c>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C105" t="s">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
         <v>896</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D116" t="s">
         <v>1159</v>
       </c>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C106" t="s">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
         <v>897</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D117" t="s">
         <v>1160</v>
       </c>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
         <v>898</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D118" t="s">
         <v>1161</v>
       </c>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C108" t="s">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
         <v>899</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D119" t="s">
         <v>1162</v>
       </c>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
         <v>900</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D120" t="s">
         <v>1163</v>
       </c>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
         <v>901</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D121" t="s">
         <v>1164</v>
       </c>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
         <v>902</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D122" t="s">
         <v>1165</v>
       </c>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
         <v>903</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D123" t="s">
         <v>1166</v>
       </c>
     </row>
-    <row r="113" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
         <v>904</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D124" t="s">
         <v>1167</v>
       </c>
     </row>
-    <row r="114" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C114" t="s">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
         <v>905</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D125" t="s">
         <v>1168</v>
       </c>
     </row>
-    <row r="115" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C115" t="s">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
         <v>906</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D126" t="s">
         <v>1169</v>
       </c>
     </row>
-    <row r="116" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
         <v>907</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D127" t="s">
         <v>1170</v>
       </c>
     </row>
-    <row r="117" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
         <v>908</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D128" t="s">
         <v>1171</v>
       </c>
     </row>
-    <row r="118" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
+    <row r="129" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
         <v>909</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D129" t="s">
         <v>1172</v>
       </c>
     </row>
-    <row r="119" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C119" t="s">
+    <row r="130" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
         <v>910</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D130" t="s">
         <v>1173</v>
       </c>
     </row>
-    <row r="120" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
+    <row r="131" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
         <v>911</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D131" t="s">
         <v>1174</v>
       </c>
     </row>
-    <row r="121" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
+    <row r="132" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
         <v>912</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D132" t="s">
         <v>1175</v>
       </c>
     </row>
-    <row r="122" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
+    <row r="133" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
         <v>913</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D133" t="s">
         <v>1176</v>
       </c>
     </row>
-    <row r="123" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
+    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
         <v>914</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D134" t="s">
         <v>1177</v>
       </c>
     </row>
-    <row r="124" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
+    <row r="135" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
         <v>915</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D135" t="s">
         <v>1178</v>
       </c>
     </row>
-    <row r="125" spans="3:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C125" s="37"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="37"/>
-      <c r="H125" s="37"/>
-      <c r="I125" s="37"/>
-      <c r="J125" s="37"/>
-      <c r="K125" s="37"/>
-      <c r="L125" s="37"/>
-      <c r="M125" s="38"/>
-      <c r="N125" s="37"/>
-    </row>
-    <row r="126" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C126" s="39"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="39"/>
-      <c r="F126" s="39"/>
-      <c r="G126" s="39"/>
-      <c r="H126" s="39"/>
-      <c r="I126" s="39"/>
-      <c r="J126" s="39"/>
-      <c r="K126" s="39"/>
-      <c r="L126" s="39"/>
-      <c r="M126" s="40"/>
-      <c r="N126" s="39"/>
+    <row r="136" spans="3:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C136" s="37"/>
+      <c r="D136" s="37"/>
+      <c r="E136" s="37"/>
+      <c r="F136" s="37"/>
+      <c r="G136" s="37"/>
+      <c r="H136" s="37"/>
+      <c r="I136" s="37"/>
+      <c r="J136" s="37"/>
+      <c r="K136" s="37"/>
+      <c r="L136" s="37"/>
+      <c r="M136" s="38"/>
+      <c r="N136" s="37"/>
+    </row>
+    <row r="137" spans="3:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C137" s="39"/>
+      <c r="D137" s="39"/>
+      <c r="E137" s="39"/>
+      <c r="F137" s="39"/>
+      <c r="G137" s="39"/>
+      <c r="H137" s="39"/>
+      <c r="I137" s="39"/>
+      <c r="J137" s="39"/>
+      <c r="K137" s="39"/>
+      <c r="L137" s="39"/>
+      <c r="M137" s="40"/>
+      <c r="N137" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
started working on IDB, IFC and EBRD
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="-345" windowWidth="11805" windowHeight="10155" tabRatio="810" activeTab="6"/>
-    <workbookView xWindow="9915" yWindow="45" windowWidth="10560" windowHeight="9780" activeTab="4"/>
+    <workbookView xWindow="450" yWindow="-345" windowWidth="10635" windowHeight="10155" tabRatio="810" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="10905" yWindow="-30" windowWidth="11070" windowHeight="9780" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5152" uniqueCount="2282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5257" uniqueCount="2284">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -6872,6 +6872,12 @@
   </si>
   <si>
     <t>OP 6.30 &gt; Annex A</t>
+  </si>
+  <si>
+    <t>Operations Policies</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/en/about-us/operations-policies-of-the-inter-american-development-bank,6127.html</t>
   </si>
 </sst>
 </file>
@@ -6921,7 +6927,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7048,6 +7054,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -7062,7 +7074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -7146,6 +7158,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7451,8 +7464,8 @@
   <dimension ref="A2:V141"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="9" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A138" sqref="A138"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -11704,8 +11717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB624"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -27456,14 +27469,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U124"/>
+  <dimension ref="A1:U113"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q45" sqref="Q45"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H105" sqref="E103:H105"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="A125" sqref="A125:XFD183"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27603,6 +27616,9 @@
       <c r="A15" t="s">
         <v>1179</v>
       </c>
+      <c r="B15" t="s">
+        <v>667</v>
+      </c>
       <c r="C15" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27623,6 +27639,9 @@
       <c r="A16" t="s">
         <v>1179</v>
       </c>
+      <c r="B16" t="s">
+        <v>667</v>
+      </c>
       <c r="C16" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27639,134 +27658,100 @@
         <v>640</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
       <c r="H17" t="s">
+        <v>535</v>
+      </c>
+      <c r="I17" t="s">
+        <v>901</v>
+      </c>
+      <c r="J17" t="s">
+        <v>640</v>
+      </c>
+      <c r="P17">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="14" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="14" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="14" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E18" t="s">
-        <v>851</v>
-      </c>
-      <c r="F18">
-        <v>201</v>
-      </c>
-      <c r="H18" t="s">
-        <v>859</v>
-      </c>
-      <c r="J18" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E19" t="s">
-        <v>851</v>
-      </c>
-      <c r="F19">
-        <v>202</v>
-      </c>
-      <c r="H19" t="s">
-        <v>860</v>
-      </c>
-      <c r="J19" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E21" t="s">
-        <v>852</v>
-      </c>
-      <c r="F21">
-        <v>301</v>
-      </c>
-      <c r="H21" t="s">
-        <v>861</v>
-      </c>
-      <c r="J21" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>1179</v>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>667</v>
       </c>
       <c r="C22" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E22" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F22">
-        <v>302</v>
+        <v>201</v>
       </c>
       <c r="H22" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="J22" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>1179</v>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>667</v>
       </c>
       <c r="C23" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F23">
-        <v>303</v>
+        <v>202</v>
       </c>
       <c r="H23" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="J23" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C24" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E24" t="s">
-        <v>852</v>
-      </c>
-      <c r="F24">
-        <v>304</v>
-      </c>
+        <v>676</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
-        <v>864</v>
-      </c>
-      <c r="J24" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1179</v>
       </c>
+      <c r="B25" t="s">
+        <v>667</v>
+      </c>
       <c r="C25" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27774,19 +27759,22 @@
         <v>852</v>
       </c>
       <c r="F25">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H25" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="J25" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1179</v>
       </c>
+      <c r="B26" t="s">
+        <v>667</v>
+      </c>
       <c r="C26" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27794,19 +27782,22 @@
         <v>852</v>
       </c>
       <c r="F26">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="H26" t="s">
-        <v>866</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+      <c r="J26" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1179</v>
       </c>
+      <c r="B27" t="s">
+        <v>667</v>
+      </c>
       <c r="C27" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27814,19 +27805,22 @@
         <v>852</v>
       </c>
       <c r="F27">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H27" t="s">
-        <v>867</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>863</v>
+      </c>
+      <c r="J27" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1179</v>
       </c>
+      <c r="B28" t="s">
+        <v>667</v>
+      </c>
       <c r="C28" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27834,19 +27828,22 @@
         <v>852</v>
       </c>
       <c r="F28">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H28" t="s">
-        <v>868</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>864</v>
+      </c>
+      <c r="J28" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1179</v>
       </c>
+      <c r="B29" t="s">
+        <v>667</v>
+      </c>
       <c r="C29" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27854,19 +27851,22 @@
         <v>852</v>
       </c>
       <c r="F29">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="H29" t="s">
-        <v>869</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>865</v>
+      </c>
+      <c r="J29" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1179</v>
       </c>
+      <c r="B30" t="s">
+        <v>667</v>
+      </c>
       <c r="C30" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27874,19 +27874,22 @@
         <v>852</v>
       </c>
       <c r="F30">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="H30" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1179</v>
       </c>
+      <c r="B31" t="s">
+        <v>667</v>
+      </c>
       <c r="C31" s="44" t="s">
         <v>1165</v>
       </c>
@@ -27894,169 +27897,214 @@
         <v>852</v>
       </c>
       <c r="F31">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H31" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B32" t="s">
+        <v>667</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E32" t="s">
+        <v>852</v>
+      </c>
+      <c r="F32">
+        <v>308</v>
+      </c>
       <c r="H32" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>868</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1179</v>
       </c>
+      <c r="B33" t="s">
+        <v>667</v>
+      </c>
       <c r="C33" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E33" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F33">
-        <v>400</v>
+        <v>309</v>
       </c>
       <c r="H33" t="s">
-        <v>872</v>
-      </c>
-      <c r="J33" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+        <v>869</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1179</v>
       </c>
+      <c r="B34" t="s">
+        <v>667</v>
+      </c>
       <c r="C34" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E34" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F34">
-        <v>401</v>
+        <v>310</v>
       </c>
       <c r="H34" t="s">
-        <v>873</v>
-      </c>
-      <c r="J34" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>870</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1179</v>
       </c>
+      <c r="B35" t="s">
+        <v>667</v>
+      </c>
       <c r="C35" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E35" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F35">
-        <v>402</v>
+        <v>311</v>
       </c>
       <c r="H35" t="s">
-        <v>874</v>
-      </c>
-      <c r="J35" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>871</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B37" t="s">
+        <v>667</v>
+      </c>
       <c r="C37" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E37" t="s">
-        <v>855</v>
-      </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
+        <v>853</v>
+      </c>
+      <c r="F37">
+        <v>400</v>
+      </c>
       <c r="H37" t="s">
-        <v>672</v>
+        <v>872</v>
       </c>
       <c r="J37" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B38" t="s">
+        <v>667</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E38" t="s">
+        <v>853</v>
+      </c>
+      <c r="F38">
+        <v>401</v>
+      </c>
       <c r="H38" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>873</v>
+      </c>
+      <c r="J38" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B39" t="s">
+        <v>667</v>
+      </c>
       <c r="C39" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E39" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="F39">
-        <v>601</v>
+        <v>402</v>
       </c>
       <c r="H39" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="J39" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C40" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E40" t="s">
-        <v>856</v>
-      </c>
-      <c r="F40">
-        <v>602</v>
-      </c>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
-        <v>876</v>
-      </c>
-      <c r="J40" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>667</v>
+      </c>
       <c r="C41" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E41" t="s">
-        <v>856</v>
-      </c>
+        <v>855</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
       <c r="H41" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C42" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E42" t="s">
-        <v>856</v>
-      </c>
-      <c r="F42">
-        <v>703</v>
-      </c>
+        <v>672</v>
+      </c>
+      <c r="J41" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
-        <v>877</v>
-      </c>
-      <c r="J42" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>667</v>
+      </c>
       <c r="C43" s="44" t="s">
         <v>1165</v>
       </c>
@@ -28064,16 +28112,19 @@
         <v>856</v>
       </c>
       <c r="F43">
-        <v>704</v>
+        <v>601</v>
       </c>
       <c r="H43" t="s">
-        <v>897</v>
+        <v>875</v>
       </c>
       <c r="J43" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>667</v>
+      </c>
       <c r="C44" s="44" t="s">
         <v>1165</v>
       </c>
@@ -28081,786 +28132,887 @@
         <v>856</v>
       </c>
       <c r="F44">
-        <v>707</v>
+        <v>602</v>
       </c>
       <c r="H44" t="s">
-        <v>896</v>
+        <v>876</v>
       </c>
       <c r="J44" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C45" s="44" t="s">
         <v>1165</v>
       </c>
-      <c r="E45" t="s">
-        <v>856</v>
-      </c>
-      <c r="F45">
-        <v>708</v>
-      </c>
       <c r="H45" t="s">
-        <v>895</v>
-      </c>
-      <c r="J45" t="s">
-        <v>700</v>
-      </c>
-      <c r="P45">
-        <v>2014</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>964</v>
+      </c>
       <c r="C46" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E46" t="s">
-        <v>856</v>
+        <v>694</v>
       </c>
       <c r="F46">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="H46" t="s">
-        <v>157</v>
+        <v>877</v>
       </c>
       <c r="J46" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
       <c r="H47" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C48" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E48" t="s">
-        <v>695</v>
-      </c>
-      <c r="F48">
-        <v>733</v>
-      </c>
+        <v>630</v>
+      </c>
+      <c r="J47" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
       <c r="H48" t="s">
-        <v>893</v>
+        <v>629</v>
       </c>
       <c r="J48" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C49" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E49" t="s">
-        <v>695</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="G49" s="3"/>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
       <c r="H49" t="s">
-        <v>894</v>
-      </c>
-      <c r="J49" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+      <c r="I49" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
       <c r="H50" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>1179</v>
+        <v>629</v>
+      </c>
+      <c r="K50" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>964</v>
       </c>
       <c r="C51" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E51" t="s">
-        <v>696</v>
-      </c>
-      <c r="F51">
-        <v>761</v>
+        <v>694</v>
+      </c>
+      <c r="F51" s="10">
+        <v>704</v>
       </c>
       <c r="H51" t="s">
-        <v>892</v>
-      </c>
-      <c r="I51" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C52" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E52" t="s">
-        <v>696</v>
-      </c>
-      <c r="F52">
-        <v>765</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="J51" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
       <c r="H52" t="s">
-        <v>153</v>
-      </c>
-      <c r="I52" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H54" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C55" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E55" t="s">
-        <v>697</v>
-      </c>
-      <c r="F55">
-        <v>2001</v>
-      </c>
-      <c r="H55" t="s">
-        <v>891</v>
+        <v>628</v>
+      </c>
+      <c r="I52" s="29" t="s">
+        <v>904</v>
+      </c>
+      <c r="J52" s="29" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
+      <c r="H53" t="s">
+        <v>627</v>
+      </c>
+      <c r="I53" t="s">
+        <v>905</v>
+      </c>
+      <c r="J53" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="14" t="s">
+        <v>912</v>
+      </c>
+      <c r="J54" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
+      <c r="H55" s="27" t="s">
+        <v>914</v>
       </c>
       <c r="J55" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C56" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E56" t="s">
-        <v>697</v>
-      </c>
-      <c r="F56">
-        <v>2002</v>
-      </c>
-      <c r="H56" t="s">
-        <v>890</v>
-      </c>
-      <c r="L56" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C57" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E57" t="s">
-        <v>697</v>
-      </c>
-      <c r="F57">
-        <v>2003</v>
-      </c>
+        <v>913</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
+      <c r="H56" s="29" t="s">
+        <v>628</v>
+      </c>
+      <c r="I56" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F57" s="61"/>
+      <c r="G57" s="61"/>
       <c r="H57" t="s">
-        <v>889</v>
+        <v>661</v>
       </c>
       <c r="K57" t="s">
-        <v>950</v>
-      </c>
-      <c r="L57" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>964</v>
+      </c>
       <c r="C58" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E58" t="s">
-        <v>697</v>
+        <v>856</v>
       </c>
       <c r="F58">
-        <v>2004</v>
+        <v>707</v>
       </c>
       <c r="H58" t="s">
-        <v>888</v>
-      </c>
-      <c r="K58" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>896</v>
+      </c>
+      <c r="J58" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>964</v>
+      </c>
       <c r="C59" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E59" t="s">
-        <v>697</v>
+        <v>856</v>
       </c>
       <c r="F59">
-        <v>2005</v>
+        <v>708</v>
       </c>
       <c r="H59" t="s">
-        <v>887</v>
-      </c>
-      <c r="K59" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+      <c r="J59" t="s">
+        <v>700</v>
+      </c>
+      <c r="P59">
+        <v>2014</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>964</v>
+      </c>
       <c r="C60" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E60" t="s">
-        <v>697</v>
+        <v>856</v>
       </c>
       <c r="F60">
-        <v>2006</v>
+        <v>710</v>
       </c>
       <c r="H60" t="s">
-        <v>886</v>
-      </c>
-      <c r="K60" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C61" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E61" t="s">
-        <v>697</v>
-      </c>
-      <c r="F61">
-        <v>2007</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="J60" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F61" s="61"/>
+      <c r="G61" s="61"/>
       <c r="H61" t="s">
-        <v>885</v>
-      </c>
-      <c r="K61" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C62" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E62" t="s">
-        <v>697</v>
-      </c>
-      <c r="F62">
-        <v>2008</v>
-      </c>
+        <v>636</v>
+      </c>
+      <c r="J61" t="s">
+        <v>637</v>
+      </c>
+      <c r="P61">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
       <c r="H62" t="s">
-        <v>884</v>
-      </c>
-      <c r="K62" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E63" t="s">
-        <v>697</v>
-      </c>
-      <c r="F63">
-        <v>2009</v>
-      </c>
+        <v>638</v>
+      </c>
+      <c r="J62" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F63" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G63" s="8"/>
       <c r="H63" t="s">
-        <v>883</v>
+        <v>636</v>
       </c>
       <c r="K63" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E64" t="s">
-        <v>697</v>
-      </c>
-      <c r="F64">
-        <v>2010</v>
-      </c>
+        <v>655</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F64" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G64" s="8"/>
       <c r="H64" t="s">
-        <v>882</v>
+        <v>638</v>
       </c>
       <c r="K64" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="65" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C65" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="E65" t="s">
-        <v>697</v>
-      </c>
-      <c r="F65">
-        <v>2011</v>
-      </c>
+        <v>656</v>
+      </c>
+      <c r="P64">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H65" t="s">
-        <v>881</v>
-      </c>
-      <c r="K65" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="66" spans="3:16" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>964</v>
+      </c>
       <c r="C66" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E66" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F66">
-        <v>2012</v>
+        <v>733</v>
       </c>
       <c r="H66" t="s">
-        <v>880</v>
-      </c>
-      <c r="K66" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="67" spans="3:16" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+      <c r="J66" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>964</v>
+      </c>
       <c r="C67" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="E67" t="s">
-        <v>697</v>
-      </c>
-      <c r="F67">
+        <v>695</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" t="s">
+        <v>894</v>
+      </c>
+      <c r="J67" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B69" t="s">
+        <v>964</v>
+      </c>
+      <c r="C69" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E69" t="s">
+        <v>696</v>
+      </c>
+      <c r="F69">
+        <v>761</v>
+      </c>
+      <c r="H69" t="s">
+        <v>892</v>
+      </c>
+      <c r="I69" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F70" s="61"/>
+      <c r="G70" s="61"/>
+      <c r="H70" t="s">
+        <v>657</v>
+      </c>
+      <c r="I70" t="s">
+        <v>908</v>
+      </c>
+      <c r="J70" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F71" s="61"/>
+      <c r="G71" s="61"/>
+      <c r="H71" s="14" t="s">
+        <v>657</v>
+      </c>
+      <c r="I71" s="29" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
+      <c r="H72" t="s">
+        <v>658</v>
+      </c>
+      <c r="K72" t="s">
+        <v>659</v>
+      </c>
+      <c r="P72">
         <v>2013</v>
       </c>
-      <c r="H67" t="s">
-        <v>879</v>
-      </c>
-      <c r="K67" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="68" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C68" s="44" t="s">
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F73" s="61"/>
+      <c r="G73" s="61"/>
+      <c r="H73" s="14" t="s">
+        <v>658</v>
+      </c>
+      <c r="I73" s="29" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B74" t="s">
+        <v>964</v>
+      </c>
+      <c r="C74" s="44" t="s">
         <v>1165</v>
       </c>
-      <c r="E68" t="s">
-        <v>697</v>
-      </c>
-      <c r="F68">
-        <v>2014</v>
-      </c>
-      <c r="H68" t="s">
-        <v>878</v>
-      </c>
-      <c r="K68" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="70" spans="3:16" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H73" s="20" t="s">
-        <v>631</v>
-      </c>
-      <c r="J73" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="74" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>696</v>
+      </c>
+      <c r="F74">
+        <v>765</v>
+      </c>
       <c r="H74" t="s">
-        <v>630</v>
-      </c>
-      <c r="J74" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="75" spans="3:16" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="I74" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
       <c r="H75" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="J75" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="76" spans="3:16" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F76" s="61"/>
+      <c r="G76" s="61"/>
       <c r="H76" t="s">
-        <v>628</v>
-      </c>
-      <c r="I76" t="s">
-        <v>904</v>
+        <v>634</v>
       </c>
       <c r="J76" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="77" spans="3:16" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F77" s="61"/>
+      <c r="G77" s="61"/>
       <c r="H77" t="s">
-        <v>627</v>
-      </c>
-      <c r="I77" t="s">
-        <v>905</v>
-      </c>
-      <c r="J77" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="78" spans="3:16" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+      <c r="K77" t="s">
+        <v>642</v>
+      </c>
+      <c r="P77">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F78" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G78" s="8"/>
       <c r="H78" t="s">
         <v>633</v>
       </c>
-      <c r="J78" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="79" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>907</v>
+      </c>
+      <c r="J78" s="5"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F79" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G79" s="8"/>
       <c r="H79" t="s">
-        <v>634</v>
-      </c>
-      <c r="J79" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="80" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H80" t="s">
-        <v>636</v>
-      </c>
-      <c r="J80" t="s">
-        <v>637</v>
-      </c>
-      <c r="P80">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="81" spans="6:16" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+      <c r="I79" t="s">
+        <v>906</v>
+      </c>
+      <c r="K79" t="s">
+        <v>909</v>
+      </c>
+      <c r="L79" t="s">
+        <v>654</v>
+      </c>
+      <c r="P79">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H81" t="s">
-        <v>638</v>
-      </c>
-      <c r="J81" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="82" spans="6:16" x14ac:dyDescent="0.25">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>964</v>
+      </c>
+      <c r="C82" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E82" t="s">
+        <v>697</v>
+      </c>
+      <c r="F82">
+        <v>2001</v>
+      </c>
       <c r="H82" t="s">
-        <v>535</v>
-      </c>
-      <c r="I82" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="J82" t="s">
-        <v>640</v>
-      </c>
-      <c r="P82">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>964</v>
+      </c>
+      <c r="C83" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E83" t="s">
+        <v>697</v>
+      </c>
+      <c r="F83">
+        <v>2002</v>
+      </c>
+      <c r="H83" t="s">
+        <v>890</v>
+      </c>
+      <c r="L83" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>964</v>
+      </c>
+      <c r="C84" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E84" t="s">
+        <v>697</v>
+      </c>
+      <c r="F84">
+        <v>2003</v>
+      </c>
+      <c r="H84" t="s">
+        <v>889</v>
+      </c>
+      <c r="K84" t="s">
+        <v>950</v>
+      </c>
+      <c r="L84" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>964</v>
+      </c>
+      <c r="C85" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E85" t="s">
+        <v>697</v>
+      </c>
+      <c r="F85">
+        <v>2004</v>
+      </c>
+      <c r="H85" t="s">
+        <v>888</v>
+      </c>
+      <c r="K85" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>964</v>
+      </c>
+      <c r="C86" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E86" t="s">
+        <v>697</v>
+      </c>
+      <c r="F86">
+        <v>2005</v>
+      </c>
+      <c r="H86" t="s">
+        <v>887</v>
+      </c>
+      <c r="K86" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>964</v>
+      </c>
+      <c r="C87" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E87" t="s">
+        <v>697</v>
+      </c>
+      <c r="F87">
+        <v>2006</v>
+      </c>
+      <c r="H87" t="s">
+        <v>886</v>
+      </c>
+      <c r="K87" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>964</v>
+      </c>
+      <c r="C88" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E88" t="s">
+        <v>697</v>
+      </c>
+      <c r="F88">
+        <v>2007</v>
+      </c>
+      <c r="H88" t="s">
+        <v>885</v>
+      </c>
+      <c r="K88" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>964</v>
+      </c>
+      <c r="C89" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E89" t="s">
+        <v>697</v>
+      </c>
+      <c r="F89">
+        <v>2008</v>
+      </c>
+      <c r="H89" t="s">
+        <v>884</v>
+      </c>
+      <c r="K89" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>964</v>
+      </c>
+      <c r="C90" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E90" t="s">
+        <v>697</v>
+      </c>
+      <c r="F90">
+        <v>2009</v>
+      </c>
+      <c r="H90" t="s">
+        <v>883</v>
+      </c>
+      <c r="K90" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>964</v>
+      </c>
+      <c r="C91" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E91" t="s">
+        <v>697</v>
+      </c>
+      <c r="F91">
+        <v>2010</v>
+      </c>
+      <c r="H91" t="s">
+        <v>882</v>
+      </c>
+      <c r="K91" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>964</v>
+      </c>
+      <c r="C92" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E92" t="s">
+        <v>697</v>
+      </c>
+      <c r="F92">
         <v>2011</v>
       </c>
-    </row>
-    <row r="83" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H83" s="14" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="84" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H84" s="14" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="85" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H85" s="14" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="86" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H86" t="s">
-        <v>641</v>
-      </c>
-      <c r="K86" t="s">
-        <v>642</v>
-      </c>
-      <c r="P86">
+      <c r="H92" t="s">
+        <v>881</v>
+      </c>
+      <c r="K92" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>964</v>
+      </c>
+      <c r="C93" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E93" t="s">
+        <v>697</v>
+      </c>
+      <c r="F93">
+        <v>2012</v>
+      </c>
+      <c r="H93" t="s">
+        <v>880</v>
+      </c>
+      <c r="K93" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>964</v>
+      </c>
+      <c r="C94" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E94" t="s">
+        <v>697</v>
+      </c>
+      <c r="F94">
+        <v>2013</v>
+      </c>
+      <c r="H94" t="s">
+        <v>879</v>
+      </c>
+      <c r="K94" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>964</v>
+      </c>
+      <c r="C95" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E95" t="s">
+        <v>697</v>
+      </c>
+      <c r="F95">
+        <v>2014</v>
+      </c>
+      <c r="H95" t="s">
+        <v>878</v>
+      </c>
+      <c r="K95" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>643</v>
+      </c>
+      <c r="J100" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
+        <v>1181</v>
+      </c>
+      <c r="H101" t="s">
+        <v>646</v>
+      </c>
+      <c r="K101" t="s">
+        <v>645</v>
+      </c>
+      <c r="P101">
         <v>2006</v>
       </c>
     </row>
-    <row r="87" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H87" t="s">
-        <v>643</v>
-      </c>
-      <c r="J87" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="88" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H88" t="s">
-        <v>646</v>
-      </c>
-      <c r="K88" t="s">
-        <v>645</v>
-      </c>
-      <c r="P88">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="90" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H90" t="s">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
+        <v>1181</v>
+      </c>
+      <c r="H103" t="s">
         <v>647</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J103" t="s">
         <v>649</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K103" t="s">
         <v>648</v>
       </c>
-      <c r="P90">
+      <c r="P103">
         <v>2011</v>
       </c>
     </row>
-    <row r="91" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H91" t="s">
-        <v>650</v>
-      </c>
-      <c r="J91" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="93" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F93" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="G93" s="8"/>
-      <c r="H93" t="s">
-        <v>633</v>
-      </c>
-      <c r="I93" t="s">
-        <v>907</v>
-      </c>
-      <c r="J93" s="5"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="7" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="94" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F94" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="G94" s="8"/>
-      <c r="H94" t="s">
-        <v>652</v>
-      </c>
-      <c r="I94" t="s">
-        <v>906</v>
-      </c>
-      <c r="K94" t="s">
-        <v>909</v>
-      </c>
-      <c r="L94" t="s">
-        <v>654</v>
-      </c>
-      <c r="P94">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="96" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F96" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="G96" s="8"/>
-      <c r="H96" t="s">
-        <v>636</v>
-      </c>
-      <c r="K96" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="97" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F97" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="G97" s="8"/>
-      <c r="H97" t="s">
-        <v>638</v>
-      </c>
-      <c r="K97" t="s">
-        <v>656</v>
-      </c>
-      <c r="P97">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="99" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H99" t="s">
-        <v>657</v>
-      </c>
-      <c r="I99" t="s">
-        <v>908</v>
-      </c>
-      <c r="J99" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="100" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H100" s="14" t="s">
-        <v>657</v>
-      </c>
-      <c r="I100" s="29" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="101" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H101" t="s">
-        <v>658</v>
-      </c>
-      <c r="K101" t="s">
-        <v>659</v>
-      </c>
-      <c r="P101">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="102" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H102" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="I102" s="29" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="104" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H104" t="s">
-        <v>630</v>
-      </c>
-      <c r="I104" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="105" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H105" t="s">
-        <v>629</v>
-      </c>
-      <c r="K105" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="106" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H105" s="27" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H106" s="29" t="s">
-        <v>628</v>
-      </c>
-      <c r="I106" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="107" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H107" t="s">
-        <v>661</v>
+        <v>922</v>
+      </c>
+      <c r="K106" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H107" s="29" t="s">
+        <v>925</v>
       </c>
       <c r="K107" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="110" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
-      <c r="K110" s="4"/>
-      <c r="L110" s="4"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="4"/>
-      <c r="O110" s="4"/>
-    </row>
-    <row r="111" spans="6:16" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="H112" s="14" t="s">
-        <v>912</v>
-      </c>
-      <c r="J112" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="113" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H113" s="27" t="s">
-        <v>914</v>
-      </c>
-      <c r="J113" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="114" spans="6:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
-      <c r="J115" s="4"/>
-      <c r="K115" s="4"/>
-      <c r="L115" s="4"/>
-      <c r="M115" s="4"/>
-      <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
-    </row>
-    <row r="116" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H116" s="27" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="117" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H117" s="29" t="s">
-        <v>922</v>
-      </c>
-      <c r="K117" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="118" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H118" s="29" t="s">
-        <v>925</v>
-      </c>
-      <c r="K118" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="119" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H119" t="s">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
         <v>663</v>
       </c>
-      <c r="K119" t="s">
+      <c r="K108" t="s">
         <v>936</v>
       </c>
-      <c r="L119" s="11" t="s">
+      <c r="L108" s="11" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="120" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H120" t="s">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
         <v>664</v>
       </c>
-      <c r="K120" s="29" t="s">
+      <c r="K109" s="29" t="s">
         <v>947</v>
       </c>
-      <c r="L120" s="11" t="s">
+      <c r="L109" s="11" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="121" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H121" t="s">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
         <v>665</v>
       </c>
-      <c r="L121" s="11" t="s">
+      <c r="L110" s="11" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="122" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="H122" t="s">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
         <v>666</v>
       </c>
-      <c r="K122" t="s">
+      <c r="K111" t="s">
         <v>938</v>
       </c>
     </row>
-    <row r="124" spans="6:15" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -28869,12 +29021,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="F1" workbookViewId="1">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29105,6 +29259,46 @@
         <v>933</v>
       </c>
     </row>
+    <row r="28" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H28" s="20" t="s">
+        <v>631</v>
+      </c>
+      <c r="J28" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="30" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>650</v>
+      </c>
+      <c r="J30" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>2282</v>
+      </c>
+      <c r="J33" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>667</v>
+      </c>
+      <c r="J34" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>964</v>
+      </c>
+      <c r="J35" t="s">
+        <v>963</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29114,11 +29308,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="E55" workbookViewId="1">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29834,7 +30030,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="D1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29975,7 +30171,9 @@
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="1">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30121,6 +30319,9 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H14" t="s">
         <v>732</v>
       </c>
@@ -30129,6 +30330,9 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H15" t="s">
         <v>733</v>
       </c>
@@ -30137,6 +30341,9 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H16" t="s">
         <v>734</v>
       </c>
@@ -30144,7 +30351,10 @@
         <v>797</v>
       </c>
     </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H17" t="s">
         <v>735</v>
       </c>
@@ -30152,7 +30362,10 @@
         <v>798</v>
       </c>
     </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H18" t="s">
         <v>736</v>
       </c>
@@ -30163,37 +30376,40 @@
         <v>799</v>
       </c>
     </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H19" s="14" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H20" s="14" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H21" s="14" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H22" s="14" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="23" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H23" s="14" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="24" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H24" s="14" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="25" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H25" t="s">
         <v>737</v>
       </c>
@@ -30201,22 +30417,25 @@
         <v>800</v>
       </c>
     </row>
-    <row r="26" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H26" s="14" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="27" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H27" s="14" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="28" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H28" s="14" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="29" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H29" t="s">
         <v>738</v>
       </c>
@@ -30227,7 +30446,10 @@
         <v>801</v>
       </c>
     </row>
-    <row r="30" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H30" t="s">
         <v>739</v>
       </c>
@@ -30235,7 +30457,10 @@
         <v>802</v>
       </c>
     </row>
-    <row r="31" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H31" t="s">
         <v>740</v>
       </c>
@@ -30243,7 +30468,10 @@
         <v>803</v>
       </c>
     </row>
-    <row r="32" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H32" t="s">
         <v>741</v>
       </c>
@@ -30251,7 +30479,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="33" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H33" s="14" t="s">
         <v>712</v>
       </c>
@@ -30265,7 +30493,10 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="34" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H34" t="s">
         <v>707</v>
       </c>
@@ -30273,7 +30504,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="35" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -30284,7 +30515,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="8:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H36" s="37"/>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
@@ -30298,7 +30529,7 @@
       <c r="R36" s="38"/>
       <c r="S36" s="37"/>
     </row>
-    <row r="37" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H37" s="23" t="s">
         <v>849</v>
       </c>
@@ -30312,7 +30543,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="38" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H38" s="27" t="s">
         <v>707</v>
       </c>
@@ -30329,7 +30560,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>719</v>
       </c>
@@ -30343,7 +30574,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="40" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H40" s="14" t="s">
         <v>822</v>
       </c>
@@ -30354,7 +30585,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="41" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H41" s="14" t="s">
         <v>825</v>
       </c>
@@ -30368,7 +30599,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="42" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H42" s="11" t="s">
         <v>824</v>
       </c>
@@ -30379,7 +30610,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="43" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H43" s="14" t="s">
         <v>823</v>
       </c>
@@ -30390,7 +30621,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="44" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
         <v>717</v>
       </c>
@@ -30404,7 +30635,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="45" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H45" s="14" t="s">
         <v>849</v>
       </c>
@@ -30418,7 +30649,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="46" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
         <v>716</v>
       </c>
@@ -30435,7 +30666,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="47" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
         <v>715</v>
       </c>
@@ -30452,15 +30683,18 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="48" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H48" t="s">
         <v>714</v>
       </c>
       <c r="J48" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="49" spans="8:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P48">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H49" s="37"/>
       <c r="I49" s="37"/>
       <c r="J49" s="37"/>
@@ -30474,7 +30708,7 @@
       <c r="R49" s="38"/>
       <c r="S49" s="37"/>
     </row>
-    <row r="50" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H50" s="18" t="s">
         <v>1061</v>
       </c>
@@ -30483,7 +30717,7 @@
       </c>
       <c r="R50" s="43"/>
     </row>
-    <row r="51" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H51" s="18" t="s">
         <v>1062</v>
       </c>
@@ -30492,7 +30726,7 @@
       </c>
       <c r="R51" s="43"/>
     </row>
-    <row r="52" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H52" s="18" t="s">
         <v>1063</v>
       </c>
@@ -30501,7 +30735,7 @@
       </c>
       <c r="R52" s="43"/>
     </row>
-    <row r="53" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H53" s="18" t="s">
         <v>1064</v>
       </c>
@@ -30510,7 +30744,7 @@
       </c>
       <c r="R53" s="43"/>
     </row>
-    <row r="54" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H54" s="18" t="s">
         <v>1065</v>
       </c>
@@ -30519,7 +30753,7 @@
       </c>
       <c r="R54" s="43"/>
     </row>
-    <row r="55" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H55" s="18" t="s">
         <v>1066</v>
       </c>
@@ -30528,7 +30762,7 @@
       </c>
       <c r="R55" s="43"/>
     </row>
-    <row r="56" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H56" s="18" t="s">
         <v>1067</v>
       </c>
@@ -30537,7 +30771,7 @@
       </c>
       <c r="R56" s="43"/>
     </row>
-    <row r="57" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H57" s="18" t="s">
         <v>1068</v>
       </c>
@@ -30546,7 +30780,7 @@
       </c>
       <c r="R57" s="43"/>
     </row>
-    <row r="58" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H58" s="18" t="s">
         <v>1069</v>
       </c>
@@ -30555,7 +30789,7 @@
       </c>
       <c r="R58" s="43"/>
     </row>
-    <row r="59" spans="8:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H59" s="18" t="s">
         <v>1070</v>
       </c>
@@ -30564,7 +30798,7 @@
       </c>
       <c r="R59" s="43"/>
     </row>
-    <row r="60" spans="8:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H60" s="37"/>
       <c r="I60" s="37"/>
       <c r="J60" s="37"/>
@@ -30578,7 +30812,7 @@
       <c r="R60" s="38"/>
       <c r="S60" s="37"/>
     </row>
-    <row r="61" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
@@ -30589,7 +30823,10 @@
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
     </row>
-    <row r="62" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B62" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H62" t="s">
         <v>742</v>
       </c>
@@ -30597,7 +30834,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="63" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H63" s="14" t="s">
         <v>848</v>
       </c>
@@ -30617,7 +30854,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B64" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H64" t="s">
         <v>725</v>
       </c>
@@ -30625,7 +30865,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="65" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H65" s="14" t="s">
         <v>725</v>
       </c>
@@ -30636,7 +30876,10 @@
         <v>727</v>
       </c>
     </row>
-    <row r="66" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B66" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H66" t="s">
         <v>743</v>
       </c>
@@ -30644,7 +30887,10 @@
         <v>808</v>
       </c>
     </row>
-    <row r="67" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B67" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H67" t="s">
         <v>744</v>
       </c>
@@ -30652,7 +30898,10 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B68" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H68" t="s">
         <v>745</v>
       </c>
@@ -30660,7 +30909,10 @@
         <v>809</v>
       </c>
     </row>
-    <row r="69" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B69" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H69" t="s">
         <v>746</v>
       </c>
@@ -30668,7 +30920,10 @@
         <v>810</v>
       </c>
     </row>
-    <row r="70" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H70" t="s">
         <v>747</v>
       </c>
@@ -30676,17 +30931,23 @@
         <v>811</v>
       </c>
     </row>
-    <row r="71" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B71" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H71" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="72" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B72" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H72" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="73" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H73" s="14" t="s">
         <v>829</v>
       </c>
@@ -30700,7 +30961,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="74" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H74" s="14" t="s">
         <v>830</v>
       </c>
@@ -30711,12 +30972,15 @@
         <v>797</v>
       </c>
     </row>
-    <row r="75" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B75" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H75" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="76" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -30727,7 +30991,7 @@
       <c r="O76" s="4"/>
       <c r="P76" s="4"/>
     </row>
-    <row r="77" spans="8:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:19" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H77" s="37"/>
       <c r="I77" s="37"/>
       <c r="J77" s="37"/>
@@ -30741,7 +31005,7 @@
       <c r="R77" s="38"/>
       <c r="S77" s="37"/>
     </row>
-    <row r="78" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H78" t="s">
         <v>720</v>
       </c>
@@ -30758,7 +31022,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="79" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H79" t="s">
         <v>722</v>
       </c>
@@ -30766,7 +31030,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="80" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H80" t="s">
         <v>723</v>
       </c>
@@ -30929,7 +31193,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="97" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H97" s="23" t="s">
         <v>990</v>
       </c>
@@ -30937,7 +31201,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="98" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H98" t="s">
         <v>754</v>
       </c>
@@ -30948,12 +31212,12 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="99" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H99" s="23" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="100" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H100" t="s">
         <v>755</v>
       </c>
@@ -30964,7 +31228,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="101" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H101" s="23" t="s">
         <v>722</v>
       </c>
@@ -30975,7 +31239,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="102" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H102" t="s">
         <v>756</v>
       </c>
@@ -30986,7 +31250,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="103" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H103" s="23" t="s">
         <v>995</v>
       </c>
@@ -30994,7 +31258,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="104" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H104" t="s">
         <v>757</v>
       </c>
@@ -31005,7 +31269,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="105" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H105" s="23" t="s">
         <v>995</v>
       </c>
@@ -31013,7 +31277,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="106" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H106" t="s">
         <v>758</v>
       </c>
@@ -31021,7 +31285,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="107" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H107" t="s">
         <v>759</v>
       </c>
@@ -31032,7 +31296,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="108" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H108" t="s">
         <v>760</v>
       </c>
@@ -31040,7 +31304,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="110" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H110" s="5" t="s">
         <v>730</v>
       </c>
@@ -31048,7 +31312,10 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="111" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B111" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H111" t="s">
         <v>761</v>
       </c>
@@ -31056,7 +31323,10 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="112" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B112" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H112" t="s">
         <v>762</v>
       </c>
@@ -31064,7 +31334,10 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="113" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H113" t="s">
         <v>763</v>
       </c>
@@ -31072,7 +31345,10 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="114" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H114" t="s">
         <v>764</v>
       </c>
@@ -31080,7 +31356,10 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="115" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H115" t="s">
         <v>765</v>
       </c>
@@ -31088,7 +31367,10 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="116" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H116" t="s">
         <v>766</v>
       </c>
@@ -31096,7 +31378,10 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="117" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H117" t="s">
         <v>767</v>
       </c>
@@ -31104,7 +31389,10 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="118" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H118" t="s">
         <v>768</v>
       </c>
@@ -31112,7 +31400,10 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="119" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H119" t="s">
         <v>769</v>
       </c>
@@ -31120,7 +31411,10 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="120" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H120" t="s">
         <v>770</v>
       </c>
@@ -31128,7 +31422,10 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="121" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H121" t="s">
         <v>771</v>
       </c>
@@ -31136,7 +31433,10 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="122" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H122" t="s">
         <v>772</v>
       </c>
@@ -31144,7 +31444,10 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="123" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H123" t="s">
         <v>773</v>
       </c>
@@ -31152,7 +31455,10 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="124" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H124" t="s">
         <v>774</v>
       </c>
@@ -31160,7 +31466,10 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="125" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H125" t="s">
         <v>775</v>
       </c>
@@ -31168,7 +31477,10 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="126" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H126" t="s">
         <v>776</v>
       </c>
@@ -31176,7 +31488,10 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="127" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B127" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H127" t="s">
         <v>777</v>
       </c>
@@ -31184,7 +31499,10 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="128" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H128" t="s">
         <v>778</v>
       </c>
@@ -31192,7 +31510,10 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="129" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B129" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H129" t="s">
         <v>779</v>
       </c>
@@ -31200,7 +31521,10 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="130" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B130" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H130" t="s">
         <v>780</v>
       </c>
@@ -31208,7 +31532,10 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="131" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B131" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H131" t="s">
         <v>781</v>
       </c>
@@ -31216,7 +31543,10 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="132" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B132" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H132" t="s">
         <v>782</v>
       </c>
@@ -31224,7 +31554,10 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="133" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B133" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H133" t="s">
         <v>783</v>
       </c>
@@ -31232,7 +31565,10 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="134" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B134" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H134" t="s">
         <v>784</v>
       </c>
@@ -31240,7 +31576,10 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="135" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B135" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H135" t="s">
         <v>785</v>
       </c>
@@ -31248,7 +31587,10 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="136" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B136" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H136" t="s">
         <v>786</v>
       </c>
@@ -31256,7 +31598,10 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="137" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B137" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H137" t="s">
         <v>787</v>
       </c>
@@ -31264,7 +31609,10 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="138" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B138" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H138" t="s">
         <v>788</v>
       </c>
@@ -31272,7 +31620,10 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="139" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B139" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H139" t="s">
         <v>789</v>
       </c>
@@ -31280,7 +31631,10 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="140" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B140" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H140" t="s">
         <v>790</v>
       </c>
@@ -31288,7 +31642,10 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="141" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B141" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H141" t="s">
         <v>791</v>
       </c>
@@ -31296,7 +31653,10 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="142" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B142" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H142" t="s">
         <v>792</v>
       </c>
@@ -31304,7 +31664,10 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="143" spans="8:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B143" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H143" t="s">
         <v>793</v>
       </c>
@@ -31312,7 +31675,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="144" spans="8:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H144" s="35"/>
       <c r="I144" s="35"/>
       <c r="J144" s="35"/>

</xml_diff>

<commit_message>
adding archival links for EBRD policy
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="-345" windowWidth="19755" windowHeight="10155" tabRatio="810" activeTab="8"/>
-    <workbookView xWindow="10905" yWindow="-30" windowWidth="11070" windowHeight="9780" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="10905" yWindow="-30" windowWidth="11040" windowHeight="9780" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5283" uniqueCount="2286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5395" uniqueCount="2313">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -6884,6 +6884,87 @@
   </si>
   <si>
     <t>german</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/1996-09-01,_Environmental_Policy-_Russian_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/1996-09-01,_Environmental_Policy-_German_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/1996-09-01,_Environmental_Policy-_French_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/1992-02-13_Environmental__Policy.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/2003-07-01,_Environmental_Policy-_Russian_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_policy/2008-05-14,_Environmental_and_Social_Policy-_Publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/esp-english.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/esp-french.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/esp-russian.pdf</t>
+  </si>
+  <si>
+    <t>Environmental Proceedures, 1992</t>
+  </si>
+  <si>
+    <t>Environmental Proceedures, 1996</t>
+  </si>
+  <si>
+    <t>Environmental Proceedures, 2003</t>
+  </si>
+  <si>
+    <t>Environmental Proceedures, 2008</t>
+  </si>
+  <si>
+    <t>Environmental Proceedures, 2010</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_procedure/1996-09-01,_Environmental_Procedures-_English_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_procedure/1996-09-01,_Environmental_Procedures-_Russian_publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_procedure/2003-12-12,_EBRD_Environmental_Procedures.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_procedure/1992-02-13_Environmental_Procedures.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_procedure/2008-11-01__Environmental_and_Social_Procedures-_Publication.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/about/policies/environmental_procedure/2010-04-01,_Environmental_and_Social_Procedures-_Publication.pdf</t>
+  </si>
+  <si>
+    <t>Procurement Policies and Proceedures, 1992</t>
+  </si>
+  <si>
+    <t>Procurement Policies and Proceedures, 1996</t>
+  </si>
+  <si>
+    <t>Procurement Policies and Proceedures, 1998</t>
+  </si>
+  <si>
+    <t>Procurement Policies and Proceedures, 2000</t>
+  </si>
+  <si>
+    <t>Procurement Policies and Proceedures, 2007</t>
+  </si>
+  <si>
+    <t>Procurement Policies and Proceedures, 2009</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -30363,11 +30444,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V145"/>
+  <dimension ref="A2:V162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
+      <pane ySplit="10" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="1">
       <selection activeCell="H39" sqref="H39"/>
@@ -30528,6 +30609,9 @@
       <c r="B14" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C14" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H14" t="s">
         <v>732</v>
       </c>
@@ -30539,6 +30623,9 @@
       <c r="B15" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C15" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H15" t="s">
         <v>733</v>
       </c>
@@ -30550,6 +30637,9 @@
       <c r="B16" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C16" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H16" t="s">
         <v>734</v>
       </c>
@@ -30561,6 +30651,9 @@
       <c r="B17" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C17" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H17" t="s">
         <v>735</v>
       </c>
@@ -30570,6 +30663,9 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C18" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H18" t="s">
@@ -30616,6 +30712,9 @@
       <c r="B25" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C25" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H25" t="s">
         <v>737</v>
       </c>
@@ -30642,6 +30741,9 @@
       <c r="B29" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C29" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H29" t="s">
         <v>738</v>
       </c>
@@ -30656,6 +30758,9 @@
       <c r="B30" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C30" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H30" t="s">
         <v>739</v>
       </c>
@@ -30665,6 +30770,9 @@
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C31" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H31" t="s">
@@ -30771,6 +30879,9 @@
       </c>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C39" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H39" t="s">
         <v>719</v>
       </c>
@@ -30785,6 +30896,9 @@
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C40" s="44" t="s">
+        <v>2312</v>
+      </c>
       <c r="H40" s="14" t="s">
         <v>822</v>
       </c>
@@ -30796,92 +30910,98 @@
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H41" s="14" t="s">
+      <c r="C41" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H41" t="s">
+        <v>719</v>
+      </c>
+      <c r="I41" t="s">
+        <v>2292</v>
+      </c>
+      <c r="N41" t="s">
+        <v>2294</v>
+      </c>
+      <c r="P41" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H42" s="14" t="s">
         <v>825</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I42" t="s">
         <v>831</v>
-      </c>
-      <c r="L41" t="s">
-        <v>797</v>
-      </c>
-      <c r="R41">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H42" s="11" t="s">
-        <v>824</v>
-      </c>
-      <c r="I42" t="s">
-        <v>827</v>
       </c>
       <c r="L42" t="s">
         <v>797</v>
       </c>
+      <c r="R42">
+        <v>1992</v>
+      </c>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H43" s="14" t="s">
-        <v>823</v>
-      </c>
-      <c r="J43" t="s">
-        <v>797</v>
+      <c r="H43" s="11" t="s">
+        <v>824</v>
+      </c>
+      <c r="I43" t="s">
+        <v>827</v>
       </c>
       <c r="L43" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
+      <c r="H44" s="14" t="s">
+        <v>823</v>
+      </c>
+      <c r="J44" t="s">
+        <v>797</v>
+      </c>
+      <c r="L44" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
         <v>717</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>705</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J45" t="s">
         <v>706</v>
       </c>
-      <c r="R44">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H45" s="14" t="s">
-        <v>849</v>
-      </c>
-      <c r="I45" t="s">
-        <v>713</v>
-      </c>
       <c r="L45" t="s">
-        <v>845</v>
+        <v>2291</v>
       </c>
       <c r="R45">
         <v>2008</v>
       </c>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
+      <c r="H46" s="14" t="s">
+        <v>849</v>
+      </c>
+      <c r="I46" t="s">
+        <v>713</v>
+      </c>
+      <c r="L46" t="s">
+        <v>845</v>
+      </c>
+      <c r="R46">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C47" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H47" t="s">
         <v>716</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>708</v>
-      </c>
-      <c r="J46" t="s">
-        <v>711</v>
-      </c>
-      <c r="L46" t="s">
-        <v>710</v>
-      </c>
-      <c r="R46">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H47" t="s">
-        <v>715</v>
-      </c>
-      <c r="I47" t="s">
-        <v>709</v>
       </c>
       <c r="J47" t="s">
         <v>711</v>
@@ -30890,1046 +31010,1371 @@
         <v>710</v>
       </c>
       <c r="R47">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C48" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H48" t="s">
+        <v>716</v>
+      </c>
+      <c r="I48" t="s">
+        <v>708</v>
+      </c>
+      <c r="N48" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C49" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H49" t="s">
+        <v>715</v>
+      </c>
+      <c r="I49" t="s">
+        <v>709</v>
+      </c>
+      <c r="J49" t="s">
+        <v>711</v>
+      </c>
+      <c r="L49" t="s">
+        <v>710</v>
+      </c>
+      <c r="R49">
         <v>1996</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H48" t="s">
+    <row r="50" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C50" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H50" t="s">
+        <v>715</v>
+      </c>
+      <c r="I50" t="s">
+        <v>709</v>
+      </c>
+      <c r="N50" t="s">
+        <v>2286</v>
+      </c>
+      <c r="P50" t="s">
+        <v>2288</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="51" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C51" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H51" t="s">
         <v>714</v>
       </c>
-      <c r="J48" t="s">
+      <c r="I51" t="s">
+        <v>2289</v>
+      </c>
+      <c r="J51" t="s">
         <v>711</v>
       </c>
-      <c r="R48">
+      <c r="R51">
         <v>1992</v>
       </c>
     </row>
-    <row r="49" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
-      <c r="N49" s="37"/>
-      <c r="O49" s="37"/>
-      <c r="P49" s="37"/>
-      <c r="Q49" s="37"/>
-      <c r="R49" s="37"/>
-      <c r="S49" s="37"/>
-      <c r="T49" s="38"/>
-      <c r="U49" s="37"/>
-    </row>
-    <row r="50" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H50" s="18" t="s">
+    <row r="52" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="37"/>
+      <c r="P52" s="37"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="37"/>
+      <c r="S52" s="37"/>
+      <c r="T52" s="38"/>
+      <c r="U52" s="37"/>
+    </row>
+    <row r="53" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="18" t="s">
         <v>1061</v>
       </c>
-      <c r="I50" s="18" t="s">
+      <c r="I53" s="18" t="s">
         <v>1071</v>
       </c>
-      <c r="T50" s="43"/>
-    </row>
-    <row r="51" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H51" s="18" t="s">
+      <c r="T53" s="43"/>
+    </row>
+    <row r="54" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="18" t="s">
         <v>1062</v>
       </c>
-      <c r="I51" s="18" t="s">
+      <c r="I54" s="18" t="s">
         <v>1072</v>
       </c>
-      <c r="T51" s="43"/>
-    </row>
-    <row r="52" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H52" s="18" t="s">
+      <c r="T54" s="43"/>
+    </row>
+    <row r="55" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="18" t="s">
         <v>1063</v>
       </c>
-      <c r="I52" s="18" t="s">
+      <c r="I55" s="18" t="s">
         <v>1073</v>
       </c>
-      <c r="T52" s="43"/>
-    </row>
-    <row r="53" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H53" s="18" t="s">
+      <c r="T55" s="43"/>
+    </row>
+    <row r="56" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="18" t="s">
         <v>1064</v>
       </c>
-      <c r="I53" s="18" t="s">
+      <c r="I56" s="18" t="s">
         <v>1074</v>
       </c>
-      <c r="T53" s="43"/>
-    </row>
-    <row r="54" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H54" s="18" t="s">
+      <c r="T56" s="43"/>
+    </row>
+    <row r="57" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="18" t="s">
         <v>1065</v>
       </c>
-      <c r="I54" s="18" t="s">
+      <c r="I57" s="18" t="s">
         <v>1075</v>
       </c>
-      <c r="T54" s="43"/>
-    </row>
-    <row r="55" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H55" s="18" t="s">
+      <c r="T57" s="43"/>
+    </row>
+    <row r="58" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="18" t="s">
         <v>1066</v>
       </c>
-      <c r="I55" s="18" t="s">
+      <c r="I58" s="18" t="s">
         <v>1076</v>
       </c>
-      <c r="T55" s="43"/>
-    </row>
-    <row r="56" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H56" s="18" t="s">
+      <c r="T58" s="43"/>
+    </row>
+    <row r="59" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="18" t="s">
         <v>1067</v>
       </c>
-      <c r="I56" s="18" t="s">
+      <c r="I59" s="18" t="s">
         <v>1077</v>
       </c>
-      <c r="T56" s="43"/>
-    </row>
-    <row r="57" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H57" s="18" t="s">
+      <c r="T59" s="43"/>
+    </row>
+    <row r="60" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="18" t="s">
         <v>1068</v>
       </c>
-      <c r="I57" s="18" t="s">
+      <c r="I60" s="18" t="s">
         <v>1078</v>
       </c>
-      <c r="T57" s="43"/>
-    </row>
-    <row r="58" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H58" s="18" t="s">
+      <c r="T60" s="43"/>
+    </row>
+    <row r="61" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="18" t="s">
         <v>1069</v>
       </c>
-      <c r="I58" s="18" t="s">
+      <c r="I61" s="18" t="s">
         <v>1079</v>
       </c>
-      <c r="T58" s="43"/>
-    </row>
-    <row r="59" spans="2:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H59" s="18" t="s">
+      <c r="T61" s="43"/>
+    </row>
+    <row r="62" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="18" t="s">
         <v>1070</v>
       </c>
-      <c r="I59" s="18" t="s">
+      <c r="I62" s="18" t="s">
         <v>1080</v>
       </c>
-      <c r="T59" s="43"/>
-    </row>
-    <row r="60" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="37"/>
-      <c r="M60" s="37"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="37"/>
-      <c r="P60" s="37"/>
-      <c r="Q60" s="37"/>
-      <c r="R60" s="37"/>
-      <c r="S60" s="37"/>
-      <c r="T60" s="38"/>
-      <c r="U60" s="37"/>
-    </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-    </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B62" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H62" t="s">
+      <c r="T62" s="43"/>
+    </row>
+    <row r="63" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" s="37"/>
+      <c r="P63" s="37"/>
+      <c r="Q63" s="37"/>
+      <c r="R63" s="37"/>
+      <c r="S63" s="37"/>
+      <c r="T63" s="38"/>
+      <c r="U63" s="37"/>
+    </row>
+    <row r="64" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+    </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B65" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C65" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H65" t="s">
         <v>742</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I65" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H63" s="14" t="s">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H66" s="14" t="s">
         <v>848</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I66" t="s">
         <v>847</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J66" t="s">
         <v>846</v>
       </c>
-      <c r="R63">
+      <c r="R66">
         <v>2010</v>
       </c>
-      <c r="S63" t="s">
+      <c r="S66" t="s">
         <v>187</v>
       </c>
-      <c r="T63">
+      <c r="T66">
         <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B64" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H64" t="s">
-        <v>725</v>
-      </c>
-      <c r="I64" s="7" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H65" s="14" t="s">
-        <v>725</v>
-      </c>
-      <c r="I65" t="s">
-        <v>728</v>
-      </c>
-      <c r="J65" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B66" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H66" t="s">
-        <v>743</v>
-      </c>
-      <c r="I66" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="67" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B67" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C67" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H67" t="s">
-        <v>744</v>
-      </c>
-      <c r="J67" t="s">
-        <v>797</v>
+        <v>725</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="68" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B68" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H68" t="s">
-        <v>745</v>
+      <c r="H68" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="I68" t="s">
+        <v>728</v>
       </c>
       <c r="J68" t="s">
-        <v>809</v>
+        <v>727</v>
       </c>
     </row>
     <row r="69" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B69" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C69" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H69" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="I69" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="70" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B70" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C70" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H70" t="s">
-        <v>747</v>
-      </c>
-      <c r="I70" t="s">
-        <v>811</v>
+        <v>744</v>
+      </c>
+      <c r="J70" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="71" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B71" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C71" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H71" t="s">
-        <v>748</v>
+        <v>745</v>
+      </c>
+      <c r="J71" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B72" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C72" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H72" t="s">
-        <v>749</v>
+        <v>746</v>
+      </c>
+      <c r="I72" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="73" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H73" s="14" t="s">
-        <v>829</v>
+      <c r="B73" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C73" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H73" t="s">
+        <v>747</v>
       </c>
       <c r="I73" t="s">
-        <v>833</v>
-      </c>
-      <c r="J73" t="s">
-        <v>835</v>
-      </c>
-      <c r="L73" t="s">
-        <v>797</v>
+        <v>811</v>
       </c>
     </row>
     <row r="74" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H74" s="14" t="s">
-        <v>830</v>
-      </c>
-      <c r="I74" t="s">
-        <v>834</v>
-      </c>
-      <c r="L74" t="s">
-        <v>797</v>
+      <c r="B74" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C74" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H74" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="75" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B75" s="44" t="s">
         <v>1165</v>
       </c>
+      <c r="C75" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H75" t="s">
-        <v>720</v>
+        <v>749</v>
       </c>
     </row>
     <row r="76" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-      <c r="Q76" s="4"/>
-      <c r="R76" s="4"/>
-    </row>
-    <row r="77" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H77" s="37"/>
-      <c r="I77" s="37"/>
-      <c r="J77" s="37"/>
-      <c r="K77" s="37"/>
-      <c r="L77" s="37"/>
-      <c r="M77" s="37"/>
-      <c r="N77" s="37"/>
-      <c r="O77" s="37"/>
-      <c r="P77" s="37"/>
-      <c r="Q77" s="37"/>
-      <c r="R77" s="37"/>
-      <c r="S77" s="37"/>
-      <c r="T77" s="38"/>
-      <c r="U77" s="37"/>
+      <c r="H76" s="14" t="s">
+        <v>829</v>
+      </c>
+      <c r="I76" t="s">
+        <v>833</v>
+      </c>
+      <c r="J76" t="s">
+        <v>835</v>
+      </c>
+      <c r="L76" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H77" s="14" t="s">
+        <v>830</v>
+      </c>
+      <c r="I77" t="s">
+        <v>834</v>
+      </c>
+      <c r="L77" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="78" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B78" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C78" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H78" t="s">
         <v>720</v>
       </c>
-      <c r="I78" t="s">
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="4"/>
+    </row>
+    <row r="80" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="37"/>
+      <c r="K80" s="37"/>
+      <c r="L80" s="37"/>
+      <c r="M80" s="37"/>
+      <c r="N80" s="37"/>
+      <c r="O80" s="37"/>
+      <c r="P80" s="37"/>
+      <c r="Q80" s="37"/>
+      <c r="R80" s="37"/>
+      <c r="S80" s="37"/>
+      <c r="T80" s="38"/>
+      <c r="U80" s="37"/>
+    </row>
+    <row r="81" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C81" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H81" t="s">
+        <v>720</v>
+      </c>
+      <c r="I81" t="s">
         <v>721</v>
-      </c>
-      <c r="J78" t="s">
-        <v>726</v>
-      </c>
-      <c r="R78">
-        <v>2014</v>
-      </c>
-      <c r="S78" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H79" t="s">
-        <v>722</v>
-      </c>
-      <c r="K79" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H80" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="81" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H81" s="14" t="s">
-        <v>828</v>
-      </c>
-      <c r="I81" t="s">
-        <v>832</v>
       </c>
       <c r="J81" t="s">
         <v>726</v>
       </c>
-      <c r="L81" t="s">
-        <v>797</v>
-      </c>
       <c r="R81">
         <v>2014</v>
       </c>
-    </row>
-    <row r="82" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H82" s="14" t="s">
+      <c r="S81" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
         <v>722</v>
       </c>
-      <c r="I82" t="s">
+      <c r="K82" t="s">
         <v>724</v>
       </c>
-      <c r="J82" t="s">
+    </row>
+    <row r="83" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="84" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H84" s="14" t="s">
+        <v>828</v>
+      </c>
+      <c r="I84" t="s">
+        <v>832</v>
+      </c>
+      <c r="J84" t="s">
         <v>726</v>
       </c>
-      <c r="L82" t="s">
+      <c r="L84" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="83" spans="8:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H83" s="37"/>
-      <c r="I83" s="37"/>
-      <c r="J83" s="37"/>
-      <c r="K83" s="37"/>
-      <c r="L83" s="37"/>
-      <c r="M83" s="37"/>
-      <c r="N83" s="37"/>
-      <c r="O83" s="37"/>
-      <c r="P83" s="37"/>
-      <c r="Q83" s="37"/>
-      <c r="R83" s="37"/>
-      <c r="S83" s="37"/>
-      <c r="T83" s="38"/>
-      <c r="U83" s="37"/>
-    </row>
-    <row r="84" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
-      <c r="Q84" s="4"/>
-      <c r="R84" s="4"/>
-    </row>
-    <row r="85" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H85" t="s">
+      <c r="R84">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="85" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H85" s="14" t="s">
+        <v>722</v>
+      </c>
+      <c r="I85" t="s">
+        <v>724</v>
+      </c>
+      <c r="J85" t="s">
+        <v>726</v>
+      </c>
+      <c r="L85" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="86" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
+      <c r="M86" s="37"/>
+      <c r="N86" s="37"/>
+      <c r="O86" s="37"/>
+      <c r="P86" s="37"/>
+      <c r="Q86" s="37"/>
+      <c r="R86" s="37"/>
+      <c r="S86" s="37"/>
+      <c r="T86" s="38"/>
+      <c r="U86" s="37"/>
+    </row>
+    <row r="87" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="4"/>
+    </row>
+    <row r="88" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C88" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H88" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="86" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H86" t="s">
+    <row r="89" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C89" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H89" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="88" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H88" s="5" t="s">
+    <row r="91" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H91" s="5" t="s">
         <v>729</v>
       </c>
-      <c r="J88" t="s">
+      <c r="J91" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="89" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H89" t="s">
+    <row r="92" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C92" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H92" t="s">
         <v>751</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I92" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="90" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H90" s="23" t="s">
+    <row r="93" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H93" s="23" t="s">
         <v>989</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I93" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="91" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H91" s="23" t="s">
+    <row r="94" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H94" s="23" t="s">
         <v>990</v>
       </c>
-      <c r="K91" t="s">
+      <c r="K94" t="s">
         <v>1002</v>
       </c>
     </row>
-    <row r="92" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H92" s="23" t="s">
+    <row r="95" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H95" s="23" t="s">
         <v>991</v>
       </c>
-      <c r="J92" t="s">
+      <c r="J95" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="93" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H93" t="s">
+    <row r="96" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C96" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H96" t="s">
         <v>752</v>
       </c>
-      <c r="I93" s="29" t="s">
+      <c r="I96" s="29" t="s">
         <v>1005</v>
       </c>
-      <c r="J93" t="s">
+      <c r="J96" t="s">
         <v>1004</v>
       </c>
-      <c r="K93" s="16"/>
-      <c r="L93" t="s">
-        <v>1009</v>
-      </c>
-      <c r="N93" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="94" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H94" s="23" t="s">
-        <v>994</v>
-      </c>
-      <c r="K94" t="s">
-        <v>1006</v>
-      </c>
-      <c r="L94" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="95" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H95" s="23" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I95" s="29" t="s">
-        <v>1008</v>
-      </c>
-      <c r="K95" s="16"/>
-    </row>
-    <row r="96" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H96" t="s">
-        <v>753</v>
-      </c>
-      <c r="I96" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J96" t="s">
-        <v>992</v>
-      </c>
+      <c r="K96" s="16"/>
       <c r="L96" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N96" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="97" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H97" s="23" t="s">
+        <v>994</v>
+      </c>
+      <c r="K97" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L97" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="98" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H98" s="23" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I98" s="29" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K98" s="16"/>
+    </row>
+    <row r="99" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C99" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H99" t="s">
+        <v>753</v>
+      </c>
+      <c r="I99" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J99" t="s">
+        <v>992</v>
+      </c>
+      <c r="L99" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="100" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H100" s="23" t="s">
         <v>990</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K100" t="s">
         <v>1010</v>
       </c>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H98" t="s">
+    <row r="101" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
         <v>754</v>
       </c>
-      <c r="J98" t="s">
+      <c r="J101" t="s">
         <v>1012</v>
       </c>
-      <c r="L98" t="s">
+      <c r="L101" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H99" s="23" t="s">
+    <row r="102" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H102" s="23" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H100" t="s">
+    <row r="103" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C103" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H103" t="s">
         <v>755</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I103" t="s">
         <v>1015</v>
       </c>
-      <c r="L100" t="s">
+      <c r="L103" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H101" s="23" t="s">
+    <row r="104" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H104" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I104" t="s">
         <v>1014</v>
-      </c>
-      <c r="L101" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H102" t="s">
-        <v>756</v>
-      </c>
-      <c r="I102" t="s">
-        <v>1016</v>
-      </c>
-      <c r="N102" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H103" s="23" t="s">
-        <v>995</v>
-      </c>
-      <c r="K103" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H104" t="s">
-        <v>757</v>
-      </c>
-      <c r="I104" t="s">
-        <v>1020</v>
       </c>
       <c r="L104" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H105" s="23" t="s">
+    <row r="105" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C105" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H105" t="s">
+        <v>756</v>
+      </c>
+      <c r="I105" t="s">
+        <v>1016</v>
+      </c>
+      <c r="N105" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="106" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H106" s="23" t="s">
         <v>995</v>
       </c>
-      <c r="K105" t="s">
+      <c r="K106" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="107" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C107" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H107" t="s">
+        <v>757</v>
+      </c>
+      <c r="I107" t="s">
+        <v>1020</v>
+      </c>
+      <c r="L107" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="108" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H108" s="23" t="s">
+        <v>995</v>
+      </c>
+      <c r="K108" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H106" t="s">
+    <row r="109" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C109" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H109" t="s">
         <v>758</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I109" t="s">
         <v>1022</v>
       </c>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H107" t="s">
+    <row r="110" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C110" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H110" t="s">
         <v>759</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I110" t="s">
         <v>997</v>
       </c>
-      <c r="J107" t="s">
+      <c r="J110" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H108" t="s">
+    <row r="111" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C111" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H111" t="s">
         <v>760</v>
       </c>
-      <c r="I108" t="s">
+      <c r="I111" t="s">
         <v>998</v>
       </c>
     </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H110" s="5" t="s">
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H113" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="J110" t="s">
+      <c r="J113" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B111" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H111" t="s">
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B114" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C114" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H114" t="s">
         <v>761</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I114" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B112" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H112" t="s">
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B115" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C115" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H115" t="s">
         <v>762</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I115" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B113" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H113" t="s">
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B116" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C116" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H116" t="s">
         <v>763</v>
       </c>
-      <c r="I113" t="s">
+      <c r="I116" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B114" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H114" t="s">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B117" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C117" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H117" t="s">
         <v>764</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I117" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H115" t="s">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B118" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C118" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H118" t="s">
         <v>765</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I118" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H116" t="s">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B119" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C119" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H119" t="s">
         <v>766</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I119" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B117" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H117" t="s">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B120" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C120" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H120" t="s">
         <v>767</v>
       </c>
-      <c r="I117" s="7" t="s">
+      <c r="I120" s="7" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B118" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H118" t="s">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B121" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C121" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H121" t="s">
         <v>768</v>
       </c>
-      <c r="I118" t="s">
+      <c r="I121" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B119" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H119" t="s">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B122" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C122" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H122" t="s">
         <v>769</v>
       </c>
-      <c r="I119" t="s">
+      <c r="I122" t="s">
         <v>1032</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B120" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H120" t="s">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B123" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C123" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H123" t="s">
         <v>770</v>
       </c>
-      <c r="I120" t="s">
+      <c r="I123" t="s">
         <v>1033</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B121" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H121" t="s">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B124" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C124" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H124" t="s">
         <v>771</v>
       </c>
-      <c r="I121" t="s">
+      <c r="I124" t="s">
         <v>1034</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B122" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H122" t="s">
+    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C125" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H125" t="s">
         <v>772</v>
       </c>
-      <c r="I122" t="s">
+      <c r="I125" t="s">
         <v>1035</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B123" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H123" t="s">
+    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C126" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H126" t="s">
         <v>773</v>
       </c>
-      <c r="I123" t="s">
+      <c r="I126" t="s">
         <v>1036</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B124" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H124" t="s">
+    <row r="127" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B127" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C127" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H127" t="s">
         <v>774</v>
       </c>
-      <c r="I124" t="s">
+      <c r="I127" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H125" t="s">
+    <row r="128" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B128" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C128" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H128" t="s">
         <v>775</v>
       </c>
-      <c r="I125" t="s">
+      <c r="I128" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B126" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H126" t="s">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B129" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C129" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H129" t="s">
         <v>776</v>
       </c>
-      <c r="I126" t="s">
+      <c r="I129" t="s">
         <v>1039</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B127" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H127" t="s">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B130" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C130" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H130" t="s">
         <v>777</v>
       </c>
-      <c r="I127" t="s">
+      <c r="I130" t="s">
         <v>1040</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B128" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H128" t="s">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B131" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C131" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H131" t="s">
         <v>778</v>
       </c>
-      <c r="I128" t="s">
+      <c r="I131" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="129" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B129" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H129" t="s">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C132" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H132" t="s">
         <v>779</v>
       </c>
-      <c r="I129" t="s">
+      <c r="I132" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="130" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B130" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H130" t="s">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B133" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C133" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H133" t="s">
         <v>780</v>
       </c>
-      <c r="I130" t="s">
+      <c r="I133" t="s">
         <v>1043</v>
       </c>
     </row>
-    <row r="131" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B131" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H131" t="s">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B134" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C134" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H134" t="s">
         <v>781</v>
       </c>
-      <c r="I131" t="s">
+      <c r="I134" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="132" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B132" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H132" t="s">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B135" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C135" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H135" t="s">
         <v>782</v>
       </c>
-      <c r="I132" t="s">
+      <c r="I135" t="s">
         <v>1045</v>
       </c>
     </row>
-    <row r="133" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B133" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H133" t="s">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B136" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C136" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H136" t="s">
         <v>783</v>
       </c>
-      <c r="I133" t="s">
+      <c r="I136" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="134" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B134" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H134" t="s">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B137" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C137" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H137" t="s">
         <v>784</v>
       </c>
-      <c r="I134" t="s">
+      <c r="I137" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="135" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B135" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H135" t="s">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B138" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C138" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H138" t="s">
         <v>785</v>
       </c>
-      <c r="I135" t="s">
+      <c r="I138" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="136" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B136" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H136" t="s">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C139" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H139" t="s">
         <v>786</v>
       </c>
-      <c r="I136" t="s">
+      <c r="I139" t="s">
         <v>1049</v>
       </c>
     </row>
-    <row r="137" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B137" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H137" t="s">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C140" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H140" t="s">
         <v>787</v>
       </c>
-      <c r="I137" t="s">
+      <c r="I140" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="138" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B138" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H138" t="s">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B141" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C141" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H141" t="s">
         <v>788</v>
       </c>
-      <c r="I138" t="s">
+      <c r="I141" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="139" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B139" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H139" t="s">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C142" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H142" t="s">
         <v>789</v>
       </c>
-      <c r="I139" t="s">
+      <c r="I142" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="140" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B140" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H140" t="s">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B143" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C143" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H143" t="s">
         <v>790</v>
       </c>
-      <c r="I140" t="s">
+      <c r="I143" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="141" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B141" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H141" t="s">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B144" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C144" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H144" t="s">
         <v>791</v>
       </c>
-      <c r="I141" t="s">
+      <c r="I144" t="s">
         <v>1054</v>
       </c>
     </row>
-    <row r="142" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B142" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H142" t="s">
+    <row r="145" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B145" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C145" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H145" t="s">
         <v>792</v>
       </c>
-      <c r="I142" t="s">
+      <c r="I145" t="s">
         <v>1055</v>
       </c>
     </row>
-    <row r="143" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B143" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H143" t="s">
+    <row r="146" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B146" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C146" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H146" t="s">
         <v>793</v>
       </c>
-      <c r="I143" t="s">
+      <c r="I146" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="144" spans="2:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H144" s="35"/>
-      <c r="I144" s="35"/>
-      <c r="J144" s="35"/>
-      <c r="K144" s="35"/>
-      <c r="L144" s="35"/>
-      <c r="M144" s="35"/>
-      <c r="N144" s="35"/>
-      <c r="O144" s="35"/>
-      <c r="P144" s="35"/>
-      <c r="Q144" s="35"/>
-      <c r="R144" s="35"/>
-      <c r="S144" s="35"/>
-      <c r="T144" s="36"/>
-      <c r="U144" s="35"/>
-    </row>
-    <row r="145" spans="8:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H145" s="37"/>
-      <c r="I145" s="37"/>
-      <c r="J145" s="37"/>
-      <c r="K145" s="37"/>
-      <c r="L145" s="37"/>
-      <c r="M145" s="37"/>
-      <c r="N145" s="37"/>
-      <c r="O145" s="37"/>
-      <c r="P145" s="37"/>
-      <c r="Q145" s="37"/>
-      <c r="R145" s="37"/>
-      <c r="S145" s="37"/>
-      <c r="T145" s="38"/>
-      <c r="U145" s="37"/>
+    <row r="147" spans="2:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H147" s="35"/>
+      <c r="I147" s="35"/>
+      <c r="J147" s="35"/>
+      <c r="K147" s="35"/>
+      <c r="L147" s="35"/>
+      <c r="M147" s="35"/>
+      <c r="N147" s="35"/>
+      <c r="O147" s="35"/>
+      <c r="P147" s="35"/>
+      <c r="Q147" s="35"/>
+      <c r="R147" s="35"/>
+      <c r="S147" s="35"/>
+      <c r="T147" s="36"/>
+      <c r="U147" s="35"/>
+    </row>
+    <row r="148" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H148" s="37"/>
+      <c r="I148" s="37"/>
+      <c r="J148" s="37"/>
+      <c r="K148" s="37"/>
+      <c r="L148" s="37"/>
+      <c r="M148" s="37"/>
+      <c r="N148" s="37"/>
+      <c r="O148" s="37"/>
+      <c r="P148" s="37"/>
+      <c r="Q148" s="37"/>
+      <c r="R148" s="37"/>
+      <c r="S148" s="37"/>
+      <c r="T148" s="38"/>
+      <c r="U148" s="37"/>
+    </row>
+    <row r="150" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C150" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H150" t="s">
+        <v>2295</v>
+      </c>
+      <c r="I150" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="151" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C151" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H151" t="s">
+        <v>2296</v>
+      </c>
+      <c r="I151" t="s">
+        <v>2300</v>
+      </c>
+      <c r="N151" t="s">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="152" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C152" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H152" t="s">
+        <v>2297</v>
+      </c>
+      <c r="I152" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="153" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C153" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H153" t="s">
+        <v>2298</v>
+      </c>
+      <c r="I153" t="s">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="154" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H154" t="s">
+        <v>2299</v>
+      </c>
+      <c r="I154" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="157" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C157" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H157" t="s">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="158" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C158" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H158" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="159" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C159" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H159" t="s">
+        <v>2308</v>
+      </c>
+    </row>
+    <row r="160" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C160" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H160" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="161" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C161" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H161" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="162" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H162" t="s">
+        <v>2311</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding in random links from open tabs
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="-345" windowWidth="19755" windowHeight="10155" tabRatio="810" activeTab="8"/>
-    <workbookView xWindow="10905" yWindow="-30" windowWidth="11040" windowHeight="9780" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="450" yWindow="-345" windowWidth="15255" windowHeight="10155" tabRatio="810" activeTab="2"/>
+    <workbookView xWindow="10905" yWindow="-30" windowWidth="6150" windowHeight="9780" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5395" uniqueCount="2313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5476" uniqueCount="2374">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -5746,18 +5746,12 @@
     <t>http://web.worldbank.org/WBSITE/EXTERNAL/PROJECTS/EXTPOLICIES/EXTOPMANUAL/0,,contentMDK:21304797~menuPK:51508119~pagePK:64141683~piPK:4688102~theSitePK:502184,00.html</t>
   </si>
   <si>
-    <t>http://web.worldbank.org/WBSITE/EXTERNAL/PROJECTS/0,,contentMDK:20120722~hlPK:581478~menuPK:41392~pagePK:41367~piPK:51533~theSitePK:40941,00.html</t>
-  </si>
-  <si>
     <t>Policies &amp; Procedures</t>
   </si>
   <si>
     <t>Guidebooks/Sourcebooks</t>
   </si>
   <si>
-    <t>http://web.worldbank.org/WBSITE/EXTERNAL/PROJECTS/EXTPOLICIES/EXTSAFEPOL/0,,contentMDK:20583835~menuPK:1430924~pagePK:64168445~piPK:64168309~theSitePK:584435,00.html</t>
-  </si>
-  <si>
     <t>http://web.worldbank.org/WBSITE/EXTERNAL/PROJECTS/EXTPOLICIES/EXTOPMANUAL/0,,contentMDK:20064622~menuPK:51508119~pagePK:64141683~piPK:4688102~theSitePK:502184,00.html</t>
   </si>
   <si>
@@ -6965,6 +6959,195 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Proposed Adoption and Application of World Bank Performance Standards for Private Sector Projects Supported by IBRD/IDA (English)</t>
+  </si>
+  <si>
+    <t>http://www-wds.worldbank.org/external/default/WDSContentServer/WDSP/IB/2012/06/06/000406484_20120606112612/Rendered/PDF/695590BR0R201200606020120Box369278B.pdf</t>
+  </si>
+  <si>
+    <t>Safeguards</t>
+  </si>
+  <si>
+    <t>http://go.worldbank.org/2YCB0ORXU0</t>
+  </si>
+  <si>
+    <t>http://go.worldbank.org/K37F0RJ2B0</t>
+  </si>
+  <si>
+    <t>http://go.worldbank.org/5SQNJ7AF70</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Biofuels Sustainability Scorecard</t>
+  </si>
+  <si>
+    <t>Tourism Sustainability Scorecard for Private Sector Projects</t>
+  </si>
+  <si>
+    <t>Guidelines</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/biofuelsscorecard/</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/tourismscorecard/index.cfm?lang=en</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=35601768</t>
+  </si>
+  <si>
+    <t>http://www.iadb.org/document.cfm?id=35596985</t>
+  </si>
+  <si>
+    <t>OPIC Policies</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies</t>
+  </si>
+  <si>
+    <t>Economic Analysis</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/economic-analysis</t>
+  </si>
+  <si>
+    <t>Project Monitoring</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/project-monitoring</t>
+  </si>
+  <si>
+    <t>The Environment</t>
+  </si>
+  <si>
+    <t>Environmental and Social Policies</t>
+  </si>
+  <si>
+    <t>Final Environmental and Social Policy Statement (October 15 2010)</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/environment/documents</t>
+  </si>
+  <si>
+    <t>Environmental and Social Projects Documents</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/greenhouse-gas-accounting-reports</t>
+  </si>
+  <si>
+    <t>Greenhouse Gas Accounting Reports</t>
+  </si>
+  <si>
+    <t>Renewable Energy Guidelines</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/renewable-guidelines</t>
+  </si>
+  <si>
+    <t>Wind Energy Guidelines</t>
+  </si>
+  <si>
+    <t>Biofuels Guidelines</t>
+  </si>
+  <si>
+    <t>Geothermal Energy Guidelines</t>
+  </si>
+  <si>
+    <t>Hydroelectric Energy Guidelines</t>
+  </si>
+  <si>
+    <t>Solar Energy Guidelines</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/files/Wind-Jan31-to-OPIC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/files/Biofuels-Guidance-Notes.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/files/Geothermal-Jan31-to-OPIC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/files/hydro-guidance-note.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/files/Solar-Jan31-to-OPIC.pdf</t>
+  </si>
+  <si>
+    <t>Archived Documents</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/archived-documents</t>
+  </si>
+  <si>
+    <t>2004 OPIC Environmental Handbook</t>
+  </si>
+  <si>
+    <t>1999 OPIC Environmental Handbook</t>
+  </si>
+  <si>
+    <t>OPIC's Transparency Initiative</t>
+  </si>
+  <si>
+    <t>OPIC's Greenhouse Gas/Clean Energy Initiative Fact Sheet</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/docs/notices/2004_Environmental_Handbook.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/docs/notices/1999_Environmental_Handbook.pdf</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/who-we-are/transparency</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/sites/default/files/docs/ghg_fact-sheet_070109.pdf</t>
+  </si>
+  <si>
+    <t>Worker &amp; Human Rights</t>
+  </si>
+  <si>
+    <t>https://www.opic.gov/doing-business-us/OPIC-policies/worker-human-rights</t>
+  </si>
+  <si>
+    <t>http://www.worldbank.org/en/about/leadership</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Socially responsible investments</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395239037269&amp;pagename=EBRD%2FContent%2FContentLayout</t>
+  </si>
+  <si>
+    <t>Development banks agree common approach to measure climate finance</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/2015/development-banks-agree-common-approach-to-measure-climate-finance.html</t>
+  </si>
+  <si>
+    <t>EBRD enhances openness by publishing data via IATI</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/news/2015/ebrd-enhances-openness-by-publishing-data-via-iati.html</t>
+  </si>
+  <si>
+    <t>Environmental and Social Policy (ESP)</t>
+  </si>
+  <si>
+    <t>Other Operational Policies and Strategies</t>
+  </si>
+  <si>
+    <t>http://www.adb.org/about/other-operational-policies-and-strategies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving Project Outcomes </t>
   </si>
 </sst>
 </file>
@@ -7548,11 +7731,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X141"/>
+  <dimension ref="A2:X146"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9:Q9"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K146" sqref="K146"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -7668,10 +7851,10 @@
         <v>552</v>
       </c>
       <c r="P9" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q9" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R9" s="21" t="s">
         <v>1308</v>
@@ -10970,6 +11153,22 @@
     <row r="141" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T141" s="33"/>
     </row>
+    <row r="145" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>2371</v>
+      </c>
+      <c r="J145" t="s">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="146" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>2373</v>
+      </c>
+      <c r="K146" t="s">
+        <v>1178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10978,10 +11177,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V16"/>
+  <dimension ref="A2:V21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -11162,6 +11361,38 @@
       </c>
       <c r="K16" t="s">
         <v>1091</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>2364</v>
+      </c>
+      <c r="J17" t="s">
+        <v>2365</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>2366</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>2368</v>
+      </c>
+      <c r="J19" t="s">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>2370</v>
+      </c>
+      <c r="J21" t="s">
+        <v>711</v>
       </c>
     </row>
   </sheetData>
@@ -11372,14 +11603,17 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V9"/>
+  <dimension ref="A2:V41"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="T2" s="25"/>
@@ -11494,6 +11728,190 @@
       </c>
       <c r="V9" s="4" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J13" t="s">
+        <v>2330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J14" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>2332</v>
+      </c>
+      <c r="J15" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>2333</v>
+      </c>
+      <c r="K16" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>836</v>
+      </c>
+      <c r="K17" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>837</v>
+      </c>
+      <c r="K18" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>2335</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J22" t="s">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>2338</v>
+      </c>
+      <c r="J23" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>2340</v>
+      </c>
+      <c r="K25" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>2341</v>
+      </c>
+      <c r="K26" t="s">
+        <v>2346</v>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>2342</v>
+      </c>
+      <c r="K27" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>2343</v>
+      </c>
+      <c r="K28" t="s">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>2344</v>
+      </c>
+      <c r="K29" t="s">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="31" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>2350</v>
+      </c>
+      <c r="J31" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>2352</v>
+      </c>
+      <c r="K33" t="s">
+        <v>2356</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>2353</v>
+      </c>
+      <c r="K34" t="s">
+        <v>2357</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>2354</v>
+      </c>
+      <c r="K35" t="s">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>2355</v>
+      </c>
+      <c r="K36" t="s">
+        <v>2359</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>2360</v>
+      </c>
+      <c r="J39" t="s">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="41" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J41" t="s">
+        <v>2328</v>
       </c>
     </row>
   </sheetData>
@@ -11505,7 +11923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N8" sqref="N8:Q8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
@@ -11616,10 +12034,10 @@
         <v>552</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R8" s="21" t="s">
         <v>1308</v>
@@ -11938,8 +12356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD624"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:Q10"/>
+    <sheetView tabSelected="1" topLeftCell="H58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -12087,10 +12505,10 @@
         <v>552</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q10" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R10" s="21" t="s">
         <v>1314</v>
@@ -12817,6 +13235,15 @@
       <c r="L37" t="s">
         <v>1272</v>
       </c>
+      <c r="R37">
+        <v>1998</v>
+      </c>
+      <c r="U37" s="22">
+        <v>36130</v>
+      </c>
+      <c r="V37" s="22">
+        <v>38200</v>
+      </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -15306,10 +15733,10 @@
         <v>1166</v>
       </c>
       <c r="D191" t="s">
-        <v>2238</v>
+        <v>2236</v>
       </c>
       <c r="F191" s="45" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
       <c r="G191" s="2">
         <v>41878</v>
@@ -15332,10 +15759,10 @@
         <v>1166</v>
       </c>
       <c r="D192" t="s">
-        <v>2240</v>
+        <v>2238</v>
       </c>
       <c r="F192" s="45" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
       <c r="G192" s="2">
         <v>41878</v>
@@ -15358,10 +15785,10 @@
         <v>1166</v>
       </c>
       <c r="D193" t="s">
-        <v>2239</v>
+        <v>2237</v>
       </c>
       <c r="F193" s="45" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="G193" s="2">
         <v>41878</v>
@@ -15989,10 +16416,10 @@
         <v>1166</v>
       </c>
       <c r="D216" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
       <c r="F216" s="45" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
       <c r="G216" s="2">
         <v>41729</v>
@@ -16293,7 +16720,7 @@
         <v>1166</v>
       </c>
       <c r="D227" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="F227" s="45">
         <v>13</v>
@@ -16322,7 +16749,7 @@
         <v>1166</v>
       </c>
       <c r="D228" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="F228" s="45">
         <v>6</v>
@@ -16348,7 +16775,7 @@
         <v>1166</v>
       </c>
       <c r="D229" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="F229" s="45">
         <v>6</v>
@@ -16374,10 +16801,10 @@
         <v>1166</v>
       </c>
       <c r="D230" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F230" s="45" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="G230" s="2">
         <v>41372</v>
@@ -16458,7 +16885,7 @@
         <v>1166</v>
       </c>
       <c r="D233" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F233" s="45">
         <v>13.2</v>
@@ -16484,7 +16911,7 @@
         <v>1166</v>
       </c>
       <c r="D234" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F234" s="45">
         <v>13.2</v>
@@ -16513,7 +16940,7 @@
         <v>1166</v>
       </c>
       <c r="D235" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="F235" s="45">
         <v>6</v>
@@ -16539,7 +16966,7 @@
         <v>1166</v>
       </c>
       <c r="D236" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="F236" s="45">
         <v>6</v>
@@ -16565,10 +16992,10 @@
         <v>1166</v>
       </c>
       <c r="D237" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F237" s="45" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="G237" s="2">
         <v>41372</v>
@@ -16594,7 +17021,7 @@
         <v>1166</v>
       </c>
       <c r="D238" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F238" s="45">
         <v>13.2</v>
@@ -16620,7 +17047,7 @@
         <v>1166</v>
       </c>
       <c r="D239" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F239" s="45">
         <v>13.2</v>
@@ -16704,7 +17131,7 @@
         <v>1166</v>
       </c>
       <c r="D242" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F242" s="45">
         <v>13.2</v>
@@ -16730,7 +17157,7 @@
         <v>1166</v>
       </c>
       <c r="D243" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
       <c r="F243" s="45">
         <v>13.2</v>
@@ -16811,10 +17238,10 @@
         <v>1166</v>
       </c>
       <c r="D246" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F246" s="45" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="G246" s="2">
         <v>41372</v>
@@ -16840,7 +17267,7 @@
         <v>1166</v>
       </c>
       <c r="D247" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="F247" s="45">
         <v>6</v>
@@ -16866,10 +17293,10 @@
         <v>1166</v>
       </c>
       <c r="D248" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F248" s="45" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="G248" s="2">
         <v>41372</v>
@@ -16892,7 +17319,7 @@
         <v>1166</v>
       </c>
       <c r="D249" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="F249" s="45">
         <v>8.4</v>
@@ -16918,10 +17345,10 @@
         <v>1166</v>
       </c>
       <c r="D250" t="s">
-        <v>2261</v>
+        <v>2259</v>
       </c>
       <c r="F250" s="45" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="G250" s="2">
         <v>41372</v>
@@ -16947,7 +17374,7 @@
         <v>1166</v>
       </c>
       <c r="D251" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="F251" s="45">
         <v>13.55</v>
@@ -16976,7 +17403,7 @@
         <v>1166</v>
       </c>
       <c r="D252" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="F252" s="45">
         <v>13.4</v>
@@ -17005,7 +17432,7 @@
         <v>1166</v>
       </c>
       <c r="D253" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="F253" s="45">
         <v>13.3</v>
@@ -17034,7 +17461,7 @@
         <v>1166</v>
       </c>
       <c r="D254" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="F254" s="45">
         <v>13.25</v>
@@ -17060,7 +17487,7 @@
         <v>1166</v>
       </c>
       <c r="D255" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="F255" s="45">
         <v>13.55</v>
@@ -17086,7 +17513,7 @@
         <v>1166</v>
       </c>
       <c r="D256" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="F256" s="45">
         <v>13.5</v>
@@ -17112,10 +17539,10 @@
         <v>1166</v>
       </c>
       <c r="D257" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
       <c r="F257" s="45" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
       <c r="G257" s="2">
         <v>41372</v>
@@ -17138,10 +17565,10 @@
         <v>1166</v>
       </c>
       <c r="D258" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="F258" s="45" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
       <c r="G258" s="2">
         <v>41372</v>
@@ -17164,10 +17591,10 @@
         <v>1166</v>
       </c>
       <c r="D259" t="s">
-        <v>2218</v>
+        <v>2216</v>
       </c>
       <c r="F259" s="45" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="G259" s="2">
         <v>41372</v>
@@ -17190,10 +17617,10 @@
         <v>1166</v>
       </c>
       <c r="D260" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="F260" s="45" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="G260" s="2">
         <v>41372</v>
@@ -17216,10 +17643,10 @@
         <v>1166</v>
       </c>
       <c r="D261" t="s">
-        <v>2216</v>
+        <v>2214</v>
       </c>
       <c r="F261" s="45" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="G261" s="2">
         <v>41372</v>
@@ -17242,10 +17669,10 @@
         <v>1166</v>
       </c>
       <c r="D262" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="F262" s="45" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
       <c r="G262" s="2">
         <v>41372</v>
@@ -17268,10 +17695,10 @@
         <v>1166</v>
       </c>
       <c r="D263" t="s">
-        <v>2214</v>
+        <v>2212</v>
       </c>
       <c r="F263" s="45" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="G263" s="2">
         <v>41372</v>
@@ -17294,10 +17721,10 @@
         <v>1166</v>
       </c>
       <c r="D264" t="s">
-        <v>2213</v>
+        <v>2211</v>
       </c>
       <c r="F264" s="45" t="s">
-        <v>2116</v>
+        <v>2114</v>
       </c>
       <c r="G264" s="2">
         <v>41372</v>
@@ -17320,10 +17747,10 @@
         <v>1166</v>
       </c>
       <c r="D265" t="s">
-        <v>2212</v>
+        <v>2210</v>
       </c>
       <c r="F265" s="45" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="G265" s="2">
         <v>41372</v>
@@ -17346,10 +17773,10 @@
         <v>1166</v>
       </c>
       <c r="D266" t="s">
-        <v>2211</v>
+        <v>2209</v>
       </c>
       <c r="F266" s="45" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="G266" s="2">
         <v>41372</v>
@@ -17372,10 +17799,10 @@
         <v>1166</v>
       </c>
       <c r="D267" t="s">
-        <v>2210</v>
+        <v>2208</v>
       </c>
       <c r="F267" s="45" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
       <c r="G267" s="2">
         <v>41372</v>
@@ -17398,7 +17825,7 @@
         <v>1166</v>
       </c>
       <c r="D268" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="F268" s="45">
         <v>13.4</v>
@@ -17424,7 +17851,7 @@
         <v>1166</v>
       </c>
       <c r="D269" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="F269" s="45">
         <v>13.3</v>
@@ -17450,7 +17877,7 @@
         <v>1166</v>
       </c>
       <c r="D270" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="F270" s="45">
         <v>13.25</v>
@@ -17479,7 +17906,7 @@
         <v>1166</v>
       </c>
       <c r="D271" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F271" s="45">
         <v>13.2</v>
@@ -17505,7 +17932,7 @@
         <v>1166</v>
       </c>
       <c r="D272" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F272" s="45">
         <v>13.2</v>
@@ -17534,7 +17961,7 @@
         <v>1166</v>
       </c>
       <c r="D273" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="F273" s="45">
         <v>13.05</v>
@@ -17563,7 +17990,7 @@
         <v>1166</v>
       </c>
       <c r="D274" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="F274" s="45">
         <v>13</v>
@@ -17589,7 +18016,7 @@
         <v>1166</v>
       </c>
       <c r="D275" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="F275" s="45">
         <v>13.05</v>
@@ -17618,7 +18045,7 @@
         <v>1166</v>
       </c>
       <c r="D276" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="F276" s="45">
         <v>12</v>
@@ -17644,10 +18071,10 @@
         <v>1166</v>
       </c>
       <c r="D277" t="s">
-        <v>2204</v>
+        <v>2202</v>
       </c>
       <c r="F277" s="45" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="G277" s="2">
         <v>41372</v>
@@ -17670,7 +18097,7 @@
         <v>1166</v>
       </c>
       <c r="D278" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="F278" s="45">
         <v>12</v>
@@ -17699,7 +18126,7 @@
         <v>1166</v>
       </c>
       <c r="D279" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="F279" s="45">
         <v>10.039999999999999</v>
@@ -17728,7 +18155,7 @@
         <v>1166</v>
       </c>
       <c r="D280" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="F280" s="45">
         <v>10.02</v>
@@ -17754,7 +18181,7 @@
         <v>1166</v>
       </c>
       <c r="D281" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="F281" s="45">
         <v>10.039999999999999</v>
@@ -17780,7 +18207,7 @@
         <v>1166</v>
       </c>
       <c r="D282" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="F282" s="45">
         <v>10.02</v>
@@ -17806,7 +18233,7 @@
         <v>1166</v>
       </c>
       <c r="D283" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="F283" s="45">
         <v>8.3000000000000007</v>
@@ -17835,7 +18262,7 @@
         <v>1166</v>
       </c>
       <c r="D284" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="F284" s="45">
         <v>8.3000000000000007</v>
@@ -17864,7 +18291,7 @@
         <v>1166</v>
       </c>
       <c r="D285" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F285" s="45">
         <v>8.1</v>
@@ -17890,7 +18317,7 @@
         <v>1166</v>
       </c>
       <c r="D286" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="F286" s="45">
         <v>8.1</v>
@@ -17916,7 +18343,7 @@
         <v>1166</v>
       </c>
       <c r="D287" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="F287" s="45">
         <v>8</v>
@@ -17945,7 +18372,7 @@
         <v>1166</v>
       </c>
       <c r="D288" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="F288" s="45">
         <v>6</v>
@@ -17971,7 +18398,7 @@
         <v>1166</v>
       </c>
       <c r="D289" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="F289" s="45">
         <v>6</v>
@@ -17997,10 +18424,10 @@
         <v>1166</v>
       </c>
       <c r="D290" t="s">
-        <v>2203</v>
+        <v>2201</v>
       </c>
       <c r="F290" s="45" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="G290" s="2">
         <v>41372</v>
@@ -18023,10 +18450,10 @@
         <v>1166</v>
       </c>
       <c r="D291" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="F291" s="45" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="G291" s="2">
         <v>41372</v>
@@ -18049,10 +18476,10 @@
         <v>1166</v>
       </c>
       <c r="D292" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="F292" s="45" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="G292" s="2">
         <v>41372</v>
@@ -18075,10 +18502,10 @@
         <v>1166</v>
       </c>
       <c r="D293" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="F293" s="45" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
       <c r="G293" s="2">
         <v>41372</v>
@@ -18101,10 +18528,10 @@
         <v>1166</v>
       </c>
       <c r="D294" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="F294" s="45" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
       <c r="G294" s="2">
         <v>41372</v>
@@ -18127,10 +18554,10 @@
         <v>1166</v>
       </c>
       <c r="D295" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
       <c r="F295" s="45" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="G295" s="2">
         <v>41372</v>
@@ -18153,10 +18580,10 @@
         <v>1166</v>
       </c>
       <c r="D296" t="s">
-        <v>2197</v>
+        <v>2195</v>
       </c>
       <c r="F296" s="45" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="G296" s="2">
         <v>41372</v>
@@ -18179,10 +18606,10 @@
         <v>1166</v>
       </c>
       <c r="D297" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="F297" s="45" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
       <c r="G297" s="2">
         <v>41372</v>
@@ -18205,10 +18632,10 @@
         <v>1166</v>
       </c>
       <c r="D298" t="s">
-        <v>2195</v>
+        <v>2193</v>
       </c>
       <c r="F298" s="45" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
       <c r="G298" s="2">
         <v>41372</v>
@@ -18231,10 +18658,10 @@
         <v>1166</v>
       </c>
       <c r="D299" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
       <c r="F299" s="45" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
       <c r="G299" s="2">
         <v>41372</v>
@@ -18257,10 +18684,10 @@
         <v>1166</v>
       </c>
       <c r="D300" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
       <c r="F300" s="45" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
       <c r="G300" s="2">
         <v>41372</v>
@@ -18283,10 +18710,10 @@
         <v>1166</v>
       </c>
       <c r="D301" t="s">
-        <v>2192</v>
+        <v>2190</v>
       </c>
       <c r="F301" s="45" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
       <c r="G301" s="2">
         <v>41372</v>
@@ -18309,10 +18736,10 @@
         <v>1166</v>
       </c>
       <c r="D302" t="s">
-        <v>2191</v>
+        <v>2189</v>
       </c>
       <c r="F302" s="45" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
       <c r="G302" s="2">
         <v>41372</v>
@@ -18639,7 +19066,7 @@
         <v>1166</v>
       </c>
       <c r="D314" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="F314" s="45">
         <v>13.6</v>
@@ -18969,7 +19396,7 @@
         <v>1166</v>
       </c>
       <c r="D326" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="F326" s="45">
         <v>2.2999999999999998</v>
@@ -19609,10 +20036,10 @@
         <v>1166</v>
       </c>
       <c r="D349" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="F349" s="45" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="G349" s="2">
         <v>41089</v>
@@ -19832,7 +20259,7 @@
         <v>1166</v>
       </c>
       <c r="D357" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F357" s="45">
         <v>13.2</v>
@@ -19861,7 +20288,7 @@
         <v>1166</v>
       </c>
       <c r="D358" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F358" s="45">
         <v>13.2</v>
@@ -19887,7 +20314,7 @@
         <v>1166</v>
       </c>
       <c r="D359" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="F359" s="45">
         <v>13.3</v>
@@ -19939,7 +20366,7 @@
         <v>1166</v>
       </c>
       <c r="D361" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="F361" s="45">
         <v>13.55</v>
@@ -19965,7 +20392,7 @@
         <v>1166</v>
       </c>
       <c r="D362" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="F362" s="45">
         <v>13.5</v>
@@ -19991,7 +20418,7 @@
         <v>1166</v>
       </c>
       <c r="D363" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="F363" s="45">
         <v>13</v>
@@ -20017,7 +20444,7 @@
         <v>1166</v>
       </c>
       <c r="D364" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="F364" s="45">
         <v>12</v>
@@ -20043,7 +20470,7 @@
         <v>1166</v>
       </c>
       <c r="D365" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="F365" s="45">
         <v>8.1</v>
@@ -20199,7 +20626,7 @@
         <v>1166</v>
       </c>
       <c r="D371" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="F371" s="45">
         <v>13.55</v>
@@ -20225,7 +20652,7 @@
         <v>1166</v>
       </c>
       <c r="D372" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="F372" s="45">
         <v>13.5</v>
@@ -20251,7 +20678,7 @@
         <v>1166</v>
       </c>
       <c r="D373" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="F373" s="45">
         <v>13.3</v>
@@ -20277,7 +20704,7 @@
         <v>1166</v>
       </c>
       <c r="D374" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F374" s="45">
         <v>13.2</v>
@@ -20329,7 +20756,7 @@
         <v>1166</v>
       </c>
       <c r="D376" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="F376" s="45">
         <v>13.05</v>
@@ -20355,7 +20782,7 @@
         <v>1166</v>
       </c>
       <c r="D377" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="F377" s="45">
         <v>12</v>
@@ -20407,7 +20834,7 @@
         <v>1166</v>
       </c>
       <c r="D379" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="F379" s="45">
         <v>10.02</v>
@@ -20650,7 +21077,7 @@
         <v>1166</v>
       </c>
       <c r="D388" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="F388" s="45">
         <v>13.55</v>
@@ -20679,7 +21106,7 @@
         <v>1166</v>
       </c>
       <c r="D389" t="s">
-        <v>2102</v>
+        <v>2100</v>
       </c>
       <c r="F389" s="45">
         <v>13.5</v>
@@ -20708,7 +21135,7 @@
         <v>1166</v>
       </c>
       <c r="D390" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="F390" s="45">
         <v>13.3</v>
@@ -20737,7 +21164,7 @@
         <v>1166</v>
       </c>
       <c r="D391" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="F391" s="45">
         <v>13.25</v>
@@ -20766,7 +21193,7 @@
         <v>1166</v>
       </c>
       <c r="D392" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F392" s="45">
         <v>13.2</v>
@@ -20824,7 +21251,7 @@
         <v>1166</v>
       </c>
       <c r="D394" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="F394" s="45">
         <v>13.05</v>
@@ -20853,7 +21280,7 @@
         <v>1166</v>
       </c>
       <c r="D395" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="F395" s="45">
         <v>12</v>
@@ -20911,7 +21338,7 @@
         <v>1166</v>
       </c>
       <c r="D397" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="F397" s="45">
         <v>10.02</v>
@@ -20969,7 +21396,7 @@
         <v>1166</v>
       </c>
       <c r="D399" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F399" s="45">
         <v>8.1</v>
@@ -21285,7 +21712,7 @@
         <v>1166</v>
       </c>
       <c r="D410" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F410" s="45">
         <v>13.2</v>
@@ -21427,7 +21854,7 @@
         <v>1166</v>
       </c>
       <c r="D415" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F415" s="45">
         <v>8.1</v>
@@ -21453,7 +21880,7 @@
         <v>1166</v>
       </c>
       <c r="D416" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="F416" s="45">
         <v>13</v>
@@ -21479,7 +21906,7 @@
         <v>1166</v>
       </c>
       <c r="D417" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="F417" s="45">
         <v>13.55</v>
@@ -21508,7 +21935,7 @@
         <v>1166</v>
       </c>
       <c r="D418" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="F418" s="45">
         <v>13.55</v>
@@ -21537,7 +21964,7 @@
         <v>1166</v>
       </c>
       <c r="D419" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="F419" s="45">
         <v>13</v>
@@ -21563,7 +21990,7 @@
         <v>1166</v>
       </c>
       <c r="D420" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="F420" s="45">
         <v>8.1</v>
@@ -21641,7 +22068,7 @@
         <v>1166</v>
       </c>
       <c r="D423" t="s">
-        <v>2259</v>
+        <v>2257</v>
       </c>
       <c r="F423" s="45" t="s">
         <v>1200</v>
@@ -21919,10 +22346,10 @@
         <v>1166</v>
       </c>
       <c r="D433" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F433" s="45" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="G433" s="2">
         <v>40633</v>
@@ -22165,7 +22592,7 @@
         <v>1166</v>
       </c>
       <c r="D442" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="F442" s="45">
         <v>10.02</v>
@@ -22194,7 +22621,7 @@
         <v>1166</v>
       </c>
       <c r="D443" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="F443" s="45">
         <v>10.02</v>
@@ -22220,7 +22647,7 @@
         <v>1166</v>
       </c>
       <c r="D444" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="F444" s="45">
         <v>8</v>
@@ -22249,10 +22676,10 @@
         <v>1166</v>
       </c>
       <c r="D445" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="F445" s="45" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="G445" s="2">
         <v>40360</v>
@@ -22301,10 +22728,10 @@
         <v>1166</v>
       </c>
       <c r="D447" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
       <c r="F447" s="45" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
       <c r="G447" s="2">
         <v>40233</v>
@@ -22388,7 +22815,7 @@
         <v>1166</v>
       </c>
       <c r="D450" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F450" s="45">
         <v>13.2</v>
@@ -22414,7 +22841,7 @@
         <v>1166</v>
       </c>
       <c r="D451" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F451" s="45">
         <v>13.2</v>
@@ -22443,7 +22870,7 @@
         <v>1166</v>
       </c>
       <c r="D452" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F452" s="45">
         <v>8.1</v>
@@ -22512,10 +22939,10 @@
         <v>1166</v>
       </c>
       <c r="D455" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
       <c r="F455" s="45" t="s">
-        <v>2135</v>
+        <v>2133</v>
       </c>
       <c r="G455" s="2">
         <v>40007</v>
@@ -22538,7 +22965,7 @@
         <v>1166</v>
       </c>
       <c r="D456" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="F456" s="45">
         <v>9.01</v>
@@ -22564,10 +22991,10 @@
         <v>1166</v>
       </c>
       <c r="D457" t="s">
-        <v>2274</v>
+        <v>2272</v>
       </c>
       <c r="F457" s="45" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="G457" s="2">
         <v>40007</v>
@@ -22590,10 +23017,10 @@
         <v>1166</v>
       </c>
       <c r="D458" t="s">
-        <v>2275</v>
+        <v>2273</v>
       </c>
       <c r="F458" s="45" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="G458" s="2">
         <v>40007</v>
@@ -22677,7 +23104,7 @@
         <v>1166</v>
       </c>
       <c r="D461" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F461" s="45">
         <v>8.1</v>
@@ -22703,7 +23130,7 @@
         <v>1166</v>
       </c>
       <c r="D462" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="F462" s="45">
         <v>8.1</v>
@@ -22932,10 +23359,10 @@
         <v>1166</v>
       </c>
       <c r="D470" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="F470" s="45" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="G470" s="2">
         <v>39427</v>
@@ -22958,10 +23385,10 @@
         <v>1166</v>
       </c>
       <c r="D471" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
       <c r="F471" s="45" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
       <c r="G471" s="2">
         <v>39282</v>
@@ -22984,10 +23411,10 @@
         <v>1166</v>
       </c>
       <c r="D472" t="s">
-        <v>2273</v>
+        <v>2271</v>
       </c>
       <c r="F472" s="45" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
       <c r="G472" s="2">
         <v>39282</v>
@@ -23126,10 +23553,10 @@
         <v>1166</v>
       </c>
       <c r="D477" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="F477" s="45" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="G477" s="2">
         <v>39265</v>
@@ -23152,7 +23579,7 @@
         <v>1166</v>
       </c>
       <c r="D478" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
       <c r="F478" s="45">
         <v>10.7</v>
@@ -23178,7 +23605,7 @@
         <v>1166</v>
       </c>
       <c r="D479" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
       <c r="F479" s="45">
         <v>13.6</v>
@@ -23204,10 +23631,10 @@
         <v>1166</v>
       </c>
       <c r="D480" t="s">
-        <v>2262</v>
+        <v>2260</v>
       </c>
       <c r="F480" s="45" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
       <c r="G480" s="2">
         <v>39237</v>
@@ -23288,10 +23715,10 @@
         <v>1166</v>
       </c>
       <c r="D483" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="F483" s="45" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="G483" s="2">
         <v>39191</v>
@@ -23314,7 +23741,7 @@
         <v>1166</v>
       </c>
       <c r="D484" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="F484" s="45">
         <v>6</v>
@@ -23372,7 +23799,7 @@
         <v>1166</v>
       </c>
       <c r="D486" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
       <c r="F486" s="45">
         <v>12.1</v>
@@ -23384,7 +23811,7 @@
         <v>1520</v>
       </c>
       <c r="I486" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="U486" s="2">
         <v>39190</v>
@@ -23401,7 +23828,7 @@
         <v>1166</v>
       </c>
       <c r="D487" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
       <c r="F487" s="45">
         <v>6.3</v>
@@ -23413,7 +23840,7 @@
         <v>1521</v>
       </c>
       <c r="I487" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="U487" s="2">
         <v>39190</v>
@@ -23430,7 +23857,7 @@
         <v>1166</v>
       </c>
       <c r="D488" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
       <c r="F488" s="45">
         <v>6.3</v>
@@ -23442,7 +23869,7 @@
         <v>1522</v>
       </c>
       <c r="I488" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="U488" s="2">
         <v>39190</v>
@@ -23456,7 +23883,7 @@
         <v>1166</v>
       </c>
       <c r="D489" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="F489" s="45">
         <v>6.6</v>
@@ -23468,7 +23895,7 @@
         <v>1523</v>
       </c>
       <c r="I489" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="U489" s="2">
         <v>39190</v>
@@ -23482,7 +23909,7 @@
         <v>1166</v>
       </c>
       <c r="D490" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
       <c r="F490" s="45">
         <v>6.3</v>
@@ -23494,7 +23921,7 @@
         <v>1524</v>
       </c>
       <c r="I490" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="U490" s="2">
         <v>39190</v>
@@ -23511,10 +23938,10 @@
         <v>1166</v>
       </c>
       <c r="D491" t="s">
-        <v>2281</v>
+        <v>2279</v>
       </c>
       <c r="F491" s="45" t="s">
-        <v>2141</v>
+        <v>2139</v>
       </c>
       <c r="G491" s="2">
         <v>39190</v>
@@ -23523,7 +23950,7 @@
         <v>1525</v>
       </c>
       <c r="I491" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="U491" s="2">
         <v>39190</v>
@@ -23569,7 +23996,7 @@
         <v>1166</v>
       </c>
       <c r="D493" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="F493" s="45">
         <v>13.4</v>
@@ -23581,7 +24008,7 @@
         <v>1409</v>
       </c>
       <c r="I493" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="U493" s="2">
         <v>39177</v>
@@ -23610,7 +24037,7 @@
         <v>1526</v>
       </c>
       <c r="I494" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="U494" s="2">
         <v>39177</v>
@@ -23624,10 +24051,10 @@
         <v>1166</v>
       </c>
       <c r="D495" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="F495" s="45" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="G495" s="2">
         <v>39177</v>
@@ -23636,7 +24063,7 @@
         <v>1527</v>
       </c>
       <c r="I495" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="U495" s="2">
         <v>39177</v>
@@ -23650,10 +24077,10 @@
         <v>1166</v>
       </c>
       <c r="D496" t="s">
-        <v>2216</v>
+        <v>2214</v>
       </c>
       <c r="F496" s="45" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="G496" s="2">
         <v>39177</v>
@@ -23662,7 +24089,7 @@
         <v>1418</v>
       </c>
       <c r="I496" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="U496" s="2">
         <v>39177</v>
@@ -23679,7 +24106,7 @@
         <v>1166</v>
       </c>
       <c r="D497" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F497" s="45">
         <v>8.1</v>
@@ -23691,7 +24118,7 @@
         <v>1528</v>
       </c>
       <c r="I497" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="U497" s="2">
         <v>39177</v>
@@ -23705,10 +24132,10 @@
         <v>1166</v>
       </c>
       <c r="D498" t="s">
-        <v>2218</v>
+        <v>2216</v>
       </c>
       <c r="F498" s="45" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="G498" s="2">
         <v>39177</v>
@@ -23731,7 +24158,7 @@
         <v>1166</v>
       </c>
       <c r="D499" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="F499" s="45">
         <v>13.4</v>
@@ -23743,7 +24170,7 @@
         <v>1425</v>
       </c>
       <c r="I499" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="U499" s="2">
         <v>39177</v>
@@ -23760,7 +24187,7 @@
         <v>1166</v>
       </c>
       <c r="D500" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="F500" s="45">
         <v>13.25</v>
@@ -23772,7 +24199,7 @@
         <v>1529</v>
       </c>
       <c r="I500" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="U500" s="2">
         <v>39177</v>
@@ -23786,10 +24213,10 @@
         <v>1166</v>
       </c>
       <c r="D501" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="F501" s="45" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="G501" s="2">
         <v>39177</v>
@@ -23798,7 +24225,7 @@
         <v>1530</v>
       </c>
       <c r="I501" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="U501" s="2">
         <v>39177</v>
@@ -23824,7 +24251,7 @@
         <v>1381</v>
       </c>
       <c r="I502" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="U502" s="2">
         <v>39176</v>
@@ -23853,7 +24280,7 @@
         <v>1366</v>
       </c>
       <c r="I503" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="U503" s="2">
         <v>39176</v>
@@ -23867,7 +24294,7 @@
         <v>1166</v>
       </c>
       <c r="D504" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="F504" s="45">
         <v>13.05</v>
@@ -23879,7 +24306,7 @@
         <v>1432</v>
       </c>
       <c r="I504" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="U504" s="2">
         <v>39176</v>
@@ -23893,7 +24320,7 @@
         <v>1166</v>
       </c>
       <c r="D505" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="F505" s="45">
         <v>9.01</v>
@@ -23905,7 +24332,7 @@
         <v>1509</v>
       </c>
       <c r="I505" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="U505" s="2">
         <v>39176</v>
@@ -23919,7 +24346,7 @@
         <v>1166</v>
       </c>
       <c r="D506" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="F506" s="45">
         <v>8.1</v>
@@ -23931,7 +24358,7 @@
         <v>1443</v>
       </c>
       <c r="I506" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
       <c r="U506" s="2">
         <v>39176</v>
@@ -23960,7 +24387,7 @@
         <v>1464</v>
       </c>
       <c r="I507" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="U507" s="2">
         <v>39176</v>
@@ -23977,7 +24404,7 @@
         <v>1166</v>
       </c>
       <c r="D508" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="F508" s="45">
         <v>3.1</v>
@@ -23989,7 +24416,7 @@
         <v>1531</v>
       </c>
       <c r="I508" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="U508" s="2">
         <v>39176</v>
@@ -24015,7 +24442,7 @@
         <v>1467</v>
       </c>
       <c r="I509" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="U509" s="2">
         <v>39176</v>
@@ -24029,10 +24456,10 @@
         <v>1166</v>
       </c>
       <c r="D510" t="s">
-        <v>2261</v>
+        <v>2259</v>
       </c>
       <c r="F510" s="45" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="G510" s="2">
         <v>39176</v>
@@ -24041,7 +24468,7 @@
         <v>1407</v>
       </c>
       <c r="I510" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="U510" s="2">
         <v>39176</v>
@@ -24070,7 +24497,7 @@
         <v>1383</v>
       </c>
       <c r="I511" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="U511" s="2">
         <v>39176</v>
@@ -24087,7 +24514,7 @@
         <v>1166</v>
       </c>
       <c r="D512" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="F512" s="45">
         <v>8.3000000000000007</v>
@@ -24099,7 +24526,7 @@
         <v>1441</v>
       </c>
       <c r="I512" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="U512" s="2">
         <v>39176</v>
@@ -24116,7 +24543,7 @@
         <v>1166</v>
       </c>
       <c r="D513" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="F513" s="45">
         <v>13.25</v>
@@ -24128,7 +24555,7 @@
         <v>1411</v>
       </c>
       <c r="I513" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
       <c r="U513" s="2">
         <v>39176</v>
@@ -24142,7 +24569,7 @@
         <v>1166</v>
       </c>
       <c r="D514" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="F514" s="45">
         <v>13.3</v>
@@ -24154,7 +24581,7 @@
         <v>1426</v>
       </c>
       <c r="I514" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="U514" s="2">
         <v>39176</v>
@@ -24171,7 +24598,7 @@
         <v>1166</v>
       </c>
       <c r="D515" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F515" s="45">
         <v>8.1</v>
@@ -24183,7 +24610,7 @@
         <v>1442</v>
       </c>
       <c r="I515" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="U515" s="2">
         <v>39176</v>
@@ -24197,7 +24624,7 @@
         <v>1166</v>
       </c>
       <c r="D516" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="F516" s="45">
         <v>13.5</v>
@@ -24209,7 +24636,7 @@
         <v>1413</v>
       </c>
       <c r="I516" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="U516" s="2">
         <v>39176</v>
@@ -24238,7 +24665,7 @@
         <v>1378</v>
       </c>
       <c r="I517" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="U517" s="2">
         <v>39175</v>
@@ -24267,7 +24694,7 @@
         <v>1513</v>
       </c>
       <c r="I518" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="U518" s="2">
         <v>39175</v>
@@ -24293,7 +24720,7 @@
         <v>1468</v>
       </c>
       <c r="I519" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="U519" s="2">
         <v>39175</v>
@@ -24307,10 +24734,10 @@
         <v>1166</v>
       </c>
       <c r="D520" t="s">
-        <v>2208</v>
+        <v>2206</v>
       </c>
       <c r="F520" s="45" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="G520" s="2">
         <v>39163</v>
@@ -24319,7 +24746,7 @@
         <v>1532</v>
       </c>
       <c r="I520" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="U520" s="2">
         <v>39163</v>
@@ -24333,7 +24760,7 @@
         <v>1166</v>
       </c>
       <c r="D521" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="F521" s="45">
         <v>12</v>
@@ -24345,7 +24772,7 @@
         <v>1435</v>
       </c>
       <c r="I521" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="U521" s="2">
         <v>39163</v>
@@ -24359,10 +24786,10 @@
         <v>1166</v>
       </c>
       <c r="D522" t="s">
-        <v>2205</v>
+        <v>2203</v>
       </c>
       <c r="F522" s="45" t="s">
-        <v>2144</v>
+        <v>2142</v>
       </c>
       <c r="G522" s="2">
         <v>39163</v>
@@ -24371,7 +24798,7 @@
         <v>1533</v>
       </c>
       <c r="I522" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="U522" s="2">
         <v>39163</v>
@@ -24388,7 +24815,7 @@
         <v>1166</v>
       </c>
       <c r="D523" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="F523" s="45">
         <v>12</v>
@@ -24400,7 +24827,7 @@
         <v>1433</v>
       </c>
       <c r="I523" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="U523" s="2">
         <v>39163</v>
@@ -24414,7 +24841,7 @@
         <v>1166</v>
       </c>
       <c r="D524" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="F524" s="45">
         <v>10.02</v>
@@ -24426,7 +24853,7 @@
         <v>1439</v>
       </c>
       <c r="I524" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="U524" s="2">
         <v>39163</v>
@@ -24443,7 +24870,7 @@
         <v>1166</v>
       </c>
       <c r="D525" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="F525" s="45">
         <v>10.02</v>
@@ -24455,7 +24882,7 @@
         <v>1437</v>
       </c>
       <c r="I525" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="U525" s="2">
         <v>39163</v>
@@ -24469,10 +24896,10 @@
         <v>1166</v>
       </c>
       <c r="D526" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
       <c r="F526" s="45" t="s">
-        <v>2145</v>
+        <v>2143</v>
       </c>
       <c r="G526" s="2">
         <v>39163</v>
@@ -24481,7 +24908,7 @@
         <v>1534</v>
       </c>
       <c r="I526" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="U526" s="2">
         <v>39163</v>
@@ -24495,10 +24922,10 @@
         <v>1166</v>
       </c>
       <c r="D527" t="s">
-        <v>2204</v>
+        <v>2202</v>
       </c>
       <c r="F527" s="45" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="G527" s="2">
         <v>39163</v>
@@ -24507,7 +24934,7 @@
         <v>1535</v>
       </c>
       <c r="I527" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="U527" s="2">
         <v>39163</v>
@@ -24524,7 +24951,7 @@
         <v>1166</v>
       </c>
       <c r="D528" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="F528" s="45">
         <v>12.2</v>
@@ -24536,7 +24963,7 @@
         <v>1536</v>
       </c>
       <c r="I528" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="U528" s="2">
         <v>39163</v>
@@ -24553,10 +24980,10 @@
         <v>1166</v>
       </c>
       <c r="D529" t="s">
-        <v>2278</v>
+        <v>2276</v>
       </c>
       <c r="F529" s="45" t="s">
-        <v>2146</v>
+        <v>2144</v>
       </c>
       <c r="G529" s="2">
         <v>39163</v>
@@ -24565,7 +24992,7 @@
         <v>1537</v>
       </c>
       <c r="I529" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="U529" s="2">
         <v>39163</v>
@@ -24582,7 +25009,7 @@
         <v>1166</v>
       </c>
       <c r="D530" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="F530" s="45">
         <v>12.3</v>
@@ -24594,7 +25021,7 @@
         <v>1538</v>
       </c>
       <c r="I530" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="U530" s="2">
         <v>39163</v>
@@ -24611,10 +25038,10 @@
         <v>1166</v>
       </c>
       <c r="D531" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
       <c r="F531" s="45" t="s">
-        <v>2147</v>
+        <v>2145</v>
       </c>
       <c r="G531" s="2">
         <v>39163</v>
@@ -24623,7 +25050,7 @@
         <v>1539</v>
       </c>
       <c r="I531" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="U531" s="2">
         <v>39163</v>
@@ -24640,10 +25067,10 @@
         <v>1166</v>
       </c>
       <c r="D532" t="s">
-        <v>2277</v>
+        <v>2275</v>
       </c>
       <c r="F532" s="45" t="s">
-        <v>2148</v>
+        <v>2146</v>
       </c>
       <c r="G532" s="2">
         <v>39163</v>
@@ -24652,7 +25079,7 @@
         <v>1540</v>
       </c>
       <c r="I532" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="U532" s="2">
         <v>39163</v>
@@ -24666,7 +25093,7 @@
         <v>1166</v>
       </c>
       <c r="D533" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="F533" s="45">
         <v>12.2</v>
@@ -24678,7 +25105,7 @@
         <v>1541</v>
       </c>
       <c r="I533" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="U533" s="2">
         <v>39163</v>
@@ -24707,7 +25134,7 @@
         <v>1485</v>
       </c>
       <c r="I534" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="U534" s="2">
         <v>39149</v>
@@ -24733,7 +25160,7 @@
         <v>1488</v>
       </c>
       <c r="I535" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="U535" s="2">
         <v>39149</v>
@@ -24759,7 +25186,7 @@
         <v>1484</v>
       </c>
       <c r="I536" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="U536" s="2">
         <v>39149</v>
@@ -24788,7 +25215,7 @@
         <v>1460</v>
       </c>
       <c r="I537" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="U537" s="2">
         <v>39149</v>
@@ -24814,7 +25241,7 @@
         <v>1461</v>
       </c>
       <c r="I538" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="U538" s="2">
         <v>39149</v>
@@ -24828,7 +25255,7 @@
         <v>1166</v>
       </c>
       <c r="D539" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="F539" s="45">
         <v>13.2</v>
@@ -24840,7 +25267,7 @@
         <v>1429</v>
       </c>
       <c r="I539" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="U539" s="2">
         <v>39148</v>
@@ -24857,7 +25284,7 @@
         <v>1166</v>
       </c>
       <c r="D540" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="F540" s="45">
         <v>13.55</v>
@@ -24869,7 +25296,7 @@
         <v>1408</v>
       </c>
       <c r="I540" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="U540" s="2">
         <v>39148</v>
@@ -24886,7 +25313,7 @@
         <v>1166</v>
       </c>
       <c r="D541" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="F541" s="45">
         <v>13.2</v>
@@ -24898,7 +25325,7 @@
         <v>1428</v>
       </c>
       <c r="I541" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="U541" s="2">
         <v>39148</v>
@@ -24927,7 +25354,7 @@
         <v>1542</v>
       </c>
       <c r="I542" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="U542" s="2">
         <v>39148</v>
@@ -24941,7 +25368,7 @@
         <v>1166</v>
       </c>
       <c r="D543" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="F543" s="45">
         <v>13.55</v>
@@ -24953,7 +25380,7 @@
         <v>1412</v>
       </c>
       <c r="I543" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="U543" s="2">
         <v>39148</v>
@@ -24970,7 +25397,7 @@
         <v>1166</v>
       </c>
       <c r="D544" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="F544" s="45">
         <v>8.5</v>
@@ -24982,7 +25409,7 @@
         <v>1543</v>
       </c>
       <c r="I544" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="U544" s="2">
         <v>39142</v>
@@ -24999,7 +25426,7 @@
         <v>1166</v>
       </c>
       <c r="D545" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
       <c r="F545" s="45">
         <v>4.5</v>
@@ -25011,7 +25438,7 @@
         <v>1544</v>
       </c>
       <c r="I545" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="U545" s="2">
         <v>39114</v>
@@ -25028,7 +25455,7 @@
         <v>1166</v>
       </c>
       <c r="D546" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="F546" s="45">
         <v>13.3</v>
@@ -25040,7 +25467,7 @@
         <v>1410</v>
       </c>
       <c r="I546" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="U546" s="2">
         <v>39112</v>
@@ -25069,7 +25496,7 @@
         <v>1464</v>
       </c>
       <c r="I547" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="U547" s="2">
         <v>39105</v>
@@ -25083,7 +25510,7 @@
         <v>1166</v>
       </c>
       <c r="D548" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="F548" s="45">
         <v>13.5</v>
@@ -25095,7 +25522,7 @@
         <v>1413</v>
       </c>
       <c r="I548" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="U548" s="2">
         <v>39104</v>
@@ -25124,7 +25551,7 @@
         <v>1531</v>
       </c>
       <c r="I549" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="U549" s="2">
         <v>39104</v>
@@ -25150,7 +25577,7 @@
         <v>1381</v>
       </c>
       <c r="I550" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="U550" s="2">
         <v>39104</v>
@@ -25167,7 +25594,7 @@
         <v>1166</v>
       </c>
       <c r="D551" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="F551" s="45">
         <v>8.3000000000000007</v>
@@ -25179,7 +25606,7 @@
         <v>1441</v>
       </c>
       <c r="I551" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="U551" s="2">
         <v>39104</v>
@@ -25193,7 +25620,7 @@
         <v>1166</v>
       </c>
       <c r="D552" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="F552" s="45">
         <v>13.05</v>
@@ -25205,7 +25632,7 @@
         <v>1432</v>
       </c>
       <c r="I552" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="U552" s="2">
         <v>39104</v>
@@ -25222,10 +25649,10 @@
         <v>1166</v>
       </c>
       <c r="D553" t="s">
-        <v>2279</v>
+        <v>2277</v>
       </c>
       <c r="F553" s="45" t="s">
-        <v>2149</v>
+        <v>2147</v>
       </c>
       <c r="G553" s="2">
         <v>39099</v>
@@ -25234,7 +25661,7 @@
         <v>1378</v>
       </c>
       <c r="I553" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="U553" s="2">
         <v>39099</v>
@@ -25263,7 +25690,7 @@
         <v>1513</v>
       </c>
       <c r="I554" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="U554" s="2">
         <v>39099</v>
@@ -25289,7 +25716,7 @@
         <v>1545</v>
       </c>
       <c r="I555" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="U555" s="2">
         <v>39087</v>
@@ -25315,7 +25742,7 @@
         <v>1546</v>
       </c>
       <c r="I556" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="U556" s="2">
         <v>39087</v>
@@ -25341,7 +25768,7 @@
         <v>1361</v>
       </c>
       <c r="I557" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="U557" s="2">
         <v>39069</v>
@@ -25355,7 +25782,7 @@
         <v>1166</v>
       </c>
       <c r="D558" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="F558" s="45">
         <v>13.25</v>
@@ -25367,7 +25794,7 @@
         <v>1427</v>
       </c>
       <c r="I558" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="U558" s="2">
         <v>38974</v>
@@ -25396,7 +25823,7 @@
         <v>1475</v>
       </c>
       <c r="I559" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="U559" s="2">
         <v>38923</v>
@@ -25413,7 +25840,7 @@
         <v>1166</v>
       </c>
       <c r="D560" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
       <c r="F560" s="45">
         <v>14.1</v>
@@ -25425,7 +25852,7 @@
         <v>1547</v>
       </c>
       <c r="I560" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="U560" s="2">
         <v>38912</v>
@@ -25454,7 +25881,7 @@
         <v>1548</v>
       </c>
       <c r="I561" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="U561" s="2">
         <v>38903</v>
@@ -25480,7 +25907,7 @@
         <v>1483</v>
       </c>
       <c r="I562" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="U562" s="2">
         <v>38876</v>
@@ -25509,7 +25936,7 @@
         <v>1482</v>
       </c>
       <c r="I563" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="U563" s="2">
         <v>38876</v>
@@ -25523,7 +25950,7 @@
         <v>1166</v>
       </c>
       <c r="D564" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="F564" s="45">
         <v>13</v>
@@ -25535,7 +25962,7 @@
         <v>1384</v>
       </c>
       <c r="I564" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="U564" s="2">
         <v>38821</v>
@@ -25564,7 +25991,7 @@
         <v>1549</v>
       </c>
       <c r="I565" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="U565" s="2">
         <v>38820</v>
@@ -25593,7 +26020,7 @@
         <v>1549</v>
       </c>
       <c r="I566" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="U566" s="2">
         <v>38820</v>
@@ -25619,7 +26046,7 @@
         <v>1374</v>
       </c>
       <c r="I567" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="U567" s="2">
         <v>38788</v>
@@ -25648,7 +26075,7 @@
         <v>1371</v>
       </c>
       <c r="I568" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="U568" s="2">
         <v>38700</v>
@@ -25662,7 +26089,7 @@
         <v>1166</v>
       </c>
       <c r="D569" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="F569" s="45">
         <v>14.2</v>
@@ -25674,7 +26101,7 @@
         <v>1370</v>
       </c>
       <c r="I569" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="U569" s="2">
         <v>38700</v>
@@ -25700,7 +26127,7 @@
         <v>1374</v>
       </c>
       <c r="I570" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="U570" s="2">
         <v>38698</v>
@@ -25729,7 +26156,7 @@
         <v>1373</v>
       </c>
       <c r="I571" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="U571" s="2">
         <v>38698</v>
@@ -25743,7 +26170,7 @@
         <v>1166</v>
       </c>
       <c r="D572" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="F572" s="45">
         <v>4.2</v>
@@ -25755,7 +26182,7 @@
         <v>1550</v>
       </c>
       <c r="I572" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="U572" s="2">
         <v>38541</v>
@@ -25769,10 +26196,10 @@
         <v>1166</v>
       </c>
       <c r="D573" t="s">
-        <v>2249</v>
+        <v>2247</v>
       </c>
       <c r="F573" s="45" t="s">
-        <v>2150</v>
+        <v>2148</v>
       </c>
       <c r="G573" s="2">
         <v>38533</v>
@@ -25781,7 +26208,7 @@
         <v>1551</v>
       </c>
       <c r="I573" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="U573" s="2">
         <v>38533</v>
@@ -25795,10 +26222,10 @@
         <v>1166</v>
       </c>
       <c r="D574" t="s">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="F574" s="45" t="s">
-        <v>2151</v>
+        <v>2149</v>
       </c>
       <c r="G574" s="2">
         <v>38533</v>
@@ -25807,7 +26234,7 @@
         <v>1552</v>
       </c>
       <c r="I574" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="U574" s="2">
         <v>38533</v>
@@ -25821,10 +26248,10 @@
         <v>1166</v>
       </c>
       <c r="D575" t="s">
-        <v>2241</v>
+        <v>2239</v>
       </c>
       <c r="F575" s="45" t="s">
-        <v>2152</v>
+        <v>2150</v>
       </c>
       <c r="G575" s="2">
         <v>38533</v>
@@ -25833,7 +26260,7 @@
         <v>1553</v>
       </c>
       <c r="I575" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="U575" s="2">
         <v>38533</v>
@@ -25847,10 +26274,10 @@
         <v>1166</v>
       </c>
       <c r="D576" t="s">
-        <v>2243</v>
+        <v>2241</v>
       </c>
       <c r="F576" s="45" t="s">
-        <v>2153</v>
+        <v>2151</v>
       </c>
       <c r="G576" s="2">
         <v>38533</v>
@@ -25859,7 +26286,7 @@
         <v>1554</v>
       </c>
       <c r="I576" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="U576" s="2">
         <v>38533</v>
@@ -25873,10 +26300,10 @@
         <v>1166</v>
       </c>
       <c r="D577" t="s">
-        <v>2242</v>
+        <v>2240</v>
       </c>
       <c r="F577" s="45" t="s">
-        <v>2154</v>
+        <v>2152</v>
       </c>
       <c r="G577" s="2">
         <v>38533</v>
@@ -25885,7 +26312,7 @@
         <v>1555</v>
       </c>
       <c r="I577" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="U577" s="2">
         <v>38533</v>
@@ -25899,10 +26326,10 @@
         <v>1166</v>
       </c>
       <c r="D578" t="s">
-        <v>2246</v>
+        <v>2244</v>
       </c>
       <c r="F578" s="45" t="s">
-        <v>2155</v>
+        <v>2153</v>
       </c>
       <c r="G578" s="2">
         <v>38533</v>
@@ -25911,7 +26338,7 @@
         <v>1556</v>
       </c>
       <c r="I578" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="U578" s="2">
         <v>38533</v>
@@ -25925,10 +26352,10 @@
         <v>1166</v>
       </c>
       <c r="D579" t="s">
-        <v>2244</v>
+        <v>2242</v>
       </c>
       <c r="F579" s="45" t="s">
-        <v>2156</v>
+        <v>2154</v>
       </c>
       <c r="G579" s="2">
         <v>38533</v>
@@ -25937,7 +26364,7 @@
         <v>1557</v>
       </c>
       <c r="I579" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="U579" s="2">
         <v>38533</v>
@@ -25963,7 +26390,7 @@
         <v>1353</v>
       </c>
       <c r="I580" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="U580" s="2">
         <v>38533</v>
@@ -25977,10 +26404,10 @@
         <v>1166</v>
       </c>
       <c r="D581" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="F581" s="45" t="s">
-        <v>2157</v>
+        <v>2155</v>
       </c>
       <c r="G581" s="2">
         <v>38533</v>
@@ -25989,7 +26416,7 @@
         <v>1558</v>
       </c>
       <c r="I581" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="U581" s="2">
         <v>38533</v>
@@ -26003,10 +26430,10 @@
         <v>1166</v>
       </c>
       <c r="D582" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
       <c r="F582" s="45" t="s">
-        <v>2158</v>
+        <v>2156</v>
       </c>
       <c r="G582" s="2">
         <v>38533</v>
@@ -26015,7 +26442,7 @@
         <v>1559</v>
       </c>
       <c r="I582" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="U582" s="2">
         <v>38533</v>
@@ -26029,10 +26456,10 @@
         <v>1166</v>
       </c>
       <c r="D583" t="s">
-        <v>2255</v>
+        <v>2253</v>
       </c>
       <c r="F583" s="45" t="s">
-        <v>2159</v>
+        <v>2157</v>
       </c>
       <c r="G583" s="2">
         <v>38533</v>
@@ -26041,7 +26468,7 @@
         <v>1560</v>
       </c>
       <c r="I583" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="U583" s="2">
         <v>38533</v>
@@ -26055,10 +26482,10 @@
         <v>1166</v>
       </c>
       <c r="D584" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
       <c r="F584" s="45" t="s">
-        <v>2160</v>
+        <v>2158</v>
       </c>
       <c r="G584" s="2">
         <v>38533</v>
@@ -26067,7 +26494,7 @@
         <v>1561</v>
       </c>
       <c r="I584" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="U584" s="2">
         <v>38533</v>
@@ -26081,10 +26508,10 @@
         <v>1166</v>
       </c>
       <c r="D585" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="F585" s="45" t="s">
-        <v>2161</v>
+        <v>2159</v>
       </c>
       <c r="G585" s="2">
         <v>38533</v>
@@ -26093,7 +26520,7 @@
         <v>1562</v>
       </c>
       <c r="I585" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="U585" s="2">
         <v>38533</v>
@@ -26107,10 +26534,10 @@
         <v>1166</v>
       </c>
       <c r="D586" t="s">
-        <v>2257</v>
+        <v>2255</v>
       </c>
       <c r="F586" s="45" t="s">
-        <v>2162</v>
+        <v>2160</v>
       </c>
       <c r="G586" s="2">
         <v>38533</v>
@@ -26119,7 +26546,7 @@
         <v>1563</v>
       </c>
       <c r="I586" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="U586" s="2">
         <v>38533</v>
@@ -26133,10 +26560,10 @@
         <v>1166</v>
       </c>
       <c r="D587" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
       <c r="F587" s="45" t="s">
-        <v>2163</v>
+        <v>2161</v>
       </c>
       <c r="G587" s="2">
         <v>38533</v>
@@ -26145,7 +26572,7 @@
         <v>1564</v>
       </c>
       <c r="I587" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="U587" s="2">
         <v>38533</v>
@@ -26159,10 +26586,10 @@
         <v>1166</v>
       </c>
       <c r="D588" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="F588" s="45" t="s">
-        <v>2164</v>
+        <v>2162</v>
       </c>
       <c r="G588" s="2">
         <v>38533</v>
@@ -26171,7 +26598,7 @@
         <v>1565</v>
       </c>
       <c r="I588" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="U588" s="2">
         <v>38533</v>
@@ -26185,10 +26612,10 @@
         <v>1166</v>
       </c>
       <c r="D589" t="s">
-        <v>2252</v>
+        <v>2250</v>
       </c>
       <c r="F589" s="45" t="s">
-        <v>2165</v>
+        <v>2163</v>
       </c>
       <c r="G589" s="2">
         <v>38533</v>
@@ -26197,7 +26624,7 @@
         <v>1566</v>
       </c>
       <c r="I589" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="U589" s="2">
         <v>38533</v>
@@ -26211,10 +26638,10 @@
         <v>1166</v>
       </c>
       <c r="D590" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
       <c r="F590" s="45" t="s">
-        <v>2166</v>
+        <v>2164</v>
       </c>
       <c r="G590" s="2">
         <v>38533</v>
@@ -26223,7 +26650,7 @@
         <v>1567</v>
       </c>
       <c r="I590" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="U590" s="2">
         <v>38533</v>
@@ -26237,10 +26664,10 @@
         <v>1166</v>
       </c>
       <c r="D591" t="s">
-        <v>2258</v>
+        <v>2256</v>
       </c>
       <c r="F591" s="45" t="s">
-        <v>2167</v>
+        <v>2165</v>
       </c>
       <c r="G591" s="2">
         <v>38508</v>
@@ -26249,7 +26676,7 @@
         <v>1568</v>
       </c>
       <c r="I591" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="U591" s="2">
         <v>38508</v>
@@ -26263,10 +26690,10 @@
         <v>1166</v>
       </c>
       <c r="D592" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="F592" s="45" t="s">
-        <v>2168</v>
+        <v>2166</v>
       </c>
       <c r="G592" s="2">
         <v>38361</v>
@@ -26275,7 +26702,7 @@
         <v>1569</v>
       </c>
       <c r="I592" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="U592" s="2">
         <v>38361</v>
@@ -26292,7 +26719,7 @@
         <v>1166</v>
       </c>
       <c r="D593" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="F593" s="45">
         <v>16</v>
@@ -26304,7 +26731,7 @@
         <v>1570</v>
       </c>
       <c r="I593" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="U593" s="2">
         <v>38361</v>
@@ -26318,10 +26745,10 @@
         <v>1166</v>
       </c>
       <c r="D594" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="F594" s="45" t="s">
-        <v>2169</v>
+        <v>2167</v>
       </c>
       <c r="G594" s="2">
         <v>38361</v>
@@ -26330,7 +26757,7 @@
         <v>1571</v>
       </c>
       <c r="I594" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="U594" s="2">
         <v>38361</v>
@@ -26344,10 +26771,10 @@
         <v>1166</v>
       </c>
       <c r="D595" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
       <c r="F595" s="45" t="s">
-        <v>2170</v>
+        <v>2168</v>
       </c>
       <c r="G595" s="2">
         <v>38361</v>
@@ -26356,7 +26783,7 @@
         <v>1572</v>
       </c>
       <c r="I595" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="U595" s="2">
         <v>38361</v>
@@ -26370,10 +26797,10 @@
         <v>1166</v>
       </c>
       <c r="D596" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="F596" s="45" t="s">
-        <v>2171</v>
+        <v>2169</v>
       </c>
       <c r="G596" s="2">
         <v>38361</v>
@@ -26382,7 +26809,7 @@
         <v>1573</v>
       </c>
       <c r="I596" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="U596" s="2">
         <v>38361</v>
@@ -26396,10 +26823,10 @@
         <v>1166</v>
       </c>
       <c r="D597" t="s">
-        <v>2221</v>
+        <v>2219</v>
       </c>
       <c r="F597" s="45" t="s">
-        <v>2172</v>
+        <v>2170</v>
       </c>
       <c r="G597" s="2">
         <v>38361</v>
@@ -26408,7 +26835,7 @@
         <v>1574</v>
       </c>
       <c r="I597" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="U597" s="2">
         <v>38361</v>
@@ -26422,7 +26849,7 @@
         <v>1166</v>
       </c>
       <c r="D598" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="F598" s="45">
         <v>16</v>
@@ -26434,7 +26861,7 @@
         <v>1575</v>
       </c>
       <c r="I598" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="U598" s="2">
         <v>38355</v>
@@ -26448,10 +26875,10 @@
         <v>1166</v>
       </c>
       <c r="D599" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="F599" s="45" t="s">
-        <v>2173</v>
+        <v>2171</v>
       </c>
       <c r="G599" s="2">
         <v>38229</v>
@@ -26460,7 +26887,7 @@
         <v>1576</v>
       </c>
       <c r="I599" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="U599" s="2">
         <v>38229</v>
@@ -26474,10 +26901,10 @@
         <v>1166</v>
       </c>
       <c r="D600" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="F600" s="45" t="s">
-        <v>2174</v>
+        <v>2172</v>
       </c>
       <c r="G600" s="2">
         <v>38213</v>
@@ -26486,7 +26913,7 @@
         <v>1577</v>
       </c>
       <c r="I600" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="U600" s="2">
         <v>38213</v>
@@ -26500,7 +26927,7 @@
         <v>1166</v>
       </c>
       <c r="D601" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
       <c r="F601" s="45">
         <v>17.100000000000001</v>
@@ -26512,7 +26939,7 @@
         <v>1578</v>
       </c>
       <c r="I601" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="U601" s="2">
         <v>38213</v>
@@ -26526,10 +26953,10 @@
         <v>1166</v>
       </c>
       <c r="D602" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
       <c r="F602" s="45" t="s">
-        <v>2175</v>
+        <v>2173</v>
       </c>
       <c r="G602" s="2">
         <v>38213</v>
@@ -26538,7 +26965,7 @@
         <v>1579</v>
       </c>
       <c r="I602" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="U602" s="2">
         <v>38213</v>
@@ -26552,10 +26979,10 @@
         <v>1166</v>
       </c>
       <c r="D603" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="F603" s="45" t="s">
-        <v>2176</v>
+        <v>2174</v>
       </c>
       <c r="G603" s="2">
         <v>38213</v>
@@ -26564,7 +26991,7 @@
         <v>1580</v>
       </c>
       <c r="I603" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="U603" s="2">
         <v>38213</v>
@@ -26578,10 +27005,10 @@
         <v>1166</v>
       </c>
       <c r="D604" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="F604" s="45" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
       <c r="G604" s="2">
         <v>38213</v>
@@ -26590,7 +27017,7 @@
         <v>1581</v>
       </c>
       <c r="I604" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="U604" s="2">
         <v>38213</v>
@@ -26604,10 +27031,10 @@
         <v>1166</v>
       </c>
       <c r="D605" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="F605" s="45" t="s">
-        <v>2178</v>
+        <v>2176</v>
       </c>
       <c r="G605" s="2">
         <v>38213</v>
@@ -26616,7 +27043,7 @@
         <v>1582</v>
       </c>
       <c r="I605" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="U605" s="2">
         <v>38213</v>
@@ -26630,10 +27057,10 @@
         <v>1166</v>
       </c>
       <c r="D606" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="F606" s="45" t="s">
-        <v>2179</v>
+        <v>2177</v>
       </c>
       <c r="G606" s="2">
         <v>38213</v>
@@ -26642,7 +27069,7 @@
         <v>1583</v>
       </c>
       <c r="I606" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="U606" s="2">
         <v>38213</v>
@@ -26656,10 +27083,10 @@
         <v>1166</v>
       </c>
       <c r="D607" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
       <c r="F607" s="45" t="s">
-        <v>2180</v>
+        <v>2178</v>
       </c>
       <c r="G607" s="2">
         <v>38213</v>
@@ -26668,7 +27095,7 @@
         <v>1584</v>
       </c>
       <c r="I607" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="U607" s="2">
         <v>38213</v>
@@ -26682,7 +27109,7 @@
         <v>1166</v>
       </c>
       <c r="D608" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="F608" s="45">
         <v>8.6</v>
@@ -26694,7 +27121,7 @@
         <v>1585</v>
       </c>
       <c r="I608" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="U608" s="2">
         <v>38211</v>
@@ -26708,10 +27135,10 @@
         <v>1166</v>
       </c>
       <c r="D609" t="s">
-        <v>2234</v>
+        <v>2232</v>
       </c>
       <c r="F609" s="45" t="s">
-        <v>2181</v>
+        <v>2179</v>
       </c>
       <c r="G609" s="2">
         <v>38208</v>
@@ -26720,7 +27147,7 @@
         <v>1586</v>
       </c>
       <c r="I609" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="U609" s="2">
         <v>38208</v>
@@ -26734,7 +27161,7 @@
         <v>1166</v>
       </c>
       <c r="D610" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="F610" s="45" t="s">
         <v>1200</v>
@@ -26746,7 +27173,7 @@
         <v>1587</v>
       </c>
       <c r="I610" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="U610" s="2">
         <v>38208</v>
@@ -26760,7 +27187,7 @@
         <v>1166</v>
       </c>
       <c r="D611" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="F611" s="45">
         <v>17.5</v>
@@ -26772,7 +27199,7 @@
         <v>1588</v>
       </c>
       <c r="I611" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="U611" s="2">
         <v>38208</v>
@@ -26786,10 +27213,10 @@
         <v>1166</v>
       </c>
       <c r="D612" t="s">
-        <v>2235</v>
+        <v>2233</v>
       </c>
       <c r="F612" s="45" t="s">
-        <v>2182</v>
+        <v>2180</v>
       </c>
       <c r="G612" s="2">
         <v>38208</v>
@@ -26798,7 +27225,7 @@
         <v>1589</v>
       </c>
       <c r="I612" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="U612" s="2">
         <v>38208</v>
@@ -26812,10 +27239,10 @@
         <v>1166</v>
       </c>
       <c r="D613" t="s">
-        <v>2236</v>
+        <v>2234</v>
       </c>
       <c r="F613" s="45" t="s">
-        <v>2183</v>
+        <v>2181</v>
       </c>
       <c r="G613" s="2">
         <v>38208</v>
@@ -26824,7 +27251,7 @@
         <v>1590</v>
       </c>
       <c r="I613" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="U613" s="2">
         <v>38208</v>
@@ -26838,10 +27265,10 @@
         <v>1166</v>
       </c>
       <c r="D614" t="s">
-        <v>2233</v>
+        <v>2231</v>
       </c>
       <c r="F614" s="45" t="s">
-        <v>2184</v>
+        <v>2182</v>
       </c>
       <c r="G614" s="2">
         <v>38208</v>
@@ -26850,7 +27277,7 @@
         <v>1591</v>
       </c>
       <c r="I614" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="U614" s="2">
         <v>38208</v>
@@ -26864,10 +27291,10 @@
         <v>1166</v>
       </c>
       <c r="D615" t="s">
-        <v>2237</v>
+        <v>2235</v>
       </c>
       <c r="F615" s="45" t="s">
-        <v>2185</v>
+        <v>2183</v>
       </c>
       <c r="G615" s="2">
         <v>38208</v>
@@ -26876,7 +27303,7 @@
         <v>1592</v>
       </c>
       <c r="I615" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="U615" s="2">
         <v>38208</v>
@@ -26890,10 +27317,10 @@
         <v>1166</v>
       </c>
       <c r="D616" t="s">
-        <v>2267</v>
+        <v>2265</v>
       </c>
       <c r="F616" s="45" t="s">
-        <v>2186</v>
+        <v>2184</v>
       </c>
       <c r="G616" s="2">
         <v>38207</v>
@@ -26902,7 +27329,7 @@
         <v>1593</v>
       </c>
       <c r="I616" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="U616" s="2">
         <v>38207</v>
@@ -26916,10 +27343,10 @@
         <v>1166</v>
       </c>
       <c r="D617" t="s">
-        <v>2271</v>
+        <v>2269</v>
       </c>
       <c r="F617" s="45" t="s">
-        <v>2187</v>
+        <v>2185</v>
       </c>
       <c r="G617" s="2">
         <v>38207</v>
@@ -26928,7 +27355,7 @@
         <v>1594</v>
       </c>
       <c r="I617" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="U617" s="2">
         <v>38207</v>
@@ -26942,10 +27369,10 @@
         <v>1166</v>
       </c>
       <c r="D618" t="s">
-        <v>2270</v>
+        <v>2268</v>
       </c>
       <c r="F618" s="45" t="s">
-        <v>2188</v>
+        <v>2186</v>
       </c>
       <c r="G618" s="2">
         <v>38207</v>
@@ -26954,7 +27381,7 @@
         <v>1595</v>
       </c>
       <c r="I618" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="U618" s="2">
         <v>38207</v>
@@ -26968,7 +27395,7 @@
         <v>1166</v>
       </c>
       <c r="D619" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="F619" s="45">
         <v>4.1500000000000004</v>
@@ -26980,7 +27407,7 @@
         <v>1596</v>
       </c>
       <c r="I619" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="U619" s="2">
         <v>38207</v>
@@ -26994,10 +27421,10 @@
         <v>1166</v>
       </c>
       <c r="D620" t="s">
-        <v>2268</v>
+        <v>2266</v>
       </c>
       <c r="F620" s="45" t="s">
-        <v>2189</v>
+        <v>2187</v>
       </c>
       <c r="G620" s="2">
         <v>38207</v>
@@ -27006,7 +27433,7 @@
         <v>1597</v>
       </c>
       <c r="I620" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="U620" s="2">
         <v>38207</v>
@@ -27020,10 +27447,10 @@
         <v>1166</v>
       </c>
       <c r="D621" t="s">
-        <v>2269</v>
+        <v>2267</v>
       </c>
       <c r="F621" s="45" t="s">
-        <v>2190</v>
+        <v>2188</v>
       </c>
       <c r="G621" s="2">
         <v>38207</v>
@@ -27032,7 +27459,7 @@
         <v>1598</v>
       </c>
       <c r="I621" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="U621" s="2">
         <v>38207</v>
@@ -27046,7 +27473,7 @@
         <v>1166</v>
       </c>
       <c r="D622" t="s">
-        <v>2264</v>
+        <v>2262</v>
       </c>
       <c r="F622" s="45" t="s">
         <v>1198</v>
@@ -27058,7 +27485,7 @@
         <v>1599</v>
       </c>
       <c r="I622" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
       <c r="U622" s="2">
         <v>38205</v>
@@ -27072,7 +27499,7 @@
         <v>1166</v>
       </c>
       <c r="D623" t="s">
-        <v>2265</v>
+        <v>2263</v>
       </c>
       <c r="F623" s="45" t="s">
         <v>1199</v>
@@ -27084,7 +27511,7 @@
         <v>1600</v>
       </c>
       <c r="I623" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="U623" s="2">
         <v>38205</v>
@@ -27098,7 +27525,7 @@
         <v>1166</v>
       </c>
       <c r="D624" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
       <c r="F624" s="45">
         <v>4.01</v>
@@ -27110,7 +27537,7 @@
         <v>1601</v>
       </c>
       <c r="I624" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="U624" s="2">
         <v>38205</v>
@@ -27127,10 +27554,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W66"/>
+  <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:Q8"/>
+    <sheetView topLeftCell="F52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -27237,10 +27664,10 @@
         <v>552</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R8" s="21" t="s">
         <v>1308</v>
@@ -27691,20 +28118,47 @@
       </c>
       <c r="W63" s="10"/>
     </row>
-    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H65" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J65" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
         <v>1907</v>
       </c>
-      <c r="J65" t="s">
-        <v>1906</v>
-      </c>
-    </row>
-    <row r="66" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H66" t="s">
-        <v>1908</v>
-      </c>
       <c r="J66" t="s">
-        <v>1909</v>
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>2311</v>
+      </c>
+      <c r="J68" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K68" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>2313</v>
+      </c>
+      <c r="J70" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>2363</v>
+      </c>
+      <c r="J73" t="s">
+        <v>2362</v>
       </c>
     </row>
   </sheetData>
@@ -27717,8 +28171,8 @@
   <dimension ref="A1:W113"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9:Q9"/>
+      <pane ySplit="9" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
       <selection activeCell="B44" sqref="B44"/>
@@ -27830,10 +28284,10 @@
         <v>552</v>
       </c>
       <c r="P9" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q9" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R9" s="21" t="s">
         <v>1308</v>
@@ -29272,10 +29726,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:Q8"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
     <sheetView topLeftCell="F1" workbookViewId="1">
       <selection activeCell="H28" sqref="H28"/>
@@ -29383,10 +29837,10 @@
         <v>552</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R8" s="21" t="s">
         <v>1308</v>
@@ -29538,10 +29992,10 @@
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
       <c r="J33" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.25">
@@ -29558,6 +30012,72 @@
       </c>
       <c r="J35" t="s">
         <v>963</v>
+      </c>
+    </row>
+    <row r="38" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="39" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>2318</v>
+      </c>
+      <c r="J39" t="s">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="40" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>2319</v>
+      </c>
+      <c r="J40" t="s">
+        <v>2322</v>
+      </c>
+    </row>
+    <row r="41" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="42" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>663</v>
+      </c>
+      <c r="J42" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="43" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>664</v>
+      </c>
+      <c r="J43" t="s">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="44" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>665</v>
+      </c>
+      <c r="J44" t="s">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="45" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>666</v>
+      </c>
+      <c r="J45" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="48" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>650</v>
+      </c>
+      <c r="J48" t="s">
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -29680,10 +30200,10 @@
         <v>552</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R8" s="21" t="s">
         <v>1308</v>
@@ -30402,10 +30922,10 @@
         <v>552</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R8" s="21" t="s">
         <v>1308</v>
@@ -30446,9 +30966,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="1">
       <selection activeCell="H39" sqref="H39"/>
@@ -30559,10 +31079,10 @@
         <v>552</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="Q10" s="42" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="R10" s="21" t="s">
         <v>1308</v>
@@ -30897,7 +31417,7 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" s="44" t="s">
-        <v>2312</v>
+        <v>2310</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>822</v>
@@ -30917,13 +31437,13 @@
         <v>719</v>
       </c>
       <c r="I41" t="s">
+        <v>2290</v>
+      </c>
+      <c r="N41" t="s">
         <v>2292</v>
       </c>
-      <c r="N41" t="s">
-        <v>2294</v>
-      </c>
       <c r="P41" t="s">
-        <v>2293</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
@@ -30973,7 +31493,7 @@
         <v>706</v>
       </c>
       <c r="L45" t="s">
-        <v>2291</v>
+        <v>2289</v>
       </c>
       <c r="R45">
         <v>2008</v>
@@ -31024,7 +31544,7 @@
         <v>708</v>
       </c>
       <c r="N48" t="s">
-        <v>2290</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="49" spans="3:21" x14ac:dyDescent="0.25">
@@ -31058,13 +31578,13 @@
         <v>709</v>
       </c>
       <c r="N50" t="s">
+        <v>2284</v>
+      </c>
+      <c r="P50" t="s">
         <v>2286</v>
       </c>
-      <c r="P50" t="s">
-        <v>2288</v>
-      </c>
       <c r="Q50" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="51" spans="3:21" x14ac:dyDescent="0.25">
@@ -31075,7 +31595,7 @@
         <v>714</v>
       </c>
       <c r="I51" t="s">
-        <v>2289</v>
+        <v>2287</v>
       </c>
       <c r="J51" t="s">
         <v>711</v>
@@ -32281,10 +32801,10 @@
         <v>1166</v>
       </c>
       <c r="H150" t="s">
-        <v>2295</v>
+        <v>2293</v>
       </c>
       <c r="I150" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="151" spans="2:21" x14ac:dyDescent="0.25">
@@ -32292,13 +32812,13 @@
         <v>1166</v>
       </c>
       <c r="H151" t="s">
-        <v>2296</v>
+        <v>2294</v>
       </c>
       <c r="I151" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="N151" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="152" spans="2:21" x14ac:dyDescent="0.25">
@@ -32306,10 +32826,10 @@
         <v>1166</v>
       </c>
       <c r="H152" t="s">
-        <v>2297</v>
+        <v>2295</v>
       </c>
       <c r="I152" t="s">
-        <v>2302</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="153" spans="2:21" x14ac:dyDescent="0.25">
@@ -32317,18 +32837,18 @@
         <v>1166</v>
       </c>
       <c r="H153" t="s">
-        <v>2298</v>
+        <v>2296</v>
       </c>
       <c r="I153" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="154" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H154" t="s">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="I154" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="157" spans="2:21" x14ac:dyDescent="0.25">
@@ -32336,7 +32856,7 @@
         <v>1166</v>
       </c>
       <c r="H157" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="158" spans="2:21" x14ac:dyDescent="0.25">
@@ -32344,7 +32864,7 @@
         <v>1166</v>
       </c>
       <c r="H158" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="159" spans="2:21" x14ac:dyDescent="0.25">
@@ -32352,7 +32872,7 @@
         <v>1166</v>
       </c>
       <c r="H159" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="160" spans="2:21" x14ac:dyDescent="0.25">
@@ -32360,7 +32880,7 @@
         <v>1166</v>
       </c>
       <c r="H160" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="161" spans="3:8" x14ac:dyDescent="0.25">
@@ -32368,12 +32888,12 @@
         <v>1166</v>
       </c>
       <c r="H161" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="162" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H162" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extending out EBRD materials
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="-345" windowWidth="15255" windowHeight="10155" tabRatio="810" activeTab="2"/>
-    <workbookView xWindow="10905" yWindow="-30" windowWidth="6150" windowHeight="9780" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="2640" windowWidth="14565" windowHeight="7590" tabRatio="810"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5476" uniqueCount="2374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5451" uniqueCount="2400">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -6958,9 +6957,6 @@
     <t>Procurement Policies and Proceedures, 2009</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Proposed Adoption and Application of World Bank Performance Standards for Private Sector Projects Supported by IBRD/IDA (English)</t>
   </si>
   <si>
@@ -7148,6 +7144,87 @@
   </si>
   <si>
     <t xml:space="preserve">Improving Project Outcomes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2003 Environmental Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Политика ЕБРР в отношении охраны окружающей среды (RUS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Okolisna politika (BiH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ekologická politika (CZR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Keskkonnapoliitika (EST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Politika zastite okolisa (CRO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Környezeti politikája (HUN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aplinkos apsaugos politika (LIT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Vides aizsardzības politika (LAT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Polityka ochrony srodowiska (POL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Politica de mediu (ROM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ekologická politika (SLK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Okoljska politika (SVN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Politika zastite zivotne sredine (SER)</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/cs/Satellite?c=Content&amp;cid=1395241492866&amp;d=&amp;pagename=EBRD%2FContent%2FContentLayout</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/russia03.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/bosnia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/estonia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/croatia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/hungary.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/lith.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/latvia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/polish.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/romania.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/slovak.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/slovenia.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ebrd.com/downloads/research/policies/serbia.pdf</t>
   </si>
 </sst>
 </file>
@@ -7733,11 +7810,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X146"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K146" sqref="K146"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11155,15 +11231,15 @@
     </row>
     <row r="145" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H145" t="s">
+        <v>2370</v>
+      </c>
+      <c r="J145" t="s">
         <v>2371</v>
-      </c>
-      <c r="J145" t="s">
-        <v>2372</v>
       </c>
     </row>
     <row r="146" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H146" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="K146" t="s">
         <v>1178</v>
@@ -11182,7 +11258,6 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11365,31 +11440,31 @@
     </row>
     <row r="17" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
+        <v>2363</v>
+      </c>
+      <c r="J17" t="s">
         <v>2364</v>
-      </c>
-      <c r="J17" t="s">
-        <v>2365</v>
       </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
+        <v>2365</v>
+      </c>
+      <c r="J18" t="s">
         <v>2366</v>
-      </c>
-      <c r="J18" t="s">
-        <v>2367</v>
       </c>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
+        <v>2367</v>
+      </c>
+      <c r="J19" t="s">
         <v>2368</v>
-      </c>
-      <c r="J19" t="s">
-        <v>2369</v>
       </c>
     </row>
     <row r="21" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="J21" t="s">
         <v>711</v>
@@ -11407,7 +11482,6 @@
     <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11608,7 +11682,6 @@
     <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11732,31 +11805,31 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J11" t="s">
         <v>2325</v>
-      </c>
-      <c r="J11" t="s">
-        <v>2326</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J12" t="s">
         <v>2327</v>
-      </c>
-      <c r="J12" t="s">
-        <v>2328</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J13" t="s">
         <v>2329</v>
-      </c>
-      <c r="J13" t="s">
-        <v>2330</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="J14" t="s">
         <v>843</v>
@@ -11764,7 +11837,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="J15" t="s">
         <v>839</v>
@@ -11772,7 +11845,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="K16" t="s">
         <v>838</v>
@@ -11796,122 +11869,122 @@
     </row>
     <row r="20" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="J20" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="22" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="J22" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="23" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J23" t="s">
         <v>2338</v>
-      </c>
-      <c r="J23" t="s">
-        <v>2339</v>
       </c>
     </row>
     <row r="25" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="K25" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="26" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="K26" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="27" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="K27" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="28" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="K28" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="29" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="K29" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="31" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
+        <v>2349</v>
+      </c>
+      <c r="J31" t="s">
         <v>2350</v>
-      </c>
-      <c r="J31" t="s">
-        <v>2351</v>
       </c>
     </row>
     <row r="33" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="K33" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="34" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="K34" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="35" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="K35" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="36" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="K36" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="39" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
+        <v>2359</v>
+      </c>
+      <c r="J39" t="s">
         <v>2360</v>
-      </c>
-      <c r="J39" t="s">
-        <v>2361</v>
       </c>
     </row>
     <row r="41" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J41" t="s">
         <v>2327</v>
-      </c>
-      <c r="J41" t="s">
-        <v>2328</v>
       </c>
     </row>
   </sheetData>
@@ -11926,7 +11999,6 @@
     <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N8" sqref="N8:Q8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12356,10 +12428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD624"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -27559,7 +27630,6 @@
     <sheetView topLeftCell="F52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H80" sqref="H80"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28123,7 +28193,7 @@
         <v>1906</v>
       </c>
       <c r="J65" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="66" spans="8:11" x14ac:dyDescent="0.25">
@@ -28131,34 +28201,34 @@
         <v>1907</v>
       </c>
       <c r="J66" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="68" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H68" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="J68" t="s">
         <v>1247</v>
       </c>
       <c r="K68" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="70" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H70" t="s">
+        <v>2312</v>
+      </c>
+      <c r="J70" t="s">
         <v>2313</v>
-      </c>
-      <c r="J70" t="s">
-        <v>2314</v>
       </c>
     </row>
     <row r="73" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H73" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="J73" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
     </row>
   </sheetData>
@@ -28173,9 +28243,6 @@
     <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
-    </sheetView>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29731,9 +29798,6 @@
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
-    <sheetView topLeftCell="F1" workbookViewId="1">
-      <selection activeCell="H28" sqref="H28"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30016,28 +30080,28 @@
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="J39" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="J40" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.25">
@@ -30053,7 +30117,7 @@
         <v>664</v>
       </c>
       <c r="J43" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.25">
@@ -30061,7 +30125,7 @@
         <v>665</v>
       </c>
       <c r="J44" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.25">
@@ -30089,12 +30153,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N8" sqref="N8:Q8"/>
-    </sheetView>
-    <sheetView topLeftCell="E55" workbookViewId="1">
-      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30817,7 +30878,6 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N8" sqref="N8:Q8"/>
     </sheetView>
-    <sheetView topLeftCell="D1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30964,14 +31024,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V162"/>
+  <dimension ref="A2:V178"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="1">
-      <selection activeCell="H39" sqref="H39"/>
+      <pane ySplit="10" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31126,9 +31183,6 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
-        <v>1165</v>
-      </c>
       <c r="C14" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31140,9 +31194,6 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
-        <v>1165</v>
-      </c>
       <c r="C15" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31154,9 +31205,6 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
-        <v>1165</v>
-      </c>
       <c r="C16" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31167,10 +31215,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31181,10 +31226,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31198,40 +31240,37 @@
         <v>799</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H19" s="14" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H20" s="14" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H21" s="14" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H22" s="14" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H23" s="14" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H24" s="14" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31242,25 +31281,22 @@
         <v>800</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H26" s="14" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H27" s="14" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H28" s="14" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31274,10 +31310,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31288,10 +31321,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C31" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31302,10 +31332,8 @@
         <v>803</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
-        <v>1165</v>
-      </c>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="14"/>
       <c r="H32" t="s">
         <v>741</v>
       </c>
@@ -31313,7 +31341,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H33" s="14" t="s">
         <v>712</v>
       </c>
@@ -31327,8 +31355,8 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B34" s="44" t="s">
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C34" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H34" t="s">
@@ -31338,7 +31366,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -31351,7 +31379,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H36" s="37"/>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
@@ -31367,7 +31395,7 @@
       <c r="T36" s="38"/>
       <c r="U36" s="37"/>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H37" s="23" t="s">
         <v>849</v>
       </c>
@@ -31381,7 +31409,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H38" s="27" t="s">
         <v>707</v>
       </c>
@@ -31398,7 +31426,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C39" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31415,10 +31443,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C40" s="44" t="s">
-        <v>2310</v>
-      </c>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H40" s="14" t="s">
         <v>822</v>
       </c>
@@ -31429,7 +31454,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C41" s="44" t="s">
         <v>1165</v>
       </c>
@@ -31446,7 +31471,7 @@
         <v>2291</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H42" s="14" t="s">
         <v>825</v>
       </c>
@@ -31460,7 +31485,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H43" s="11" t="s">
         <v>824</v>
       </c>
@@ -31471,7 +31496,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H44" s="14" t="s">
         <v>823</v>
       </c>
@@ -31482,7 +31507,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
         <v>717</v>
       </c>
@@ -31499,7 +31524,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H46" s="14" t="s">
         <v>849</v>
       </c>
@@ -31513,7 +31538,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C47" s="29" t="s">
         <v>1166</v>
       </c>
@@ -31533,7 +31558,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C48" s="29" t="s">
         <v>1166</v>
       </c>
@@ -31547,506 +31572,430 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C49" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H49" t="s">
+    <row r="49" spans="8:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="38"/>
+      <c r="U49" s="37"/>
+    </row>
+    <row r="50" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>2373</v>
+      </c>
+      <c r="I50" t="s">
+        <v>708</v>
+      </c>
+      <c r="J50" t="s">
+        <v>2387</v>
+      </c>
+    </row>
+    <row r="51" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>2374</v>
+      </c>
+      <c r="I51" t="s">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="52" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>2375</v>
+      </c>
+      <c r="I52" t="s">
+        <v>2389</v>
+      </c>
+    </row>
+    <row r="53" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>2376</v>
+      </c>
+      <c r="I53" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="54" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>2377</v>
+      </c>
+      <c r="I54" t="s">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="55" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>2378</v>
+      </c>
+      <c r="I55" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="56" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>2379</v>
+      </c>
+      <c r="I56" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="57" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>2380</v>
+      </c>
+      <c r="I57" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="58" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>2381</v>
+      </c>
+      <c r="I58" t="s">
+        <v>2394</v>
+      </c>
+    </row>
+    <row r="59" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>2382</v>
+      </c>
+      <c r="I59" t="s">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="60" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>2383</v>
+      </c>
+      <c r="I60" t="s">
+        <v>2396</v>
+      </c>
+    </row>
+    <row r="61" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>2384</v>
+      </c>
+      <c r="I61" t="s">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="62" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>2385</v>
+      </c>
+      <c r="I62" t="s">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="63" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>2386</v>
+      </c>
+      <c r="I63" t="s">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="64" spans="8:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" s="37"/>
+      <c r="P64" s="37"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="37"/>
+      <c r="S64" s="37"/>
+      <c r="T64" s="38"/>
+      <c r="U64" s="37"/>
+    </row>
+    <row r="65" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C65" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H65" t="s">
         <v>715</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I65" t="s">
         <v>709</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J65" t="s">
         <v>711</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L65" t="s">
         <v>710</v>
       </c>
-      <c r="R49">
+      <c r="R65">
         <v>1996</v>
       </c>
     </row>
-    <row r="50" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C50" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H50" t="s">
+    <row r="66" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C66" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H66" t="s">
         <v>715</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I66" t="s">
         <v>709</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N66" t="s">
         <v>2284</v>
       </c>
-      <c r="P50" t="s">
+      <c r="P66" t="s">
         <v>2286</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="Q66" t="s">
         <v>2285</v>
       </c>
     </row>
-    <row r="51" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C51" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H51" t="s">
+    <row r="67" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C67" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H67" t="s">
         <v>714</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I67" t="s">
         <v>2287</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J67" t="s">
         <v>711</v>
       </c>
-      <c r="R51">
+      <c r="R67">
         <v>1992</v>
       </c>
     </row>
-    <row r="52" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
-      <c r="M52" s="37"/>
-      <c r="N52" s="37"/>
-      <c r="O52" s="37"/>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="37"/>
-      <c r="R52" s="37"/>
-      <c r="S52" s="37"/>
-      <c r="T52" s="38"/>
-      <c r="U52" s="37"/>
-    </row>
-    <row r="53" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H53" s="18" t="s">
+    <row r="68" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+      <c r="S68" s="37"/>
+      <c r="T68" s="38"/>
+      <c r="U68" s="37"/>
+    </row>
+    <row r="69" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="18" t="s">
         <v>1061</v>
       </c>
-      <c r="I53" s="18" t="s">
+      <c r="I69" s="18" t="s">
         <v>1071</v>
       </c>
-      <c r="T53" s="43"/>
-    </row>
-    <row r="54" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H54" s="18" t="s">
+      <c r="T69" s="43"/>
+    </row>
+    <row r="70" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="18" t="s">
         <v>1062</v>
       </c>
-      <c r="I54" s="18" t="s">
+      <c r="I70" s="18" t="s">
         <v>1072</v>
       </c>
-      <c r="T54" s="43"/>
-    </row>
-    <row r="55" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H55" s="18" t="s">
+      <c r="T70" s="43"/>
+    </row>
+    <row r="71" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="18" t="s">
         <v>1063</v>
       </c>
-      <c r="I55" s="18" t="s">
+      <c r="I71" s="18" t="s">
         <v>1073</v>
       </c>
-      <c r="T55" s="43"/>
-    </row>
-    <row r="56" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H56" s="18" t="s">
+      <c r="T71" s="43"/>
+    </row>
+    <row r="72" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="18" t="s">
         <v>1064</v>
       </c>
-      <c r="I56" s="18" t="s">
+      <c r="I72" s="18" t="s">
         <v>1074</v>
       </c>
-      <c r="T56" s="43"/>
-    </row>
-    <row r="57" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H57" s="18" t="s">
+      <c r="T72" s="43"/>
+    </row>
+    <row r="73" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="18" t="s">
         <v>1065</v>
       </c>
-      <c r="I57" s="18" t="s">
+      <c r="I73" s="18" t="s">
         <v>1075</v>
       </c>
-      <c r="T57" s="43"/>
-    </row>
-    <row r="58" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H58" s="18" t="s">
+      <c r="T73" s="43"/>
+    </row>
+    <row r="74" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="18" t="s">
         <v>1066</v>
       </c>
-      <c r="I58" s="18" t="s">
+      <c r="I74" s="18" t="s">
         <v>1076</v>
       </c>
-      <c r="T58" s="43"/>
-    </row>
-    <row r="59" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H59" s="18" t="s">
+      <c r="T74" s="43"/>
+    </row>
+    <row r="75" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="18" t="s">
         <v>1067</v>
       </c>
-      <c r="I59" s="18" t="s">
+      <c r="I75" s="18" t="s">
         <v>1077</v>
       </c>
-      <c r="T59" s="43"/>
-    </row>
-    <row r="60" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H60" s="18" t="s">
+      <c r="T75" s="43"/>
+    </row>
+    <row r="76" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="18" t="s">
         <v>1068</v>
       </c>
-      <c r="I60" s="18" t="s">
+      <c r="I76" s="18" t="s">
         <v>1078</v>
       </c>
-      <c r="T60" s="43"/>
-    </row>
-    <row r="61" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H61" s="18" t="s">
+      <c r="T76" s="43"/>
+    </row>
+    <row r="77" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H77" s="18" t="s">
         <v>1069</v>
       </c>
-      <c r="I61" s="18" t="s">
+      <c r="I77" s="18" t="s">
         <v>1079</v>
       </c>
-      <c r="T61" s="43"/>
-    </row>
-    <row r="62" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H62" s="18" t="s">
+      <c r="T77" s="43"/>
+    </row>
+    <row r="78" spans="3:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H78" s="18" t="s">
         <v>1070</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I78" s="18" t="s">
         <v>1080</v>
       </c>
-      <c r="T62" s="43"/>
-    </row>
-    <row r="63" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H63" s="37"/>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="37"/>
-      <c r="L63" s="37"/>
-      <c r="M63" s="37"/>
-      <c r="N63" s="37"/>
-      <c r="O63" s="37"/>
-      <c r="P63" s="37"/>
-      <c r="Q63" s="37"/>
-      <c r="R63" s="37"/>
-      <c r="S63" s="37"/>
-      <c r="T63" s="38"/>
-      <c r="U63" s="37"/>
-    </row>
-    <row r="64" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
-    </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B65" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C65" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H65" t="s">
-        <v>742</v>
-      </c>
-      <c r="I65" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H66" s="14" t="s">
-        <v>848</v>
-      </c>
-      <c r="I66" t="s">
-        <v>847</v>
-      </c>
-      <c r="J66" t="s">
-        <v>846</v>
-      </c>
-      <c r="R66">
-        <v>2010</v>
-      </c>
-      <c r="S66" t="s">
-        <v>187</v>
-      </c>
-      <c r="T66">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B67" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C67" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H67" t="s">
-        <v>725</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H68" s="14" t="s">
-        <v>725</v>
-      </c>
-      <c r="I68" t="s">
-        <v>728</v>
-      </c>
-      <c r="J68" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B69" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C69" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H69" t="s">
-        <v>743</v>
-      </c>
-      <c r="I69" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B70" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C70" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H70" t="s">
-        <v>744</v>
-      </c>
-      <c r="J70" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B71" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C71" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H71" t="s">
-        <v>745</v>
-      </c>
-      <c r="J71" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B72" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C72" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H72" t="s">
-        <v>746</v>
-      </c>
-      <c r="I72" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B73" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C73" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H73" t="s">
-        <v>747</v>
-      </c>
-      <c r="I73" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B74" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C74" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H74" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B75" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C75" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H75" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H76" s="14" t="s">
-        <v>829</v>
-      </c>
-      <c r="I76" t="s">
-        <v>833</v>
-      </c>
-      <c r="J76" t="s">
-        <v>835</v>
-      </c>
-      <c r="L76" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H77" s="14" t="s">
-        <v>830</v>
-      </c>
-      <c r="I77" t="s">
-        <v>834</v>
-      </c>
-      <c r="L77" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B78" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C78" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H78" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="4"/>
-      <c r="R79" s="4"/>
-    </row>
-    <row r="80" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H80" s="37"/>
-      <c r="I80" s="37"/>
-      <c r="J80" s="37"/>
-      <c r="K80" s="37"/>
-      <c r="L80" s="37"/>
-      <c r="M80" s="37"/>
-      <c r="N80" s="37"/>
-      <c r="O80" s="37"/>
-      <c r="P80" s="37"/>
-      <c r="Q80" s="37"/>
-      <c r="R80" s="37"/>
-      <c r="S80" s="37"/>
-      <c r="T80" s="38"/>
-      <c r="U80" s="37"/>
+      <c r="T78" s="43"/>
+    </row>
+    <row r="79" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
+      <c r="L79" s="37"/>
+      <c r="M79" s="37"/>
+      <c r="N79" s="37"/>
+      <c r="O79" s="37"/>
+      <c r="P79" s="37"/>
+      <c r="Q79" s="37"/>
+      <c r="R79" s="37"/>
+      <c r="S79" s="37"/>
+      <c r="T79" s="38"/>
+      <c r="U79" s="37"/>
+    </row>
+    <row r="80" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
     </row>
     <row r="81" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C81" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H81" t="s">
-        <v>720</v>
+        <v>742</v>
       </c>
       <c r="I81" t="s">
-        <v>721</v>
-      </c>
-      <c r="J81" t="s">
-        <v>726</v>
-      </c>
-      <c r="R81">
-        <v>2014</v>
-      </c>
-      <c r="S81" t="s">
-        <v>192</v>
+        <v>805</v>
       </c>
     </row>
     <row r="82" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H82" t="s">
-        <v>722</v>
-      </c>
-      <c r="K82" t="s">
-        <v>724</v>
+      <c r="H82" s="14" t="s">
+        <v>848</v>
+      </c>
+      <c r="I82" t="s">
+        <v>847</v>
+      </c>
+      <c r="J82" t="s">
+        <v>846</v>
+      </c>
+      <c r="R82">
+        <v>2010</v>
+      </c>
+      <c r="S82" t="s">
+        <v>187</v>
+      </c>
+      <c r="T82">
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C83" s="44" t="s">
+        <v>1165</v>
+      </c>
       <c r="H83" t="s">
-        <v>723</v>
+        <v>725</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="84" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H84" s="14" t="s">
-        <v>828</v>
+        <v>725</v>
       </c>
       <c r="I84" t="s">
-        <v>832</v>
+        <v>728</v>
       </c>
       <c r="J84" t="s">
-        <v>726</v>
-      </c>
-      <c r="L84" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="85" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C85" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H85" t="s">
+        <v>743</v>
+      </c>
+      <c r="I85" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="86" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C86" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H86" t="s">
+        <v>744</v>
+      </c>
+      <c r="J86" t="s">
         <v>797</v>
       </c>
-      <c r="R84">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="85" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H85" s="14" t="s">
-        <v>722</v>
-      </c>
-      <c r="I85" t="s">
-        <v>724</v>
-      </c>
-      <c r="J85" t="s">
-        <v>726</v>
-      </c>
-      <c r="L85" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="86" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H86" s="37"/>
-      <c r="I86" s="37"/>
-      <c r="J86" s="37"/>
-      <c r="K86" s="37"/>
-      <c r="L86" s="37"/>
-      <c r="M86" s="37"/>
-      <c r="N86" s="37"/>
-      <c r="O86" s="37"/>
-      <c r="P86" s="37"/>
-      <c r="Q86" s="37"/>
-      <c r="R86" s="37"/>
-      <c r="S86" s="37"/>
-      <c r="T86" s="38"/>
-      <c r="U86" s="37"/>
     </row>
     <row r="87" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
-      <c r="Q87" s="4"/>
-      <c r="R87" s="4"/>
+      <c r="C87" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H87" t="s">
+        <v>745</v>
+      </c>
+      <c r="J87" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="88" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C88" s="44" t="s">
@@ -32055,844 +32004,939 @@
       <c r="H88" t="s">
         <v>746</v>
       </c>
+      <c r="I88" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="89" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C89" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H89" t="s">
-        <v>750</v>
+        <v>747</v>
+      </c>
+      <c r="I89" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="90" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C90" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H90" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="91" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H91" s="5" t="s">
-        <v>729</v>
-      </c>
-      <c r="J91" t="s">
-        <v>794</v>
+      <c r="C91" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H91" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="92" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C92" s="44" t="s">
+      <c r="H92" s="14" t="s">
+        <v>829</v>
+      </c>
+      <c r="I92" t="s">
+        <v>833</v>
+      </c>
+      <c r="J92" t="s">
+        <v>835</v>
+      </c>
+      <c r="L92" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="93" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H93" s="14" t="s">
+        <v>830</v>
+      </c>
+      <c r="I93" t="s">
+        <v>834</v>
+      </c>
+      <c r="L93" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="94" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C94" s="44" t="s">
         <v>1165</v>
       </c>
-      <c r="H92" t="s">
-        <v>751</v>
-      </c>
-      <c r="I92" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="93" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H93" s="23" t="s">
-        <v>989</v>
-      </c>
-      <c r="I93" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="94" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H94" s="23" t="s">
-        <v>990</v>
-      </c>
-      <c r="K94" t="s">
-        <v>1002</v>
+      <c r="H94" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="95" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="H95" s="23" t="s">
-        <v>991</v>
-      </c>
-      <c r="J95" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="96" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C96" s="44" t="s">
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="4"/>
+    </row>
+    <row r="96" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="37"/>
+      <c r="K96" s="37"/>
+      <c r="L96" s="37"/>
+      <c r="M96" s="37"/>
+      <c r="N96" s="37"/>
+      <c r="O96" s="37"/>
+      <c r="P96" s="37"/>
+      <c r="Q96" s="37"/>
+      <c r="R96" s="37"/>
+      <c r="S96" s="37"/>
+      <c r="T96" s="38"/>
+      <c r="U96" s="37"/>
+    </row>
+    <row r="97" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C97" s="44" t="s">
         <v>1165</v>
       </c>
-      <c r="H96" t="s">
-        <v>752</v>
-      </c>
-      <c r="I96" s="29" t="s">
-        <v>1005</v>
-      </c>
-      <c r="J96" t="s">
-        <v>1004</v>
-      </c>
-      <c r="K96" s="16"/>
-      <c r="L96" t="s">
-        <v>1009</v>
-      </c>
-      <c r="N96" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="97" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H97" s="23" t="s">
-        <v>994</v>
-      </c>
-      <c r="K97" t="s">
-        <v>1006</v>
-      </c>
-      <c r="L97" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="98" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H98" s="23" t="s">
-        <v>1007</v>
-      </c>
-      <c r="I98" s="29" t="s">
-        <v>1008</v>
-      </c>
-      <c r="K98" s="16"/>
-    </row>
-    <row r="99" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C99" s="44" t="s">
+      <c r="H97" t="s">
+        <v>720</v>
+      </c>
+      <c r="I97" t="s">
+        <v>721</v>
+      </c>
+      <c r="J97" t="s">
+        <v>726</v>
+      </c>
+      <c r="R97">
+        <v>2014</v>
+      </c>
+      <c r="S97" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="98" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>722</v>
+      </c>
+      <c r="K98" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="99" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="100" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H100" s="14" t="s">
+        <v>828</v>
+      </c>
+      <c r="I100" t="s">
+        <v>832</v>
+      </c>
+      <c r="J100" t="s">
+        <v>726</v>
+      </c>
+      <c r="L100" t="s">
+        <v>797</v>
+      </c>
+      <c r="R100">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="101" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H101" s="14" t="s">
+        <v>722</v>
+      </c>
+      <c r="I101" t="s">
+        <v>724</v>
+      </c>
+      <c r="J101" t="s">
+        <v>726</v>
+      </c>
+      <c r="L101" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="102" spans="3:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+      <c r="J102" s="37"/>
+      <c r="K102" s="37"/>
+      <c r="L102" s="37"/>
+      <c r="M102" s="37"/>
+      <c r="N102" s="37"/>
+      <c r="O102" s="37"/>
+      <c r="P102" s="37"/>
+      <c r="Q102" s="37"/>
+      <c r="R102" s="37"/>
+      <c r="S102" s="37"/>
+      <c r="T102" s="38"/>
+      <c r="U102" s="37"/>
+    </row>
+    <row r="103" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="4"/>
+    </row>
+    <row r="104" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C104" s="44" t="s">
         <v>1165</v>
       </c>
-      <c r="H99" t="s">
-        <v>753</v>
-      </c>
-      <c r="I99" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J99" t="s">
-        <v>992</v>
-      </c>
-      <c r="L99" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="100" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H100" s="23" t="s">
-        <v>990</v>
-      </c>
-      <c r="K100" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="101" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H101" t="s">
-        <v>754</v>
-      </c>
-      <c r="J101" t="s">
-        <v>1012</v>
-      </c>
-      <c r="L101" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="102" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H102" s="23" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="103" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C103" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H103" t="s">
-        <v>755</v>
-      </c>
-      <c r="I103" t="s">
-        <v>1015</v>
-      </c>
-      <c r="L103" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="104" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H104" s="23" t="s">
-        <v>722</v>
-      </c>
-      <c r="I104" t="s">
-        <v>1014</v>
-      </c>
-      <c r="L104" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="105" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="105" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C105" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H105" t="s">
-        <v>756</v>
-      </c>
-      <c r="I105" t="s">
-        <v>1016</v>
-      </c>
-      <c r="N105" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="106" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H106" s="23" t="s">
-        <v>995</v>
-      </c>
-      <c r="K106" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="107" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C107" s="44" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="107" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H107" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="J107" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="108" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C108" s="44" t="s">
         <v>1165</v>
       </c>
-      <c r="H107" t="s">
-        <v>757</v>
-      </c>
-      <c r="I107" t="s">
-        <v>1020</v>
-      </c>
-      <c r="L107" t="s">
+      <c r="H108" t="s">
+        <v>751</v>
+      </c>
+      <c r="I108" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="109" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H109" s="23" t="s">
+        <v>989</v>
+      </c>
+      <c r="I109" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="110" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H110" s="23" t="s">
+        <v>990</v>
+      </c>
+      <c r="K110" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="111" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="H111" s="23" t="s">
+        <v>991</v>
+      </c>
+      <c r="J111" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="112" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C112" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H112" t="s">
+        <v>752</v>
+      </c>
+      <c r="I112" s="29" t="s">
+        <v>1005</v>
+      </c>
+      <c r="J112" t="s">
+        <v>1004</v>
+      </c>
+      <c r="K112" s="16"/>
+      <c r="L112" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="108" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="H108" s="23" t="s">
-        <v>995</v>
-      </c>
-      <c r="K108" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="109" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C109" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H109" t="s">
-        <v>758</v>
-      </c>
-      <c r="I109" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="110" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C110" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H110" t="s">
-        <v>759</v>
-      </c>
-      <c r="I110" t="s">
-        <v>997</v>
-      </c>
-      <c r="J110" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="111" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C111" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H111" t="s">
-        <v>760</v>
-      </c>
-      <c r="I111" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H113" s="5" t="s">
-        <v>730</v>
-      </c>
-      <c r="J113" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B114" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C114" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H114" t="s">
-        <v>761</v>
-      </c>
-      <c r="I114" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B115" s="44" t="s">
-        <v>1165</v>
-      </c>
+      <c r="N112" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="113" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H113" s="23" t="s">
+        <v>994</v>
+      </c>
+      <c r="K113" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L113" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="114" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H114" s="23" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I114" s="29" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K114" s="16"/>
+    </row>
+    <row r="115" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C115" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H115" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
       <c r="I115" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B116" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C116" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H116" t="s">
-        <v>763</v>
-      </c>
-      <c r="I116" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B117" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C117" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1011</v>
+      </c>
+      <c r="J115" t="s">
+        <v>992</v>
+      </c>
+      <c r="L115" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="116" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H116" s="23" t="s">
+        <v>990</v>
+      </c>
+      <c r="K116" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="117" spans="3:14" x14ac:dyDescent="0.25">
       <c r="H117" t="s">
-        <v>764</v>
-      </c>
-      <c r="I117" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B118" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C118" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H118" t="s">
-        <v>765</v>
-      </c>
-      <c r="I118" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B119" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>754</v>
+      </c>
+      <c r="J117" t="s">
+        <v>1012</v>
+      </c>
+      <c r="L117" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="118" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H118" s="23" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="119" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C119" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H119" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
       <c r="I119" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B120" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C120" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H120" t="s">
-        <v>767</v>
-      </c>
-      <c r="I120" s="7" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B121" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1015</v>
+      </c>
+      <c r="L119" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="120" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H120" s="23" t="s">
+        <v>722</v>
+      </c>
+      <c r="I120" t="s">
+        <v>1014</v>
+      </c>
+      <c r="L120" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="121" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C121" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H121" t="s">
-        <v>768</v>
+        <v>756</v>
       </c>
       <c r="I121" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B122" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C122" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H122" t="s">
-        <v>769</v>
-      </c>
-      <c r="I122" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B123" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1016</v>
+      </c>
+      <c r="N121" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="122" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H122" s="23" t="s">
+        <v>995</v>
+      </c>
+      <c r="K122" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="123" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C123" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H123" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="I123" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B124" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C124" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H124" t="s">
-        <v>771</v>
-      </c>
-      <c r="I124" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B125" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1020</v>
+      </c>
+      <c r="L123" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="124" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="H124" s="23" t="s">
+        <v>995</v>
+      </c>
+      <c r="K124" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="125" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C125" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H125" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
       <c r="I125" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B126" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="126" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C126" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H126" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="I126" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B127" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>997</v>
+      </c>
+      <c r="J126" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="127" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C127" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H127" t="s">
-        <v>774</v>
+        <v>760</v>
       </c>
       <c r="I127" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B128" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C128" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H128" t="s">
-        <v>775</v>
-      </c>
-      <c r="I128" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B129" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C129" s="44" t="s">
-        <v>1165</v>
-      </c>
-      <c r="H129" t="s">
-        <v>776</v>
-      </c>
-      <c r="I129" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B130" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>998</v>
+      </c>
+    </row>
+    <row r="129" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H129" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="J129" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="130" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C130" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H130" t="s">
-        <v>777</v>
+        <v>761</v>
       </c>
       <c r="I130" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B131" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="131" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C131" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H131" t="s">
-        <v>778</v>
+        <v>762</v>
       </c>
       <c r="I131" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="132" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C132" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H132" t="s">
-        <v>779</v>
+        <v>763</v>
       </c>
       <c r="I132" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B133" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="133" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C133" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H133" t="s">
-        <v>780</v>
+        <v>764</v>
       </c>
       <c r="I133" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B134" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="134" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C134" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H134" t="s">
-        <v>781</v>
+        <v>765</v>
       </c>
       <c r="I134" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B135" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="135" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C135" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H135" t="s">
-        <v>782</v>
+        <v>766</v>
       </c>
       <c r="I135" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B136" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="136" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C136" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H136" t="s">
-        <v>783</v>
-      </c>
-      <c r="I136" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B137" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>767</v>
+      </c>
+      <c r="I136" s="7" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="137" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C137" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H137" t="s">
-        <v>784</v>
+        <v>768</v>
       </c>
       <c r="I137" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B138" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="138" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C138" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H138" t="s">
-        <v>785</v>
+        <v>769</v>
       </c>
       <c r="I138" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B139" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="139" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C139" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H139" t="s">
-        <v>786</v>
+        <v>770</v>
       </c>
       <c r="I139" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B140" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="140" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C140" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H140" t="s">
-        <v>787</v>
+        <v>771</v>
       </c>
       <c r="I140" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B141" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="141" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C141" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H141" t="s">
-        <v>788</v>
+        <v>772</v>
       </c>
       <c r="I141" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B142" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="142" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C142" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H142" t="s">
-        <v>789</v>
+        <v>773</v>
       </c>
       <c r="I142" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B143" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="143" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C143" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H143" t="s">
-        <v>790</v>
+        <v>774</v>
       </c>
       <c r="I143" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B144" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="144" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C144" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H144" t="s">
-        <v>791</v>
+        <v>775</v>
       </c>
       <c r="I144" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="145" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B145" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="145" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C145" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H145" t="s">
-        <v>792</v>
+        <v>776</v>
       </c>
       <c r="I145" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="146" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B146" s="44" t="s">
-        <v>1165</v>
-      </c>
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="146" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C146" s="44" t="s">
         <v>1165</v>
       </c>
       <c r="H146" t="s">
+        <v>777</v>
+      </c>
+      <c r="I146" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="147" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C147" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H147" t="s">
+        <v>778</v>
+      </c>
+      <c r="I147" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="148" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C148" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H148" t="s">
+        <v>779</v>
+      </c>
+      <c r="I148" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="149" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C149" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H149" t="s">
+        <v>780</v>
+      </c>
+      <c r="I149" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="150" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C150" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H150" t="s">
+        <v>781</v>
+      </c>
+      <c r="I150" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="151" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C151" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H151" t="s">
+        <v>782</v>
+      </c>
+      <c r="I151" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="152" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C152" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H152" t="s">
+        <v>783</v>
+      </c>
+      <c r="I152" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="153" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C153" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H153" t="s">
+        <v>784</v>
+      </c>
+      <c r="I153" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="154" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C154" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H154" t="s">
+        <v>785</v>
+      </c>
+      <c r="I154" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="155" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C155" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H155" t="s">
+        <v>786</v>
+      </c>
+      <c r="I155" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="156" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C156" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H156" t="s">
+        <v>787</v>
+      </c>
+      <c r="I156" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="157" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C157" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H157" t="s">
+        <v>788</v>
+      </c>
+      <c r="I157" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="158" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C158" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H158" t="s">
+        <v>789</v>
+      </c>
+      <c r="I158" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="159" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C159" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H159" t="s">
+        <v>790</v>
+      </c>
+      <c r="I159" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="160" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C160" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H160" t="s">
+        <v>791</v>
+      </c>
+      <c r="I160" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="161" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C161" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H161" t="s">
+        <v>792</v>
+      </c>
+      <c r="I161" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="162" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C162" s="44" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H162" t="s">
         <v>793</v>
       </c>
-      <c r="I146" t="s">
+      <c r="I162" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="147" spans="2:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H147" s="35"/>
-      <c r="I147" s="35"/>
-      <c r="J147" s="35"/>
-      <c r="K147" s="35"/>
-      <c r="L147" s="35"/>
-      <c r="M147" s="35"/>
-      <c r="N147" s="35"/>
-      <c r="O147" s="35"/>
-      <c r="P147" s="35"/>
-      <c r="Q147" s="35"/>
-      <c r="R147" s="35"/>
-      <c r="S147" s="35"/>
-      <c r="T147" s="36"/>
-      <c r="U147" s="35"/>
-    </row>
-    <row r="148" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H148" s="37"/>
-      <c r="I148" s="37"/>
-      <c r="J148" s="37"/>
-      <c r="K148" s="37"/>
-      <c r="L148" s="37"/>
-      <c r="M148" s="37"/>
-      <c r="N148" s="37"/>
-      <c r="O148" s="37"/>
-      <c r="P148" s="37"/>
-      <c r="Q148" s="37"/>
-      <c r="R148" s="37"/>
-      <c r="S148" s="37"/>
-      <c r="T148" s="38"/>
-      <c r="U148" s="37"/>
-    </row>
-    <row r="150" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C150" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H150" t="s">
+    <row r="163" spans="2:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B163"/>
+      <c r="H163" s="35"/>
+      <c r="I163" s="35"/>
+      <c r="J163" s="35"/>
+      <c r="K163" s="35"/>
+      <c r="L163" s="35"/>
+      <c r="M163" s="35"/>
+      <c r="N163" s="35"/>
+      <c r="O163" s="35"/>
+      <c r="P163" s="35"/>
+      <c r="Q163" s="35"/>
+      <c r="R163" s="35"/>
+      <c r="S163" s="35"/>
+      <c r="T163" s="36"/>
+      <c r="U163" s="35"/>
+    </row>
+    <row r="164" spans="2:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H164" s="37"/>
+      <c r="I164" s="37"/>
+      <c r="J164" s="37"/>
+      <c r="K164" s="37"/>
+      <c r="L164" s="37"/>
+      <c r="M164" s="37"/>
+      <c r="N164" s="37"/>
+      <c r="O164" s="37"/>
+      <c r="P164" s="37"/>
+      <c r="Q164" s="37"/>
+      <c r="R164" s="37"/>
+      <c r="S164" s="37"/>
+      <c r="T164" s="38"/>
+      <c r="U164" s="37"/>
+    </row>
+    <row r="166" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C166" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H166" t="s">
         <v>2293</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I166" t="s">
         <v>2301</v>
       </c>
     </row>
-    <row r="151" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C151" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H151" t="s">
+    <row r="167" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C167" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H167" t="s">
         <v>2294</v>
       </c>
-      <c r="I151" t="s">
+      <c r="I167" t="s">
         <v>2298</v>
       </c>
-      <c r="N151" t="s">
+      <c r="N167" t="s">
         <v>2299</v>
       </c>
     </row>
-    <row r="152" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C152" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H152" t="s">
+    <row r="168" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C168" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H168" t="s">
         <v>2295</v>
       </c>
-      <c r="I152" t="s">
+      <c r="I168" t="s">
         <v>2300</v>
       </c>
     </row>
-    <row r="153" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C153" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H153" t="s">
+    <row r="169" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C169" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H169" t="s">
         <v>2296</v>
       </c>
-      <c r="I153" t="s">
+      <c r="I169" t="s">
         <v>2302</v>
       </c>
     </row>
-    <row r="154" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H154" t="s">
+    <row r="170" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H170" t="s">
         <v>2297</v>
       </c>
-      <c r="I154" t="s">
+      <c r="I170" t="s">
         <v>2303</v>
       </c>
     </row>
-    <row r="157" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C157" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H157" t="s">
+    <row r="173" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C173" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H173" t="s">
         <v>2304</v>
       </c>
     </row>
-    <row r="158" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C158" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H158" t="s">
+    <row r="174" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C174" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H174" t="s">
         <v>2305</v>
       </c>
     </row>
-    <row r="159" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C159" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H159" t="s">
+    <row r="175" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C175" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H175" t="s">
         <v>2306</v>
       </c>
     </row>
-    <row r="160" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C160" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H160" t="s">
+    <row r="176" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C176" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H176" t="s">
         <v>2307</v>
       </c>
     </row>
-    <row r="161" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C161" s="29" t="s">
-        <v>1166</v>
-      </c>
-      <c r="H161" t="s">
+    <row r="177" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C177" s="29" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H177" t="s">
         <v>2308</v>
       </c>
     </row>
-    <row r="162" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="H162" t="s">
+    <row r="178" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H178" t="s">
         <v>2309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mid-progress update: cleaning up IFC lists
</commit_message>
<xml_diff>
--- a/context/social-policy_ifi.xlsx
+++ b/context/social-policy_ifi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-135" windowWidth="14010" windowHeight="6300" tabRatio="810" activeTab="2"/>
-    <workbookView xWindow="300" yWindow="1770" windowWidth="15900" windowHeight="9345" activeTab="4"/>
+    <workbookView xWindow="300" yWindow="1770" windowWidth="15900" windowHeight="9345" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ADB_policy" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5587" uniqueCount="2465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5777" uniqueCount="2572">
   <si>
     <t>http://www.adb.org/documents/operations-manual</t>
   </si>
@@ -7279,6 +7279,9 @@
     <t>Guidance Note 8: Cultural Heritage</t>
   </si>
   <si>
+    <t>Interpretation Notes</t>
+  </si>
+  <si>
     <t>Interpretation Note on Small and Medium Enterprises and Environmental and Social Risk Management</t>
   </si>
   <si>
@@ -7421,6 +7424,324 @@
   </si>
   <si>
     <t>[akd] status unknown</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/de7d92804a29ffe9ae04af8969adcc27/InterpretationNote_SME_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/38d1a68049ddf966af3cbfda80c2ddf3/InterpretationNote_FIs_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/cd44c6004b8bbc068dbccfbbd578891b/PS_Russian_2012_Full-Document.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/5fd142004a585f48ba3ebf8969adcc27/PS_Chinese_2012_Full-Document.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/38fb14804a58c83480548f8969adcc27/PS_French_2012_Full-Document.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/2ba0a28048855498b37cf36a6515bb18/IFC%2BPerformance%2BStandards_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322804154893</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/103e500048855c6d8bccdb6a6515bb18/IFC%2BPerformance%2BStandards_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322804248148</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/47ebf4804885535daeacfe6a6515bb18/IFC%2BPerformance%2BStandards_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322804023916</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/f33d1f00488559d78444d66a6515bb18/Full_Updated%2BGN_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322804459439</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/9fb7150048855c138af4da6a6515bb18/2007%2BUpdated%2BGuidance%2BNotes_full.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322804281925</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/110fad0048855bad89acdb6a6515bb18/FULL_Updated%2BGN%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322804326163</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/3be1a68049a78dc8b7e4f7a8c6a8312a/PS1_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/b29a4600498009cfa7fcf7336b93d75f/Updated_GN1-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/2408320049a78e5db7f4f7a8c6a8312a/PS2_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/0d7a4480498007faa1f7f3336b93d75f/Updated_GN2-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/25356f8049a78eeeb804faa8c6a8312a/PS3_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/9187330049800a6baa9cfa336b93d75f/Updated_GN3-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/myconnect/topics_ext_content/ifc_external_corporate_site/ifc+sustainability/sustainability+framework/environmental%2C+health%2C+and+safety+guidelines/ehsguidelines?contentIDR=c0e9498048d2e4ada300bf4b02f32852&amp;useDefaultText=0&amp;useDefaultDesc=0</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/a40bc60049a78f49b80efaa8c6a8312a/PS4_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/dc3f4b80498007dca17ff3336b93d75f/Updated_GN4-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/3d82c70049a79073b82cfaa8c6a8312a/PS5_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/4b976700498008d3a417f6336b93d75f/Updated_GN5-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/bff0a28049a790d6b835faa8c6a8312a/PS6_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/a359a380498007e9a1b7f3336b93d75f/Updated_GN6-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/1ee7038049a79139b845faa8c6a8312a/PS7_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/50eed180498009f9a89bfa336b93d75f/Updated_GN7-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/dd8d3d0049a791a6b855faa8c6a8312a/PS8_English_2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/39e39000498007fda1fff3336b93d75f/Updated_GN8-2012.pdf?MOD=AJPERES</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 1: Social and Environmental Assessment and Management Systems</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 1: Social and Environmental Assessment and Management Systems</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 2: Labor and Working Conditions</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 2: Labor and Working Conditions</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 3: Pollution Prevention and Abatement</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 3: Pollution Prevention and Abatement</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 4: Community Health, Safety and Security</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 4: Community Health, Safety and Security</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 5: Land Acquisition and Involuntary Resettlement</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 5: Land Acquisition and Involuntary Resettlement</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 6: Biodiversity Conservation and Sustainable Natural Resource Management</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 6: Biodiversity Conservation and Sustainable Natural Resource Management</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 7: Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 7: Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>2006 Performance Standard 8: Cultural Heritage</t>
+  </si>
+  <si>
+    <t>2006 Guidance Note 8: Cultural Heritage</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/88eb4e0048855668b9f4fb6a6515bb18/PS_1_SocEnvAssessmentMgmt.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807400673</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/095daa8048855833bf44ff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_1.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807644793</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/a23dcb8048855663b9e4fb6a6515bb18/PS_2_LaborWorkingConditions.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807958114</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/2398880048855835bf4cff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_2.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808277977</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/09f3170048855662b9dcfb6a6515bb18/PS_3_PollutionPreventionAbatement.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808694555</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/ea62170048855838bf5cff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_3.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808945083</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/6a8055004885565eb9ccfb6a6515bb18/PS_4_CommHealthSafetySecurity.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322815748639</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/4af353004885583dbf6cff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_4.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816293559</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/79fe9e804885565cb9c4fb6a6515bb18/PS_5_LandAcqInvolResettlement.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816852925</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/7f690e0048855841bf7cff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_5.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817046981</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/36099a8048855658b9b4fb6a6515bb18/PS_6_BiodivConservation.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817321516</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/3c01a60048855827bf14ff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_6.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818061644</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/a6b1b6804885565ab9bcfb6a6515bb18/PS_7_IndigenousPeoples.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818661604</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/707761004885582bbf24ff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_7.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818940215</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/34d46f8048855650b9a4fb6a6515bb18/PS_8_CulturalHeritage.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819150440</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/03fd61804885582dbf2cff6a6515bb18/2007%2BUpdated%2BGuidance%2BNote_8.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819380720</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/b24bf8804885594c82a4d26a6515bb18/PS_1_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807571679</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/4b99d400488557c0bdb4ff6a6515bb18/PS_1_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807616365</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/8e4afd0048855a9b869cd66a6515bb18/PS_1_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807460655</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/728f0c004885596082ccd26a6515bb18/GN%2B1%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807769961</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/687bcc004885571abb5cfb6a6515bb18/GN%2B1%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322807671153</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/01e8410048855236aadcfa6a6515bb18/PS_2_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808191651</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/2e81bd0048855596b73cf76a6515bb18/PS_2_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808243174</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/4cd4720048865939b88afa6a6515bb18/PS_2_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808024381</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/3f43e70048855d7d8f2cdf6a6515bb18/GN%2B2%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808595347</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/258d800048865827b466f66a6515bb18/GN%2B2%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808318946</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/8fd2390048855dab8fc4df6a6515bb18/PS_3_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808840453</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/55949d8048855475b2dcf26a6515bb18/PS_3_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808918428</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/0dd8af004885596a82f4d26a6515bb18/PS_3_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808717071</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/f9522500488551b9a964fb6a6515bb18/GN%2B3%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322815709839</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/5f09588048855748bbf4fb6a6515bb18/GN%2B3%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322808976382</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/myconnect/topics_ext_content/ifc_external_corporate_site/ifc+sustainability/sustainability+framework/environmental%2C+health%2C+and+safety+guidelines/ehsguidelines_russian?contentIDR=f6d9098048d2fa2aa4b9bd4b02f32852&amp;useDefaultText=0&amp;useDefaultDesc=0</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/myconnect/topics_ext_content/ifc_external_corporate_site/ifc+sustainability/sustainability+framework/environmental%2C+health%2C+and+safety+guidelines/ehsguidelines_chinese?contentIDR=bc8ca10048d2f2a191dfbd4b02f32852&amp;useDefaultText=0&amp;useDefaultDesc=0</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/myconnect/topics_ext_content/ifc_external_corporate_site/ifc+sustainability/sustainability+framework/environmental%2C+health%2C+and+safety+guidelines/ehsguidelines_french?contentIDR=2cf4a88048d2fa80a58dbd4b02f32852&amp;useDefaultText=0&amp;useDefaultDesc=0</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/a85c5e0048855451b244f26a6515bb18/PS_4_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816115793</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/0d27250048855938824cd26a6515bb18/PS_4_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816246207</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/d01dd880488553f5b0e4f26a6515bb18/PS_4_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322815787713</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/64853c80488553f0b0c4f26a6515bb18/GN%2B4%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816814448</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/5adac8004885527cabbcfb6a6515bb18/GN%2B4%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816358306</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/0ce753804885595182b4d26a6515bb18/PS_5_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816976484</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/9d88a2804886591ab83afa6a6515bb18/PS_5_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817024761</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/7b7f2800488658fab7baf76a6515bb18/PS_5_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322816880634</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/69a1b60048855407b12cf36a6515bb18/GN%2B5%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817186383</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/36a5e68048855363aeccfe6a6515bb18/GN%2B5%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817092362</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/004d8300488553c6b07cf26a6515bb18/PS_6_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817934247</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/c491b20048855d118dd4df6a6515bb18/PS_6_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818006669</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/3eece70048855b0487ccd76a6515bb18/PS_6_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322817789803</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/f9b3f98048855d3d8e4cde6a6515bb18/GN%2B6%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818635416</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/3b0d1200488555a4b764f76a6515bb18/GN%2B6%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818106271</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/5dcda68048865899b68ef66a6515bb18/PS_7_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818859597</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/241aef80488555a5b76cf76a6515bb18/PS_8_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819361510</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/89e05080488552f3acecfe6a6515bb18/PS_8_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819187456</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/42b1640048855bff8a9cda6a6515bb18/GN%2B8%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819901760</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/a16a270048855422b17cf36a6515bb18/GN%2B8%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819415210</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/783c6a0048865903b7f2f76a6515bb18/PS_8_Russian.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819318968</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/53952080488555d4b84cfa6a6515bb18/GN%2B7%2B-%2BCh.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322819128741</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/7a022f80488658fbb7c2f76a6515bb18/GN%2B7%2B-%2BFrench.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818961106</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/341046004885598e836cd36a6515bb18/PS_7_Chinese.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818914190</t>
+  </si>
+  <si>
+    <t>http://www.ifc.org/wps/wcm/connect/75ea9200488557bebdacff6a6515bb18/PS_7_French.pdf?MOD=AJPERES&amp;attachment=true&amp;id=1322818691006</t>
+  </si>
+  <si>
+    <t>Operational Directive</t>
+  </si>
+  <si>
+    <t>Operational Policy</t>
+  </si>
+  <si>
+    <t>Operational Policy Note</t>
   </si>
 </sst>
 </file>
@@ -8128,7 +8449,7 @@
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -15158,15 +15479,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W98"/>
+  <dimension ref="A1:W118"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
       <pane ySplit="10" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15234,7 +15555,7 @@
     <row r="8" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="91"/>
       <c r="D8" s="15" t="s">
-        <v>2464</v>
+        <v>2465</v>
       </c>
       <c r="F8" s="95"/>
       <c r="U8" s="68"/>
@@ -15396,6 +15717,15 @@
       <c r="K14" t="s">
         <v>514</v>
       </c>
+      <c r="O14" t="s">
+        <v>2468</v>
+      </c>
+      <c r="P14" t="s">
+        <v>2469</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>2470</v>
+      </c>
       <c r="S14">
         <v>2012</v>
       </c>
@@ -15425,6 +15755,15 @@
       <c r="M15" s="28" t="s">
         <v>510</v>
       </c>
+      <c r="O15" t="s">
+        <v>2471</v>
+      </c>
+      <c r="P15" t="s">
+        <v>2472</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>2473</v>
+      </c>
       <c r="S15">
         <v>2006</v>
       </c>
@@ -15465,11 +15804,20 @@
       <c r="I18" t="s">
         <v>2345</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="16" t="s">
+        <v>2475</v>
+      </c>
+      <c r="M18" s="28" t="s">
         <v>529</v>
       </c>
-      <c r="S18">
-        <v>2007</v>
+      <c r="P18" t="s">
+        <v>2474</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>2476</v>
+      </c>
+      <c r="S18" s="28">
+        <v>2006</v>
       </c>
       <c r="W18" s="7" t="s">
         <v>138</v>
@@ -15628,6 +15976,9 @@
       <c r="D46" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F46" t="s">
+        <v>2570</v>
+      </c>
       <c r="G46">
         <v>4.01</v>
       </c>
@@ -15657,6 +16008,9 @@
       <c r="D47" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F47" t="s">
+        <v>2570</v>
+      </c>
       <c r="G47">
         <v>4.04</v>
       </c>
@@ -15686,6 +16040,9 @@
       <c r="D48" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F48" t="s">
+        <v>2570</v>
+      </c>
       <c r="G48">
         <v>4.09</v>
       </c>
@@ -15715,6 +16072,9 @@
       <c r="D49" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F49" t="s">
+        <v>2570</v>
+      </c>
       <c r="G49">
         <v>4.3600000000000003</v>
       </c>
@@ -15744,6 +16104,9 @@
       <c r="D50" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F50" t="s">
+        <v>2570</v>
+      </c>
       <c r="G50">
         <v>4.37</v>
       </c>
@@ -15773,6 +16136,9 @@
       <c r="D51" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F51" t="s">
+        <v>2570</v>
+      </c>
       <c r="G51">
         <v>7.5</v>
       </c>
@@ -15802,6 +16168,9 @@
       <c r="D52" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F52" t="s">
+        <v>2569</v>
+      </c>
       <c r="G52">
         <v>4.2</v>
       </c>
@@ -15831,6 +16200,9 @@
       <c r="D53" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F53" t="s">
+        <v>2569</v>
+      </c>
       <c r="G53">
         <v>4.3</v>
       </c>
@@ -15860,6 +16232,9 @@
       <c r="D54" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F54" t="s">
+        <v>2571</v>
+      </c>
       <c r="G54">
         <v>11.03</v>
       </c>
@@ -15916,6 +16291,9 @@
       <c r="D58" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F58" t="s">
+        <v>505</v>
+      </c>
       <c r="G58" s="87" t="s">
         <v>37</v>
       </c>
@@ -15923,7 +16301,7 @@
         <v>2401</v>
       </c>
       <c r="J58" t="s">
-        <v>2438</v>
+        <v>2439</v>
       </c>
       <c r="S58">
         <v>1998</v>
@@ -15939,6 +16317,9 @@
       <c r="D59" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F59" t="s">
+        <v>505</v>
+      </c>
       <c r="G59" s="87" t="s">
         <v>38</v>
       </c>
@@ -15946,7 +16327,7 @@
         <v>2402</v>
       </c>
       <c r="J59" t="s">
-        <v>2439</v>
+        <v>2440</v>
       </c>
       <c r="S59">
         <v>1998</v>
@@ -15962,6 +16343,9 @@
       <c r="D60" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F60" t="s">
+        <v>505</v>
+      </c>
       <c r="G60" s="87" t="s">
         <v>39</v>
       </c>
@@ -15969,7 +16353,7 @@
         <v>2403</v>
       </c>
       <c r="J60" t="s">
-        <v>2440</v>
+        <v>2441</v>
       </c>
       <c r="S60">
         <v>1998</v>
@@ -15985,6 +16369,9 @@
       <c r="D61" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F61" t="s">
+        <v>505</v>
+      </c>
       <c r="G61" s="87" t="s">
         <v>40</v>
       </c>
@@ -15992,7 +16379,7 @@
         <v>2404</v>
       </c>
       <c r="J61" t="s">
-        <v>2441</v>
+        <v>2442</v>
       </c>
       <c r="S61">
         <v>1998</v>
@@ -16008,6 +16395,9 @@
       <c r="D62" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F62" t="s">
+        <v>505</v>
+      </c>
       <c r="G62" s="87" t="s">
         <v>33</v>
       </c>
@@ -16015,7 +16405,7 @@
         <v>2405</v>
       </c>
       <c r="J62" t="s">
-        <v>2442</v>
+        <v>2443</v>
       </c>
       <c r="S62">
         <v>1998</v>
@@ -16031,6 +16421,9 @@
       <c r="D63" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F63" t="s">
+        <v>505</v>
+      </c>
       <c r="G63" s="87" t="s">
         <v>41</v>
       </c>
@@ -16038,7 +16431,7 @@
         <v>2406</v>
       </c>
       <c r="J63" t="s">
-        <v>2443</v>
+        <v>2444</v>
       </c>
       <c r="S63">
         <v>1998</v>
@@ -16054,11 +16447,14 @@
       <c r="D65" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F65" t="s">
+        <v>505</v>
+      </c>
       <c r="I65" t="s">
         <v>2407</v>
       </c>
       <c r="J65" t="s">
-        <v>2444</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -16068,14 +16464,17 @@
       <c r="D67" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F67" t="s">
+        <v>505</v>
+      </c>
       <c r="I67" t="s">
         <v>2408</v>
       </c>
       <c r="J67" t="s">
-        <v>2444</v>
+        <v>2445</v>
       </c>
       <c r="Q67" t="s">
-        <v>2453</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -16085,6 +16484,9 @@
       <c r="D68" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F68" t="s">
+        <v>505</v>
+      </c>
       <c r="G68">
         <v>1</v>
       </c>
@@ -16092,10 +16494,10 @@
         <v>2409</v>
       </c>
       <c r="J68" t="s">
-        <v>2445</v>
+        <v>2446</v>
       </c>
       <c r="Q68" t="s">
-        <v>2454</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -16105,6 +16507,9 @@
       <c r="D69" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F69" t="s">
+        <v>505</v>
+      </c>
       <c r="G69">
         <v>2</v>
       </c>
@@ -16112,10 +16517,10 @@
         <v>2410</v>
       </c>
       <c r="J69" t="s">
-        <v>2446</v>
+        <v>2447</v>
       </c>
       <c r="Q69" t="s">
-        <v>2455</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -16125,6 +16530,9 @@
       <c r="D70" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F70" t="s">
+        <v>505</v>
+      </c>
       <c r="G70">
         <v>3</v>
       </c>
@@ -16132,10 +16540,10 @@
         <v>2411</v>
       </c>
       <c r="J70" t="s">
-        <v>2447</v>
+        <v>2448</v>
       </c>
       <c r="Q70" t="s">
-        <v>2456</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -16145,6 +16553,9 @@
       <c r="D71" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F71" t="s">
+        <v>505</v>
+      </c>
       <c r="G71">
         <v>4</v>
       </c>
@@ -16152,10 +16563,10 @@
         <v>2412</v>
       </c>
       <c r="J71" t="s">
-        <v>2448</v>
+        <v>2449</v>
       </c>
       <c r="Q71" t="s">
-        <v>2457</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -16165,6 +16576,9 @@
       <c r="D72" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F72" t="s">
+        <v>505</v>
+      </c>
       <c r="G72">
         <v>5</v>
       </c>
@@ -16172,10 +16586,10 @@
         <v>2413</v>
       </c>
       <c r="J72" t="s">
-        <v>2449</v>
+        <v>2450</v>
       </c>
       <c r="Q72" t="s">
-        <v>2458</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -16185,6 +16599,9 @@
       <c r="D73" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F73" t="s">
+        <v>505</v>
+      </c>
       <c r="G73">
         <v>6</v>
       </c>
@@ -16192,10 +16609,10 @@
         <v>2414</v>
       </c>
       <c r="J73" t="s">
-        <v>2450</v>
+        <v>2451</v>
       </c>
       <c r="Q73" t="s">
-        <v>2459</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -16205,6 +16622,9 @@
       <c r="D74" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F74" t="s">
+        <v>505</v>
+      </c>
       <c r="G74">
         <v>7</v>
       </c>
@@ -16212,10 +16632,10 @@
         <v>2415</v>
       </c>
       <c r="J74" t="s">
-        <v>2451</v>
+        <v>2452</v>
       </c>
       <c r="Q74" t="s">
-        <v>2460</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -16225,6 +16645,9 @@
       <c r="D75" s="94" t="s">
         <v>1102</v>
       </c>
+      <c r="F75" t="s">
+        <v>505</v>
+      </c>
       <c r="G75">
         <v>8</v>
       </c>
@@ -16232,36 +16655,47 @@
         <v>2416</v>
       </c>
       <c r="J75" t="s">
-        <v>2452</v>
+        <v>2453</v>
       </c>
       <c r="Q75" t="s">
-        <v>2461</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="77" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="62"/>
-      <c r="E77"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>2436</v>
+        <v>2437</v>
       </c>
       <c r="D79" s="67" t="s">
         <v>1101</v>
       </c>
+      <c r="F79" t="s">
+        <v>2417</v>
+      </c>
       <c r="I79" t="s">
-        <v>2417</v>
+        <v>2418</v>
+      </c>
+      <c r="J79" t="s">
+        <v>2466</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>2436</v>
+        <v>2437</v>
       </c>
       <c r="D80" s="67" t="s">
         <v>1101</v>
       </c>
+      <c r="F80" t="s">
+        <v>2417</v>
+      </c>
       <c r="I80" t="s">
-        <v>2418</v>
+        <v>2419</v>
+      </c>
+      <c r="J80" t="s">
+        <v>2467</v>
       </c>
     </row>
     <row r="81" spans="2:19" x14ac:dyDescent="0.25">
@@ -16272,13 +16706,16 @@
         <v>1101</v>
       </c>
       <c r="F81" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G81">
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>2419</v>
+        <v>2420</v>
+      </c>
+      <c r="J81" t="s">
+        <v>2477</v>
       </c>
       <c r="S81">
         <v>2012</v>
@@ -16298,7 +16735,10 @@
         <v>1</v>
       </c>
       <c r="I82" t="s">
-        <v>2420</v>
+        <v>2421</v>
+      </c>
+      <c r="J82" t="s">
+        <v>2478</v>
       </c>
       <c r="S82">
         <v>2012</v>
@@ -16312,13 +16752,16 @@
         <v>1101</v>
       </c>
       <c r="F83" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G83">
         <v>2</v>
       </c>
       <c r="I83" t="s">
-        <v>2421</v>
+        <v>2422</v>
+      </c>
+      <c r="J83" t="s">
+        <v>2479</v>
       </c>
       <c r="S83">
         <v>2012</v>
@@ -16338,7 +16781,10 @@
         <v>2</v>
       </c>
       <c r="I84" t="s">
-        <v>2422</v>
+        <v>2423</v>
+      </c>
+      <c r="J84" t="s">
+        <v>2480</v>
       </c>
       <c r="S84">
         <v>2012</v>
@@ -16352,13 +16798,16 @@
         <v>1101</v>
       </c>
       <c r="F85" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G85">
         <v>3</v>
       </c>
       <c r="I85" t="s">
-        <v>2423</v>
+        <v>2424</v>
+      </c>
+      <c r="J85" t="s">
+        <v>2481</v>
       </c>
       <c r="S85">
         <v>2012</v>
@@ -16378,7 +16827,10 @@
         <v>3</v>
       </c>
       <c r="I86" t="s">
-        <v>2424</v>
+        <v>2425</v>
+      </c>
+      <c r="J86" t="s">
+        <v>2482</v>
       </c>
       <c r="S86">
         <v>2012</v>
@@ -16386,14 +16838,17 @@
     </row>
     <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>2437</v>
+        <v>2438</v>
       </c>
       <c r="D87" s="15"/>
       <c r="F87" t="s">
-        <v>2463</v>
+        <v>2464</v>
       </c>
       <c r="I87" t="s">
-        <v>2425</v>
+        <v>2426</v>
+      </c>
+      <c r="J87" t="s">
+        <v>2483</v>
       </c>
       <c r="S87">
         <v>2012</v>
@@ -16407,13 +16862,16 @@
         <v>1101</v>
       </c>
       <c r="F88" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G88">
         <v>4</v>
       </c>
       <c r="I88" t="s">
-        <v>2426</v>
+        <v>2427</v>
+      </c>
+      <c r="J88" t="s">
+        <v>2484</v>
       </c>
       <c r="S88">
         <v>2012</v>
@@ -16433,7 +16891,10 @@
         <v>4</v>
       </c>
       <c r="I89" t="s">
-        <v>2427</v>
+        <v>2428</v>
+      </c>
+      <c r="J89" t="s">
+        <v>2485</v>
       </c>
       <c r="S89">
         <v>2012</v>
@@ -16441,14 +16902,17 @@
     </row>
     <row r="90" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>2437</v>
+        <v>2438</v>
       </c>
       <c r="D90" s="15"/>
       <c r="F90" t="s">
-        <v>2463</v>
+        <v>2464</v>
       </c>
       <c r="I90" t="s">
-        <v>2425</v>
+        <v>2426</v>
+      </c>
+      <c r="J90" t="s">
+        <v>2483</v>
       </c>
       <c r="S90">
         <v>2012</v>
@@ -16462,13 +16926,16 @@
         <v>1101</v>
       </c>
       <c r="F91" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G91">
         <v>5</v>
       </c>
       <c r="I91" t="s">
-        <v>2428</v>
+        <v>2429</v>
+      </c>
+      <c r="J91" t="s">
+        <v>2486</v>
       </c>
       <c r="S91">
         <v>2012</v>
@@ -16488,7 +16955,10 @@
         <v>5</v>
       </c>
       <c r="I92" t="s">
-        <v>2429</v>
+        <v>2430</v>
+      </c>
+      <c r="J92" t="s">
+        <v>2487</v>
       </c>
       <c r="S92">
         <v>2012</v>
@@ -16502,13 +16972,16 @@
         <v>1101</v>
       </c>
       <c r="F93" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G93">
         <v>6</v>
       </c>
       <c r="I93" t="s">
-        <v>2430</v>
+        <v>2431</v>
+      </c>
+      <c r="J93" t="s">
+        <v>2488</v>
       </c>
       <c r="S93">
         <v>2012</v>
@@ -16528,7 +17001,10 @@
         <v>6</v>
       </c>
       <c r="I94" t="s">
-        <v>2431</v>
+        <v>2432</v>
+      </c>
+      <c r="J94" t="s">
+        <v>2489</v>
       </c>
       <c r="S94">
         <v>2012</v>
@@ -16542,13 +17018,16 @@
         <v>1101</v>
       </c>
       <c r="F95" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G95">
         <v>7</v>
       </c>
       <c r="I95" t="s">
-        <v>2432</v>
+        <v>2433</v>
+      </c>
+      <c r="J95" t="s">
+        <v>2490</v>
       </c>
       <c r="S95">
         <v>2012</v>
@@ -16568,7 +17047,10 @@
         <v>7</v>
       </c>
       <c r="I96" t="s">
-        <v>2433</v>
+        <v>2434</v>
+      </c>
+      <c r="J96" t="s">
+        <v>2491</v>
       </c>
       <c r="S96">
         <v>2012</v>
@@ -16582,13 +17064,16 @@
         <v>1101</v>
       </c>
       <c r="F97" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="G97">
         <v>8</v>
       </c>
       <c r="I97" t="s">
-        <v>2434</v>
+        <v>2435</v>
+      </c>
+      <c r="J97" t="s">
+        <v>2492</v>
       </c>
       <c r="S97">
         <v>2012</v>
@@ -16608,10 +17093,501 @@
         <v>8</v>
       </c>
       <c r="I98" t="s">
-        <v>2435</v>
+        <v>2436</v>
+      </c>
+      <c r="J98" t="s">
+        <v>2493</v>
       </c>
       <c r="S98">
         <v>2012</v>
+      </c>
+    </row>
+    <row r="101" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D101" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F101" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="I101" t="s">
+        <v>2494</v>
+      </c>
+      <c r="J101" t="s">
+        <v>2510</v>
+      </c>
+      <c r="O101" t="s">
+        <v>2526</v>
+      </c>
+      <c r="P101" t="s">
+        <v>2527</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>2528</v>
+      </c>
+    </row>
+    <row r="102" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D102" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F102" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="I102" t="s">
+        <v>2495</v>
+      </c>
+      <c r="J102" t="s">
+        <v>2511</v>
+      </c>
+      <c r="P102" t="s">
+        <v>2529</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="103" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D103" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F103" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G103">
+        <v>2</v>
+      </c>
+      <c r="I103" t="s">
+        <v>2496</v>
+      </c>
+      <c r="J103" t="s">
+        <v>2512</v>
+      </c>
+      <c r="O103" t="s">
+        <v>2531</v>
+      </c>
+      <c r="P103" t="s">
+        <v>2532</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="104" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D104" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F104" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+      <c r="I104" t="s">
+        <v>2497</v>
+      </c>
+      <c r="J104" t="s">
+        <v>2513</v>
+      </c>
+      <c r="P104" t="s">
+        <v>2534</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>2535</v>
+      </c>
+    </row>
+    <row r="105" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D105" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F105" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G105">
+        <v>3</v>
+      </c>
+      <c r="I105" t="s">
+        <v>2498</v>
+      </c>
+      <c r="J105" t="s">
+        <v>2514</v>
+      </c>
+      <c r="O105" t="s">
+        <v>2536</v>
+      </c>
+      <c r="P105" t="s">
+        <v>2537</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="106" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D106" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F106" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G106">
+        <v>3</v>
+      </c>
+      <c r="I106" t="s">
+        <v>2499</v>
+      </c>
+      <c r="J106" t="s">
+        <v>2515</v>
+      </c>
+      <c r="P106" t="s">
+        <v>2539</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="107" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D107" s="15"/>
+      <c r="F107" t="s">
+        <v>2464</v>
+      </c>
+      <c r="I107" t="s">
+        <v>2426</v>
+      </c>
+      <c r="J107" t="s">
+        <v>2483</v>
+      </c>
+      <c r="O107" t="s">
+        <v>2541</v>
+      </c>
+      <c r="P107" t="s">
+        <v>2542</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="108" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D108" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F108" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G108">
+        <v>4</v>
+      </c>
+      <c r="I108" t="s">
+        <v>2500</v>
+      </c>
+      <c r="J108" t="s">
+        <v>2516</v>
+      </c>
+      <c r="O108" t="s">
+        <v>2544</v>
+      </c>
+      <c r="P108" t="s">
+        <v>2545</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>2546</v>
+      </c>
+    </row>
+    <row r="109" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D109" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F109" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G109">
+        <v>4</v>
+      </c>
+      <c r="I109" t="s">
+        <v>2501</v>
+      </c>
+      <c r="J109" t="s">
+        <v>2517</v>
+      </c>
+      <c r="P109" t="s">
+        <v>2547</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="110" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D110" s="15"/>
+      <c r="F110" t="s">
+        <v>2464</v>
+      </c>
+      <c r="I110" t="s">
+        <v>2426</v>
+      </c>
+      <c r="J110" t="s">
+        <v>2483</v>
+      </c>
+      <c r="O110" t="s">
+        <v>2541</v>
+      </c>
+      <c r="P110" t="s">
+        <v>2542</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="111" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D111" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F111" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G111">
+        <v>5</v>
+      </c>
+      <c r="I111" t="s">
+        <v>2502</v>
+      </c>
+      <c r="J111" t="s">
+        <v>2518</v>
+      </c>
+      <c r="O111" t="s">
+        <v>2549</v>
+      </c>
+      <c r="P111" t="s">
+        <v>2550</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="112" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D112" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F112" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G112">
+        <v>5</v>
+      </c>
+      <c r="I112" t="s">
+        <v>2503</v>
+      </c>
+      <c r="J112" t="s">
+        <v>2519</v>
+      </c>
+      <c r="P112" t="s">
+        <v>2552</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>2553</v>
+      </c>
+    </row>
+    <row r="113" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D113" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F113" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G113">
+        <v>6</v>
+      </c>
+      <c r="I113" t="s">
+        <v>2504</v>
+      </c>
+      <c r="J113" t="s">
+        <v>2520</v>
+      </c>
+      <c r="O113" t="s">
+        <v>2554</v>
+      </c>
+      <c r="P113" t="s">
+        <v>2555</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="114" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D114" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F114" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G114">
+        <v>6</v>
+      </c>
+      <c r="I114" t="s">
+        <v>2505</v>
+      </c>
+      <c r="J114" t="s">
+        <v>2521</v>
+      </c>
+      <c r="P114" t="s">
+        <v>2557</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="115" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D115" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F115" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G115">
+        <v>7</v>
+      </c>
+      <c r="I115" t="s">
+        <v>2506</v>
+      </c>
+      <c r="J115" t="s">
+        <v>2522</v>
+      </c>
+      <c r="O115" t="s">
+        <v>2559</v>
+      </c>
+      <c r="P115" t="s">
+        <v>2567</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="116" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D116" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F116" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G116">
+        <v>7</v>
+      </c>
+      <c r="I116" t="s">
+        <v>2507</v>
+      </c>
+      <c r="J116" t="s">
+        <v>2523</v>
+      </c>
+      <c r="P116" t="s">
+        <v>2565</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="117" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D117" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F117" t="s">
+        <v>2463</v>
+      </c>
+      <c r="G117">
+        <v>8</v>
+      </c>
+      <c r="I117" t="s">
+        <v>2508</v>
+      </c>
+      <c r="J117" t="s">
+        <v>2524</v>
+      </c>
+      <c r="O117" t="s">
+        <v>2564</v>
+      </c>
+      <c r="P117" t="s">
+        <v>2560</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="118" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D118" s="94" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F118" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G118">
+        <v>8</v>
+      </c>
+      <c r="I118" t="s">
+        <v>2509</v>
+      </c>
+      <c r="J118" t="s">
+        <v>2525</v>
+      </c>
+      <c r="P118" t="s">
+        <v>2562</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>2563</v>
       </c>
     </row>
   </sheetData>
@@ -19257,8 +20233,8 @@
     <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>